<commit_message>
Update Excel for new feature
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP- monousuario\Facturador_Windows\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E92F344-EA0B-4145-9C2B-DAEC4E0991AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D6521C-BD95-46BB-980C-B45A18F60B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Factura" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AD$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AF$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="79">
   <si>
     <t>Fecha</t>
   </si>
@@ -249,6 +249,30 @@
   </si>
   <si>
     <t>MARTIN BUSTOS</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Anterior</t>
+  </si>
+  <si>
+    <t>Posterior</t>
+  </si>
+  <si>
+    <t>Derecha Tipo</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Remito R</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Unidades Facturador</t>
   </si>
 </sst>
 </file>
@@ -600,7 +624,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -730,6 +754,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -776,7 +813,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -791,11 +828,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1158,12 +1197,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH17"/>
+  <dimension ref="A1:AN17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,22 +1216,24 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="23" width="9.140625" customWidth="1"/>
-    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" customWidth="1"/>
-    <col min="27" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="9.140625" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="25" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="9.140625" customWidth="1"/>
+    <col min="32" max="32" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="36" width="13.7109375" customWidth="1"/>
+    <col min="37" max="37" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1254,62 +1295,80 @@
         <v>19</v>
       </c>
       <c r="U1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AG1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="12" t="s">
+      <c r="AL1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AM1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AN1" s="17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44992</v>
       </c>
       <c r="B2" s="9" t="str">
-        <f t="shared" ref="B2:B17" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
+        <f>TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f t="shared" ref="C2:C17" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
+        <f>TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f t="shared" ref="D2:D17" si="2">TEXT(A2+14,"dd/mm/aaaa")</f>
+        <f>TEXT(A2+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E2" s="2">
@@ -1319,7 +1378,7 @@
         <v>34</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>36</v>
@@ -1328,23 +1387,23 @@
         <v>9</v>
       </c>
       <c r="J2" s="3">
-        <v>33610006189</v>
+        <v>30525390086</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B2,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>53</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="M2" s="4">
-        <v>5.04</v>
-      </c>
-      <c r="N2" s="2">
-        <v>8851.52</v>
+        <v>9.1175320000000006</v>
+      </c>
+      <c r="N2" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O2" s="5">
-        <v>44628.1</v>
+        <f>ROUND(M2*N2,6)</f>
+        <v>170247.93684800001</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>38</v>
@@ -1352,71 +1411,96 @@
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="1" t="str">
-        <f t="shared" ref="U2" si="3">TEXT(R2,"00000")</f>
+      <c r="T2" s="12"/>
+      <c r="U2" s="14">
+        <f>COUNTIFS($F$1:F2,F2,$K$1:K2,K2)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V2" s="14" t="str">
+        <f>SUBSTITUTE(M2,",",".")</f>
+        <v>9.117532</v>
+      </c>
+      <c r="W2" s="1" t="str">
+        <f>TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <f t="shared" ref="V2" si="4">TEXT(S2,"00000000")</f>
+      <c r="X2" s="1" t="str">
+        <f>TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W2" s="1" t="str">
+      <c r="Y2" s="1" t="str">
         <f>TEXT(T2,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X2" s="14">
-        <f t="shared" ref="X2" si="5">ROUND(O2*P2,2)</f>
-        <v>9371.9</v>
-      </c>
-      <c r="Y2" s="14">
-        <f t="shared" ref="Y2" si="6">O2+X2</f>
-        <v>54000</v>
-      </c>
-      <c r="Z2" s="10" t="str">
-        <f>IF(F2="Factura A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(Y2,"0,00"),",","."))</f>
-        <v>44628.10</v>
-      </c>
-      <c r="AA2" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(Y2,0)-Y2,"0,00"),",",".")</f>
-        <v>0.00</v>
-      </c>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1">
-        <f t="shared" ref="AC2" si="7">ROW(K2)</f>
+      <c r="Z2" s="13">
+        <f>ROUND(O2*P2,2)</f>
+        <v>35752.07</v>
+      </c>
+      <c r="AA2" s="13">
+        <f>O2+Z2</f>
+        <v>206000.00684800002</v>
+      </c>
+      <c r="AB2" s="10" t="str">
+        <f>IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AA2,"0,00"),",","."))</f>
+        <v>170247.94</v>
+      </c>
+      <c r="AC2" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA2,0)-AA2,"0,00"),",",".")</f>
+        <v>0.99</v>
+      </c>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1">
+        <f>ROW(K2)</f>
         <v>2</v>
       </c>
-      <c r="AD2" s="1" t="str">
+      <c r="AF2" s="15" t="str">
         <f>J2&amp;"-"&amp;COUNTIF($J$1:J2,J2)</f>
-        <v>33610006189-1</v>
-      </c>
-      <c r="AF2" s="15">
-        <f t="shared" ref="AF2" si="8">CEILING(N2*M2*(1+P2),500)</f>
-        <v>54000</v>
-      </c>
-      <c r="AG2" s="15">
-        <f t="shared" ref="AG2" si="9">ROUND((AF2/(1+P2)),2)</f>
-        <v>44628.1</v>
-      </c>
-      <c r="AH2" s="16">
-        <f t="shared" ref="AH2" si="10">ROUND(AG2/N2,4)</f>
-        <v>5.0419</v>
+        <v>30525390086-1</v>
+      </c>
+      <c r="AG2" s="1">
+        <f>IF(K1=K2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="1">
+        <f>IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="1" t="str">
+        <f>RIGHT(F2)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ2" s="1">
+        <f>IF(LEFT(F2,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="13">
+        <f>CEILING(N2*M2*(1+P2),500)</f>
+        <v>206500</v>
+      </c>
+      <c r="AM2" s="13">
+        <f>ROUND((AL2/(1+P2)),2)</f>
+        <v>170661.16</v>
+      </c>
+      <c r="AN2" s="18">
+        <f>ROUND(AM2/N2,6)</f>
+        <v>9.1396619999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44992</v>
       </c>
       <c r="B3" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C3),MONTH(C3),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A3,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A3+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E3" s="2">
@@ -1435,22 +1519,24 @@
         <v>9</v>
       </c>
       <c r="J3" s="3">
-        <v>33610006189</v>
+        <v>30525733870</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f>"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M3" s="4">
-        <v>5.04</v>
-      </c>
-      <c r="N3" s="2">
-        <v>8851.52</v>
+        <v>8.0774249999999999</v>
+      </c>
+      <c r="N3" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O3" s="5">
-        <v>44628.1</v>
+        <f>ROUND(M3*N3,6)</f>
+        <v>150826.44528099999</v>
       </c>
       <c r="P3" s="11" t="s">
         <v>38</v>
@@ -1458,71 +1544,96 @@
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="1" t="str">
-        <f t="shared" ref="U3:U17" si="11">TEXT(R3,"00000")</f>
+      <c r="T3" s="12"/>
+      <c r="U3" s="14">
+        <f>COUNTIFS($F$1:F3,F3,$K$1:K3,K3)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V3" s="14" t="str">
+        <f>SUBSTITUTE(M3,",",".")</f>
+        <v>8.077425</v>
+      </c>
+      <c r="W3" s="1" t="str">
+        <f>TEXT(R3,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V3" s="1" t="str">
-        <f t="shared" ref="V3:V17" si="12">TEXT(S3,"00000000")</f>
+      <c r="X3" s="1" t="str">
+        <f>TEXT(S3,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W3" s="1" t="str">
+      <c r="Y3" s="1" t="str">
         <f>TEXT(T3,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X3" s="14">
-        <f t="shared" ref="X3:X17" si="13">ROUND(O3*P3,2)</f>
-        <v>9371.9</v>
-      </c>
-      <c r="Y3" s="14">
-        <f t="shared" ref="Y3:Y17" si="14">O3+X3</f>
-        <v>54000</v>
-      </c>
-      <c r="Z3" s="10" t="str">
-        <f t="shared" ref="Z3:Z17" si="15">IF(F3="Factura A",SUBSTITUTE(TEXT(O3,"0,00"),",","."),SUBSTITUTE(TEXT(Y3,"0,00"),",","."))</f>
-        <v>44628.10</v>
-      </c>
-      <c r="AA3" s="10" t="str">
-        <f t="shared" ref="AA3:AA17" si="16">SUBSTITUTE(TEXT(ROUNDUP(Y3,0)-Y3,"0,00"),",",".")</f>
+      <c r="Z3" s="13">
+        <f>ROUND(O3*P3,2)</f>
+        <v>31673.55</v>
+      </c>
+      <c r="AA3" s="13">
+        <f>O3+Z3</f>
+        <v>182499.99528099998</v>
+      </c>
+      <c r="AB3" s="10" t="str">
+        <f>IF(RIGHT(F3,1)="A",SUBSTITUTE(TEXT(O3,"0,00"),",","."),SUBSTITUTE(TEXT(AA3,"0,00"),",","."))</f>
+        <v>150826.45</v>
+      </c>
+      <c r="AC3" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA3,0)-AA3,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1">
-        <f t="shared" ref="AC3:AC17" si="17">ROW(K3)</f>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1">
+        <f>ROW(K3)</f>
         <v>3</v>
       </c>
-      <c r="AD3" s="1" t="str">
+      <c r="AF3" s="15" t="str">
         <f>J3&amp;"-"&amp;COUNTIF($J$1:J3,J3)</f>
-        <v>33610006189-2</v>
-      </c>
-      <c r="AF3" s="15">
-        <f t="shared" ref="AF3:AF17" si="18">CEILING(N3*M3*(1+P3),500)</f>
-        <v>54000</v>
-      </c>
-      <c r="AG3" s="15">
-        <f t="shared" ref="AG3:AG17" si="19">ROUND((AF3/(1+P3)),2)</f>
-        <v>44628.1</v>
-      </c>
-      <c r="AH3" s="16">
-        <f t="shared" ref="AH3:AH17" si="20">ROUND(AG3/N3,4)</f>
-        <v>5.0419</v>
+        <v>30525733870-1</v>
+      </c>
+      <c r="AG3" s="1">
+        <f>IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1">
+        <f>IF(K3=K4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI3" s="1" t="str">
+        <f>RIGHT(F3)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ3" s="1">
+        <f>IF(LEFT(F3,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="13">
+        <f>CEILING(N3*M3*(1+P3),500)</f>
+        <v>182500</v>
+      </c>
+      <c r="AM3" s="13">
+        <f>ROUND((AL3/(1+P3)),2)</f>
+        <v>150826.45000000001</v>
+      </c>
+      <c r="AN3" s="18">
+        <f>ROUND(AM3/N3,6)</f>
+        <v>8.0774249999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44992</v>
       </c>
       <c r="B4" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C4),MONTH(C4),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A4,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A4+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E4" s="2">
@@ -1551,13 +1662,14 @@
         <v>Honorarios Febrero</v>
       </c>
       <c r="M4" s="4">
-        <v>10.039999999999999</v>
-      </c>
-      <c r="N4" s="2">
-        <v>8851.52</v>
+        <v>10.091248999999999</v>
+      </c>
+      <c r="N4" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O4" s="5">
-        <v>88842.97</v>
+        <f>ROUND(M4*N4,6)</f>
+        <v>188429.75516500001</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>38</v>
@@ -1565,78 +1677,103 @@
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="14">
+        <f>COUNTIFS($F$1:F4,F4,$K$1:K4,K4)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V4" s="14" t="str">
+        <f>SUBSTITUTE(M4,",",".")</f>
+        <v>10.091249</v>
+      </c>
+      <c r="W4" s="1" t="str">
+        <f>TEXT(R4,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V4" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X4" s="1" t="str">
+        <f>TEXT(S4,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W4" s="1" t="str">
+      <c r="Y4" s="1" t="str">
         <f>TEXT(T4,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X4" s="14">
-        <f t="shared" si="13"/>
-        <v>18657.02</v>
-      </c>
-      <c r="Y4" s="14">
-        <f t="shared" si="14"/>
-        <v>107499.99</v>
-      </c>
-      <c r="Z4" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>88842.97</v>
-      </c>
-      <c r="AA4" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.01</v>
-      </c>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z4" s="13">
+        <f>ROUND(O4*P4,2)</f>
+        <v>39570.25</v>
+      </c>
+      <c r="AA4" s="13">
+        <f>O4+Z4</f>
+        <v>228000.00516500001</v>
+      </c>
+      <c r="AB4" s="10" t="str">
+        <f>IF(RIGHT(F4,1)="A",SUBSTITUTE(TEXT(O4,"0,00"),",","."),SUBSTITUTE(TEXT(AA4,"0,00"),",","."))</f>
+        <v>188429.76</v>
+      </c>
+      <c r="AC4" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA4,0)-AA4,"0,00"),",",".")</f>
+        <v>0.99</v>
+      </c>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1">
+        <f>ROW(K4)</f>
         <v>4</v>
       </c>
-      <c r="AD4" s="1" t="str">
+      <c r="AF4" s="15" t="str">
         <f>J4&amp;"-"&amp;COUNTIF($J$1:J4,J4)</f>
         <v>30610252334-1</v>
       </c>
-      <c r="AF4" s="15">
-        <f t="shared" si="18"/>
-        <v>108000</v>
-      </c>
-      <c r="AG4" s="15">
-        <f t="shared" si="19"/>
-        <v>89256.2</v>
-      </c>
-      <c r="AH4" s="16">
-        <f t="shared" si="20"/>
-        <v>10.0837</v>
+      <c r="AG4" s="1">
+        <f>IF(K3=K4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="1">
+        <f>IF(K4=K5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI4" s="1" t="str">
+        <f>RIGHT(F4)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ4" s="1">
+        <f>IF(LEFT(F4,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="13">
+        <f>CEILING(N4*M4*(1+P4),500)</f>
+        <v>228500</v>
+      </c>
+      <c r="AM4" s="13">
+        <f>ROUND((AL4/(1+P4)),2)</f>
+        <v>188842.98</v>
+      </c>
+      <c r="AN4" s="18">
+        <f>ROUND(AM4/N4,6)</f>
+        <v>10.113379</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44992</v>
       </c>
       <c r="B5" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C5),MONTH(C5),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C5" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A5,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A5+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>39</v>
@@ -1648,112 +1785,131 @@
         <v>9</v>
       </c>
       <c r="J5" s="3">
-        <v>30684125792</v>
+        <v>30710964277</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f>"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M5" s="4">
-        <v>7</v>
-      </c>
-      <c r="N5" s="2">
-        <v>8851.52</v>
+        <v>9.1175320000000006</v>
+      </c>
+      <c r="N5" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O5" s="5">
-        <v>61983.47</v>
+        <f>ROUND(M5*N5,6)</f>
+        <v>170247.93684800001</v>
       </c>
       <c r="P5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="T5" s="13">
-        <v>44816</v>
-      </c>
-      <c r="U5" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>00002</v>
-      </c>
-      <c r="V5" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000150</v>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="14">
+        <f>COUNTIFS($F$1:F5,F5,$K$1:K5,K5)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V5" s="14" t="str">
+        <f>SUBSTITUTE(M5,",",".")</f>
+        <v>9.117532</v>
       </c>
       <c r="W5" s="1" t="str">
+        <f>TEXT(R5,"00000")</f>
+        <v>00000</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f>TEXT(S5,"00000000")</f>
+        <v>00000000</v>
+      </c>
+      <c r="Y5" s="1" t="str">
         <f>TEXT(T5,"DD/MM/aaaa")</f>
-        <v>12/09/2022</v>
-      </c>
-      <c r="X5" s="14">
-        <f t="shared" si="13"/>
-        <v>13016.53</v>
-      </c>
-      <c r="Y5" s="14">
-        <f t="shared" si="14"/>
-        <v>75000</v>
-      </c>
-      <c r="Z5" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>75000.00</v>
-      </c>
-      <c r="AA5" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1">
-        <f t="shared" si="17"/>
+        <v>00/01/1900</v>
+      </c>
+      <c r="Z5" s="13">
+        <f>ROUND(O5*P5,2)</f>
+        <v>35752.07</v>
+      </c>
+      <c r="AA5" s="13">
+        <f>O5+Z5</f>
+        <v>206000.00684800002</v>
+      </c>
+      <c r="AB5" s="10" t="str">
+        <f>IF(RIGHT(F5,1)="A",SUBSTITUTE(TEXT(O5,"0,00"),",","."),SUBSTITUTE(TEXT(AA5,"0,00"),",","."))</f>
+        <v>170247.94</v>
+      </c>
+      <c r="AC5" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA5,0)-AA5,"0,00"),",",".")</f>
+        <v>0.99</v>
+      </c>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1">
+        <f>ROW(K5)</f>
         <v>5</v>
       </c>
-      <c r="AD5" s="1" t="str">
+      <c r="AF5" s="15" t="str">
         <f>J5&amp;"-"&amp;COUNTIF($J$1:J5,J5)</f>
-        <v>30684125792-1</v>
-      </c>
-      <c r="AF5" s="15">
-        <f t="shared" si="18"/>
-        <v>75000</v>
-      </c>
-      <c r="AG5" s="15">
-        <f t="shared" si="19"/>
-        <v>61983.47</v>
-      </c>
-      <c r="AH5" s="16">
-        <f t="shared" si="20"/>
-        <v>7.0026000000000002</v>
+        <v>30710964277-1</v>
+      </c>
+      <c r="AG5" s="1">
+        <f>IF(K4=K5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="1">
+        <f>IF(K5=K6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI5" s="1" t="str">
+        <f>RIGHT(F5)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ5" s="1">
+        <f>IF(LEFT(F5,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="13">
+        <f>CEILING(N5*M5*(1+P5),500)</f>
+        <v>206500</v>
+      </c>
+      <c r="AM5" s="13">
+        <f>ROUND((AL5/(1+P5)),2)</f>
+        <v>170661.16</v>
+      </c>
+      <c r="AN5" s="18">
+        <f>ROUND(AM5/N5,6)</f>
+        <v>9.1396619999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44992</v>
       </c>
       <c r="B6" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C6),MONTH(C6),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A6,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A6+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>36</v>
@@ -1762,102 +1918,129 @@
         <v>9</v>
       </c>
       <c r="J6" s="3">
-        <v>30684125792</v>
+        <v>33610006189</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f>"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M6" s="4">
-        <v>7</v>
-      </c>
-      <c r="N6" s="2">
-        <v>8851.52</v>
+        <v>5.0898839999999996</v>
+      </c>
+      <c r="N6" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O6" s="5">
-        <v>61983.47</v>
+        <f>ROUND(M6*N6,6)</f>
+        <v>95041.317079999993</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>38</v>
       </c>
       <c r="Q6" s="11" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="R6" s="11" t="s">
         <v>46</v>
       </c>
       <c r="S6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" s="13">
+        <v>77</v>
+      </c>
+      <c r="T6" s="12">
         <v>44816</v>
       </c>
-      <c r="U6" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="U6" s="14">
+        <f>COUNTIFS($F$1:F6,F6,$K$1:K6,K6)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V6" s="14" t="str">
+        <f>SUBSTITUTE(M6,",",".")</f>
+        <v>5.089884</v>
+      </c>
+      <c r="W6" s="1" t="str">
+        <f>TEXT(R6,"00000")</f>
         <v>00002</v>
       </c>
-      <c r="V6" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000151</v>
-      </c>
-      <c r="W6" s="1" t="str">
+      <c r="X6" s="1" t="str">
+        <f>TEXT(S6,"00000000")</f>
+        <v>00000003</v>
+      </c>
+      <c r="Y6" s="1" t="str">
         <f>TEXT(T6,"DD/MM/aaaa")</f>
         <v>12/09/2022</v>
       </c>
-      <c r="X6" s="14">
-        <f t="shared" si="13"/>
-        <v>13016.53</v>
-      </c>
-      <c r="Y6" s="14">
-        <f t="shared" si="14"/>
-        <v>75000</v>
-      </c>
-      <c r="Z6" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>75000.00</v>
-      </c>
-      <c r="AA6" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z6" s="13">
+        <f>ROUND(O6*P6,2)</f>
+        <v>19958.68</v>
+      </c>
+      <c r="AA6" s="13">
+        <f>O6+Z6</f>
+        <v>114999.99708</v>
+      </c>
+      <c r="AB6" s="10" t="str">
+        <f>IF(RIGHT(F6,1)="A",SUBSTITUTE(TEXT(O6,"0,00"),",","."),SUBSTITUTE(TEXT(AA6,"0,00"),",","."))</f>
+        <v>95041.32</v>
+      </c>
+      <c r="AC6" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(54501-54500.002432,"0,00"),",",".")</f>
+        <v>1.00</v>
+      </c>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1">
+        <f>ROW(K6)</f>
         <v>6</v>
       </c>
-      <c r="AD6" s="1" t="str">
+      <c r="AF6" s="15" t="str">
         <f>J6&amp;"-"&amp;COUNTIF($J$1:J6,J6)</f>
-        <v>30684125792-2</v>
-      </c>
-      <c r="AF6" s="15">
-        <f t="shared" si="18"/>
-        <v>75000</v>
-      </c>
-      <c r="AG6" s="15">
-        <f t="shared" si="19"/>
-        <v>61983.47</v>
-      </c>
-      <c r="AH6" s="16">
-        <f t="shared" si="20"/>
-        <v>7.0026000000000002</v>
+        <v>33610006189-1</v>
+      </c>
+      <c r="AG6" s="1">
+        <f>IF(K5=K6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="1">
+        <f>IF(K6=K7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI6" s="1" t="str">
+        <f>RIGHT(F6)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ6" s="1">
+        <f>IF(LEFT(F6,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="13">
+        <f>CEILING(N6*M6*(1+P6),500)</f>
+        <v>115000</v>
+      </c>
+      <c r="AM6" s="13">
+        <f>ROUND((AL6/(1+P6)),2)</f>
+        <v>95041.32</v>
+      </c>
+      <c r="AN6" s="18">
+        <f>ROUND(AM6/N6,6)</f>
+        <v>5.0898839999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44992</v>
       </c>
       <c r="B7" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C7),MONTH(C7),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A7,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A7+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E7" s="2">
@@ -1876,23 +2059,23 @@
         <v>9</v>
       </c>
       <c r="J7" s="3">
-        <v>30525733870</v>
+        <v>33610006189</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B7,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>37</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="M7" s="4">
-        <v>8.0299999999999994</v>
-      </c>
-      <c r="N7" s="2">
-        <v>8851.52</v>
+        <v>5.0898839999999996</v>
+      </c>
+      <c r="N7" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O7" s="5">
-        <v>71074.38</v>
+        <f>ROUND(M7*N7,6)</f>
+        <v>95041.317079999993</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>38</v>
@@ -1900,71 +2083,96 @@
       <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="14">
+        <f>COUNTIFS($F$1:F7,F7,$K$1:K7,K7)+1</f>
+        <v>3</v>
+      </c>
+      <c r="V7" s="14" t="str">
+        <f>SUBSTITUTE(M7,",",".")</f>
+        <v>5.089884</v>
+      </c>
+      <c r="W7" s="1" t="str">
+        <f>TEXT(R7,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V7" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X7" s="1" t="str">
+        <f>TEXT(S7,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W7" s="1" t="str">
+      <c r="Y7" s="1" t="str">
         <f>TEXT(T7,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X7" s="14">
-        <f t="shared" si="13"/>
-        <v>14925.62</v>
-      </c>
-      <c r="Y7" s="14">
-        <f t="shared" si="14"/>
-        <v>86000</v>
-      </c>
-      <c r="Z7" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>71074.38</v>
-      </c>
-      <c r="AA7" s="10" t="str">
-        <f t="shared" si="16"/>
+      <c r="Z7" s="13">
+        <f>ROUND(O7*P7,2)</f>
+        <v>19958.68</v>
+      </c>
+      <c r="AA7" s="13">
+        <f>O7+Z7</f>
+        <v>114999.99708</v>
+      </c>
+      <c r="AB7" s="10" t="str">
+        <f>IF(RIGHT(F7,1)="A",SUBSTITUTE(TEXT(O7,"0,00"),",","."),SUBSTITUTE(TEXT(AA7,"0,00"),",","."))</f>
+        <v>95041.32</v>
+      </c>
+      <c r="AC7" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA7,0)-AA7,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1">
-        <f t="shared" si="17"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1">
+        <f>ROW(K7)</f>
         <v>7</v>
       </c>
-      <c r="AD7" s="1" t="str">
+      <c r="AF7" s="15" t="str">
         <f>J7&amp;"-"&amp;COUNTIF($J$1:J7,J7)</f>
-        <v>30525733870-1</v>
-      </c>
-      <c r="AF7" s="15">
-        <f t="shared" si="18"/>
-        <v>86500</v>
-      </c>
-      <c r="AG7" s="15">
-        <f t="shared" si="19"/>
-        <v>71487.600000000006</v>
-      </c>
-      <c r="AH7" s="16">
-        <f t="shared" si="20"/>
-        <v>8.0762999999999998</v>
+        <v>33610006189-2</v>
+      </c>
+      <c r="AG7" s="1">
+        <f>IF(K6=K7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH7" s="1">
+        <f>IF(K7=K8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="1" t="str">
+        <f>RIGHT(F7)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ7" s="1">
+        <f>IF(LEFT(F7,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="13">
+        <f>CEILING(N7*M7*(1+P7),500)</f>
+        <v>115000</v>
+      </c>
+      <c r="AM7" s="13">
+        <f>ROUND((AL7/(1+P7)),2)</f>
+        <v>95041.32</v>
+      </c>
+      <c r="AN7" s="18">
+        <f>ROUND(AM7/N7,6)</f>
+        <v>5.0898839999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44992</v>
       </c>
       <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C8),MONTH(C8),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A8,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A8+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E8" s="2">
@@ -1983,23 +2191,24 @@
         <v>9</v>
       </c>
       <c r="J8" s="3">
-        <v>30710964277</v>
+        <v>33615420269</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L8" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
         <v>Honorarios Febrero</v>
       </c>
       <c r="M8" s="4">
-        <v>9.01</v>
-      </c>
-      <c r="N8" s="2">
-        <v>8851.52</v>
+        <v>10.091248999999999</v>
+      </c>
+      <c r="N8" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O8" s="5">
-        <v>79752.070000000007</v>
+        <f>ROUND(M8*N8,6)</f>
+        <v>188429.75516500001</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>38</v>
@@ -2007,71 +2216,96 @@
       <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="14">
+        <f>COUNTIFS($F$1:F8,F8,$K$1:K8,K8)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V8" s="14" t="str">
+        <f>SUBSTITUTE(M8,",",".")</f>
+        <v>10.091249</v>
+      </c>
+      <c r="W8" s="1" t="str">
+        <f>TEXT(R8,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V8" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X8" s="1" t="str">
+        <f>TEXT(S8,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W8" s="1" t="str">
+      <c r="Y8" s="1" t="str">
         <f>TEXT(T8,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X8" s="14">
-        <f t="shared" si="13"/>
-        <v>16747.93</v>
-      </c>
-      <c r="Y8" s="14">
-        <f t="shared" si="14"/>
-        <v>96500</v>
-      </c>
-      <c r="Z8" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>79752.07</v>
-      </c>
-      <c r="AA8" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z8" s="13">
+        <f>ROUND(O8*P8,2)</f>
+        <v>39570.25</v>
+      </c>
+      <c r="AA8" s="13">
+        <f>O8+Z8</f>
+        <v>228000.00516500001</v>
+      </c>
+      <c r="AB8" s="10" t="str">
+        <f>IF(RIGHT(F8,1)="A",SUBSTITUTE(TEXT(O8,"0,00"),",","."),SUBSTITUTE(TEXT(AA8,"0,00"),",","."))</f>
+        <v>188429.76</v>
+      </c>
+      <c r="AC8" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA8,0)-AA8,"0,00"),",",".")</f>
+        <v>0.99</v>
+      </c>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1">
+        <f>ROW(K8)</f>
         <v>8</v>
       </c>
-      <c r="AD8" s="1" t="str">
+      <c r="AF8" s="15" t="str">
         <f>J8&amp;"-"&amp;COUNTIF($J$1:J8,J8)</f>
-        <v>30710964277-1</v>
-      </c>
-      <c r="AF8" s="15">
-        <f t="shared" si="18"/>
-        <v>97000</v>
-      </c>
-      <c r="AG8" s="15">
-        <f t="shared" si="19"/>
-        <v>80165.289999999994</v>
-      </c>
-      <c r="AH8" s="16">
-        <f t="shared" si="20"/>
-        <v>9.0566999999999993</v>
+        <v>33615420269-1</v>
+      </c>
+      <c r="AG8" s="1">
+        <f>IF(K7=K8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="1">
+        <f>IF(K8=K9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="1" t="str">
+        <f>RIGHT(F8)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ8" s="1">
+        <f>IF(LEFT(F8,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="13">
+        <f>CEILING(N8*M8*(1+P8),500)</f>
+        <v>228500</v>
+      </c>
+      <c r="AM8" s="13">
+        <f>ROUND((AL8/(1+P8)),2)</f>
+        <v>188842.98</v>
+      </c>
+      <c r="AN8" s="18">
+        <f>ROUND(AM8/N8,6)</f>
+        <v>10.113379</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44992</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C9),MONTH(C9),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A9,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A9+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E9" s="2">
@@ -2084,29 +2318,30 @@
         <v>39</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="3">
-        <v>33615420269</v>
+      <c r="J9" s="2">
+        <v>20147130202</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="L9" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B9,"mmmm"))</f>
         <v>Honorarios Febrero</v>
       </c>
       <c r="M9" s="4">
-        <v>10.039999999999999</v>
-      </c>
-      <c r="N9" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N9" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O9" s="5">
-        <v>88842.97</v>
+        <f>ROUND(M9*N9,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>38</v>
@@ -2114,71 +2349,96 @@
       <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="14">
+        <f>COUNTIFS($F$1:F9,F9,$K$1:K9,K9)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V9" s="14" t="str">
+        <f>SUBSTITUTE(M9,",",".")</f>
+        <v>1.084366</v>
+      </c>
+      <c r="W9" s="1" t="str">
+        <f>TEXT(R9,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V9" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X9" s="1" t="str">
+        <f>TEXT(S9,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W9" s="1" t="str">
+      <c r="Y9" s="1" t="str">
         <f>TEXT(T9,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X9" s="14">
-        <f t="shared" si="13"/>
-        <v>18657.02</v>
-      </c>
-      <c r="Y9" s="14">
-        <f t="shared" si="14"/>
-        <v>107499.99</v>
-      </c>
-      <c r="Z9" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>88842.97</v>
-      </c>
-      <c r="AA9" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.01</v>
-      </c>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z9" s="13">
+        <f>ROUND(O9*P9,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA9" s="13">
+        <f>O9+Z9</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB9" s="10" t="str">
+        <f>IF(RIGHT(F9,1)="A",SUBSTITUTE(TEXT(O9,"0,00"),",","."),SUBSTITUTE(TEXT(AA9,"0,00"),",","."))</f>
+        <v>20247.92</v>
+      </c>
+      <c r="AC9" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA9,0)-AA9,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1">
+        <f>ROW(K9)</f>
         <v>9</v>
       </c>
-      <c r="AD9" s="1" t="str">
+      <c r="AF9" s="15" t="str">
         <f>J9&amp;"-"&amp;COUNTIF($J$1:J9,J9)</f>
-        <v>33615420269-1</v>
-      </c>
-      <c r="AF9" s="15">
-        <f t="shared" si="18"/>
-        <v>108000</v>
-      </c>
-      <c r="AG9" s="15">
-        <f t="shared" si="19"/>
-        <v>89256.2</v>
-      </c>
-      <c r="AH9" s="16">
-        <f t="shared" si="20"/>
-        <v>10.0837</v>
+        <v>20147130202-1</v>
+      </c>
+      <c r="AG9" s="1">
+        <f>IF(K8=K9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="1">
+        <f>IF(K9=K10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="1" t="str">
+        <f>RIGHT(F9)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ9" s="1">
+        <f>IF(LEFT(F9,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="13">
+        <f>CEILING(N9*M9*(1+P9),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM9" s="13">
+        <f>ROUND((AL9/(1+P9)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN9" s="18">
+        <f>ROUND(AM9/N9,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44992</v>
       </c>
       <c r="B10" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C10),MONTH(C10),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A10,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A10+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E10" s="2">
@@ -2191,28 +2451,30 @@
         <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="3">
-        <v>30525390086</v>
+      <c r="J10" s="2">
+        <v>20374730429</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="L10" s="1" t="str">
+        <f>"Honorarios "&amp;PROPER(TEXT(B10,"mmmm"))</f>
+        <v>Honorarios Febrero</v>
       </c>
       <c r="M10" s="4">
-        <v>9.01</v>
-      </c>
-      <c r="N10" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N10" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O10" s="5">
-        <v>79752.070000000007</v>
+        <f>ROUND(M10*N10,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>38</v>
@@ -2220,90 +2482,115 @@
       <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="14">
+        <f>COUNTIFS($F$1:F10,F10,$K$1:K10,K10)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V10" s="14" t="str">
+        <f>SUBSTITUTE(M10,",",".")</f>
+        <v>1.084366</v>
+      </c>
+      <c r="W10" s="1" t="str">
+        <f>TEXT(R10,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V10" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X10" s="1" t="str">
+        <f>TEXT(S10,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W10" s="1" t="str">
+      <c r="Y10" s="1" t="str">
         <f>TEXT(T10,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X10" s="14">
-        <f t="shared" si="13"/>
-        <v>16747.93</v>
-      </c>
-      <c r="Y10" s="14">
-        <f t="shared" si="14"/>
-        <v>96500</v>
-      </c>
-      <c r="Z10" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>79752.07</v>
-      </c>
-      <c r="AA10" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z10" s="13">
+        <f>ROUND(O10*P10,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA10" s="13">
+        <f>O10+Z10</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB10" s="10" t="str">
+        <f>IF(RIGHT(F10,1)="A",SUBSTITUTE(TEXT(O10,"0,00"),",","."),SUBSTITUTE(TEXT(AA10,"0,00"),",","."))</f>
+        <v>20247.92</v>
+      </c>
+      <c r="AC10" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA10,0)-AA10,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1">
+        <f>ROW(K10)</f>
         <v>10</v>
       </c>
-      <c r="AD10" s="1" t="str">
+      <c r="AF10" s="15" t="str">
         <f>J10&amp;"-"&amp;COUNTIF($J$1:J10,J10)</f>
-        <v>30525390086-1</v>
-      </c>
-      <c r="AF10" s="15">
-        <f t="shared" si="18"/>
-        <v>97000</v>
-      </c>
-      <c r="AG10" s="15">
-        <f t="shared" si="19"/>
-        <v>80165.289999999994</v>
-      </c>
-      <c r="AH10" s="16">
-        <f t="shared" si="20"/>
-        <v>9.0566999999999993</v>
+        <v>20374730429-1</v>
+      </c>
+      <c r="AG10" s="1">
+        <f>IF(K9=K10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH10" s="1">
+        <f>IF(K10=K11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AI10" s="1" t="str">
+        <f>RIGHT(F10)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ10" s="1">
+        <f>IF(LEFT(F10,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="13">
+        <f>CEILING(N10*M10*(1+P10),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM10" s="13">
+        <f>ROUND((AL10/(1+P10)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN10" s="18">
+        <f>ROUND(AM10/N10,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44992</v>
       </c>
       <c r="B11" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C11),MONTH(C11),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A11,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A11+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="J11" s="2">
-        <v>20374730429</v>
+        <v>37473042</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>56</v>
@@ -2313,13 +2600,14 @@
         <v>Honorarios Febrero</v>
       </c>
       <c r="M11" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N11" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N11" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O11" s="5">
-        <v>9090.91</v>
+        <f>ROUND(M11*N11,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>38</v>
@@ -2327,106 +2615,132 @@
       <c r="Q11" s="11"/>
       <c r="R11" s="11"/>
       <c r="S11" s="11"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="14">
+        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V11" s="14" t="str">
+        <f>SUBSTITUTE(M11,",",".")</f>
+        <v>1.084366</v>
+      </c>
+      <c r="W11" s="1" t="str">
+        <f>TEXT(R11,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V11" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X11" s="1" t="str">
+        <f>TEXT(S11,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W11" s="1" t="str">
+      <c r="Y11" s="1" t="str">
         <f>TEXT(T11,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X11" s="14">
-        <f t="shared" si="13"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y11" s="14">
-        <f t="shared" si="14"/>
-        <v>11000</v>
-      </c>
-      <c r="Z11" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>9090.91</v>
-      </c>
-      <c r="AA11" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z11" s="13">
+        <f>ROUND(O11*P11,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA11" s="13">
+        <f>O11+Z11</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB11" s="10" t="str">
+        <f>IF(RIGHT(F11,1)="A",SUBSTITUTE(TEXT(O11,"0,00"),",","."),SUBSTITUTE(TEXT(AA11,"0,00"),",","."))</f>
+        <v>24499.98</v>
+      </c>
+      <c r="AC11" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA11,0)-AA11,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1">
+        <f>ROW(K11)</f>
         <v>11</v>
       </c>
-      <c r="AD11" s="1" t="str">
+      <c r="AF11" s="15" t="str">
         <f>J11&amp;"-"&amp;COUNTIF($J$1:J11,J11)</f>
-        <v>20374730429-1</v>
-      </c>
-      <c r="AF11" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG11" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH11" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+        <v>37473042-1</v>
+      </c>
+      <c r="AG11" s="1">
+        <f>IF(K10=K11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AH11" s="1">
+        <f>IF(K11=K12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI11" s="1" t="str">
+        <f>RIGHT(F11)</f>
+        <v>B</v>
+      </c>
+      <c r="AJ11" s="1">
+        <f>IF(LEFT(F11,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="13">
+        <f>CEILING(N11*M11*(1+P11),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM11" s="13">
+        <f>ROUND((AL11/(1+P11)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN11" s="18">
+        <f>ROUND(AM11/N11,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>44992</v>
       </c>
       <c r="B12" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C12),MONTH(C12),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A12,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A12+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J12" s="2">
-        <v>20147130202</v>
+        <v>30707354719</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L12" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B12,"mmmm"))</f>
         <v>Honorarios Febrero</v>
       </c>
       <c r="M12" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N12" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N12" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O12" s="5">
-        <v>9090.91</v>
+        <f>ROUND(M12*N12,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>38</v>
@@ -2434,106 +2748,130 @@
       <c r="Q12" s="11"/>
       <c r="R12" s="11"/>
       <c r="S12" s="11"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="14">
+        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V12" s="14" t="str">
+        <f>SUBSTITUTE(M12,",",".")</f>
+        <v>1.084366</v>
+      </c>
+      <c r="W12" s="1" t="str">
+        <f>TEXT(R12,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V12" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X12" s="1" t="str">
+        <f>TEXT(S12,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W12" s="1" t="str">
+      <c r="Y12" s="1" t="str">
         <f>TEXT(T12,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X12" s="14">
-        <f t="shared" si="13"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y12" s="14">
-        <f t="shared" si="14"/>
-        <v>11000</v>
-      </c>
-      <c r="Z12" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>9090.91</v>
-      </c>
-      <c r="AA12" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z12" s="13">
+        <f>ROUND(O12*P12,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA12" s="13">
+        <f>O12+Z12</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB12" s="10" t="str">
+        <f>IF(RIGHT(F12,1)="A",SUBSTITUTE(TEXT(O12,"0,00"),",","."),SUBSTITUTE(TEXT(AA12,"0,00"),",","."))</f>
+        <v>24499.98</v>
+      </c>
+      <c r="AC12" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA12,0)-AA12,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1">
+        <f>ROW(K12)</f>
         <v>12</v>
       </c>
-      <c r="AD12" s="1" t="str">
+      <c r="AF12" s="15" t="str">
         <f>J12&amp;"-"&amp;COUNTIF($J$1:J12,J12)</f>
-        <v>20147130202-1</v>
-      </c>
-      <c r="AF12" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG12" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH12" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+        <v>30707354719-1</v>
+      </c>
+      <c r="AG12" s="1">
+        <f>IF(K11=K12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="1">
+        <f>IF(K12=K13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI12" s="1" t="str">
+        <f>RIGHT(F12)</f>
+        <v>B</v>
+      </c>
+      <c r="AJ12" s="1">
+        <f>IF(LEFT(F12,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="13">
+        <f>CEILING(N12*M12*(1+P12),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM12" s="13">
+        <f>ROUND((AL12/(1+P12)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN12" s="18">
+        <f>ROUND(AM12/N12,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>44992</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C13),MONTH(C13),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A13,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A13+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E13" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="2">
-        <v>30707354719</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="L13" s="1" t="str">
         <f>"Honorarios "&amp;PROPER(TEXT(B13,"mmmm"))</f>
         <v>Honorarios Febrero</v>
       </c>
       <c r="M13" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N13" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N13" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O13" s="5">
-        <v>9090.91</v>
+        <f>ROUND(M13*N13,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>38</v>
@@ -2541,178 +2879,236 @@
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="14">
+        <f>COUNTIFS($F$1:F13,F13,$K$1:K13,K13)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V13" s="14" t="str">
+        <f>SUBSTITUTE(M13,",",".")</f>
+        <v>1.084366</v>
+      </c>
+      <c r="W13" s="1" t="str">
+        <f>TEXT(R13,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="V13" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X13" s="1" t="str">
+        <f>TEXT(S13,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="W13" s="1" t="str">
+      <c r="Y13" s="1" t="str">
         <f>TEXT(T13,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
-      <c r="X13" s="14">
-        <f t="shared" si="13"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y13" s="14">
-        <f t="shared" si="14"/>
-        <v>11000</v>
-      </c>
-      <c r="Z13" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA13" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z13" s="13">
+        <f>ROUND(O13*P13,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA13" s="13">
+        <f>O13+Z13</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB13" s="10" t="str">
+        <f>IF(RIGHT(F13,1)="A",SUBSTITUTE(TEXT(O13,"0,00"),",","."),SUBSTITUTE(TEXT(AA13,"0,00"),",","."))</f>
+        <v>24499.98</v>
+      </c>
+      <c r="AC13" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA13,0)-AA13,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1">
+        <f>ROW(K13)</f>
         <v>13</v>
       </c>
-      <c r="AD13" s="1" t="str">
+      <c r="AF13" s="15" t="str">
         <f>J13&amp;"-"&amp;COUNTIF($J$1:J13,J13)</f>
-        <v>30707354719-1</v>
-      </c>
-      <c r="AF13" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG13" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH13" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+        <v>-0</v>
+      </c>
+      <c r="AG13" s="1">
+        <f>IF(K12=K13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="1">
+        <f>IF(K13=K14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI13" s="1" t="str">
+        <f>RIGHT(F13)</f>
+        <v>C</v>
+      </c>
+      <c r="AJ13" s="1">
+        <f>IF(LEFT(F13,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="13">
+        <f>CEILING(N13*M13*(1+P13),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM13" s="13">
+        <f>ROUND((AL13/(1+P13)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN13" s="18">
+        <f>ROUND(AM13/N13,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>44992</v>
       </c>
       <c r="B14" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C14),MONTH(C14),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A14,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D14" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A14+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J14" s="2">
-        <v>37473042</v>
+        <v>9</v>
+      </c>
+      <c r="J14" s="3">
+        <v>30684125792</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B14,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>44</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="M14" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N14" s="2">
-        <v>8851.52</v>
+        <v>7.0594479999999997</v>
+      </c>
+      <c r="N14" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O14" s="5">
-        <v>9090.91</v>
+        <f>ROUND(M14*N14,6)</f>
+        <v>131818.17812999999</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>00000</v>
-      </c>
-      <c r="V14" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000000</v>
+      <c r="Q14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S14" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="T14" s="12">
+        <v>44816</v>
+      </c>
+      <c r="U14" s="14">
+        <f>COUNTIFS($F$1:F14,F14,$K$1:K14,K14)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V14" s="14" t="str">
+        <f>SUBSTITUTE(M14,",",".")</f>
+        <v>7.059448</v>
       </c>
       <c r="W14" s="1" t="str">
+        <f>TEXT(R14,"00000")</f>
+        <v>00002</v>
+      </c>
+      <c r="X14" s="1" t="str">
+        <f>TEXT(S14,"00000000")</f>
+        <v>00000150</v>
+      </c>
+      <c r="Y14" s="1" t="str">
         <f>TEXT(T14,"DD/MM/aaaa")</f>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X14" s="14">
-        <f t="shared" si="13"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y14" s="14">
-        <f t="shared" si="14"/>
-        <v>11000</v>
-      </c>
-      <c r="Z14" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA14" s="10" t="str">
-        <f t="shared" si="16"/>
+        <v>12/09/2022</v>
+      </c>
+      <c r="Z14" s="13">
+        <f>ROUND(O14*P14,2)</f>
+        <v>27681.82</v>
+      </c>
+      <c r="AA14" s="13">
+        <f>O14+Z14</f>
+        <v>159499.99812999999</v>
+      </c>
+      <c r="AB14" s="10" t="str">
+        <f>IF(RIGHT(F14,1)="A",SUBSTITUTE(TEXT(O14,"0,00"),",","."),SUBSTITUTE(TEXT(AA14,"0,00"),",","."))</f>
+        <v>131818.18</v>
+      </c>
+      <c r="AC14" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA14,0)-AA14,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1">
-        <f t="shared" si="17"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1">
+        <f>ROW(K14)</f>
         <v>14</v>
       </c>
-      <c r="AD14" s="1" t="str">
+      <c r="AF14" s="15" t="str">
         <f>J14&amp;"-"&amp;COUNTIF($J$1:J14,J14)</f>
-        <v>37473042-1</v>
-      </c>
-      <c r="AF14" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG14" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH14" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+        <v>30684125792-1</v>
+      </c>
+      <c r="AG14" s="1">
+        <f>IF(K13=K14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH14" s="1">
+        <f>IF(K14=K15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI14" s="1" t="str">
+        <f>RIGHT(F14)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ14" s="1">
+        <f>IF(LEFT(F14,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="13">
+        <f>CEILING(N14*M14*(1+P14),500)</f>
+        <v>159500</v>
+      </c>
+      <c r="AM14" s="13">
+        <f>ROUND((AL14/(1+P14)),2)</f>
+        <v>131818.18</v>
+      </c>
+      <c r="AN14" s="18">
+        <f>ROUND(AM14/N14,6)</f>
+        <v>7.0594479999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>44992</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C15),MONTH(C15),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A15,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A15+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E15" s="2">
@@ -2740,13 +3136,14 @@
         <v>64</v>
       </c>
       <c r="M15" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N15" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N15" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O15" s="5">
-        <v>9090.91</v>
+        <f>ROUND(M15*N15,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>38</v>
@@ -2760,194 +3157,245 @@
       <c r="S15" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="T15" s="13">
+      <c r="T15" s="12">
         <v>44816</v>
       </c>
-      <c r="U15" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="U15" s="14">
+        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V15" s="14" t="str">
+        <f>SUBSTITUTE(M15,",",".")</f>
+        <v>1.084366</v>
+      </c>
+      <c r="W15" s="1" t="str">
+        <f>TEXT(R15,"00000")</f>
         <v>00002</v>
       </c>
-      <c r="V15" s="1" t="str">
-        <f t="shared" si="12"/>
+      <c r="X15" s="1" t="str">
+        <f>TEXT(S15,"00000000")</f>
         <v>00000152</v>
       </c>
-      <c r="W15" s="1" t="str">
+      <c r="Y15" s="1" t="str">
         <f>TEXT(T15,"DD/MM/aaaa")</f>
         <v>12/09/2022</v>
       </c>
-      <c r="X15" s="14">
-        <f t="shared" si="13"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y15" s="14">
-        <f t="shared" si="14"/>
-        <v>11000</v>
-      </c>
-      <c r="Z15" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA15" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1">
-        <f t="shared" si="17"/>
+      <c r="Z15" s="13">
+        <f>ROUND(O15*P15,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA15" s="13">
+        <f>O15+Z15</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB15" s="10" t="str">
+        <f>IF(RIGHT(F15,1)="A",SUBSTITUTE(TEXT(O15,"0,00"),",","."),SUBSTITUTE(TEXT(AA15,"0,00"),",","."))</f>
+        <v>24499.98</v>
+      </c>
+      <c r="AC15" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA15,0)-AA15,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1">
+        <f>ROW(K15)</f>
         <v>15</v>
       </c>
-      <c r="AD15" s="1" t="str">
+      <c r="AF15" s="15" t="str">
         <f>J15&amp;"-"&amp;COUNTIF($J$1:J15,J15)</f>
         <v>30707354719-2</v>
       </c>
-      <c r="AF15" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG15" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH15" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+      <c r="AG15" s="1">
+        <f>IF(K14=K15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH15" s="1">
+        <f>IF(K15=K16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI15" s="1" t="str">
+        <f>RIGHT(F15)</f>
+        <v>B</v>
+      </c>
+      <c r="AJ15" s="1">
+        <f>IF(LEFT(F15,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="13">
+        <f>CEILING(N15*M15*(1+P15),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM15" s="13">
+        <f>ROUND((AL15/(1+P15)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN15" s="18">
+        <f>ROUND(AM15/N15,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>44992</v>
       </c>
       <c r="B16" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C16),MONTH(C16),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A16,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A16+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="2">
-        <v>37473042</v>
+        <v>9</v>
+      </c>
+      <c r="J16" s="3">
+        <v>30684125792</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="M16" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N16" s="2">
-        <v>8851.52</v>
+        <v>7.0594479999999997</v>
+      </c>
+      <c r="N16" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O16" s="5">
-        <v>9090.91</v>
+        <f>ROUND(M16*N16,6)</f>
+        <v>131818.17812999999</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>38</v>
       </c>
       <c r="Q16" s="11" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="R16" s="11" t="s">
         <v>46</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T16" s="13">
+        <v>49</v>
+      </c>
+      <c r="T16" s="12">
         <v>44816</v>
       </c>
-      <c r="U16" s="1" t="str">
-        <f t="shared" si="11"/>
+      <c r="U16" s="14">
+        <f>COUNTIFS($F$1:F16,F16,$K$1:K16,K16)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V16" s="14" t="str">
+        <f>SUBSTITUTE(M16,",",".")</f>
+        <v>7.059448</v>
+      </c>
+      <c r="W16" s="1" t="str">
+        <f>TEXT(R16,"00000")</f>
         <v>00002</v>
       </c>
-      <c r="V16" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000153</v>
-      </c>
-      <c r="W16" s="1" t="str">
+      <c r="X16" s="1" t="str">
+        <f>TEXT(S16,"00000000")</f>
+        <v>00000151</v>
+      </c>
+      <c r="Y16" s="1" t="str">
         <f>TEXT(T16,"DD/MM/aaaa")</f>
         <v>12/09/2022</v>
       </c>
-      <c r="X16" s="14">
-        <f t="shared" si="13"/>
-        <v>1909.09</v>
-      </c>
-      <c r="Y16" s="14">
-        <f t="shared" si="14"/>
-        <v>11000</v>
-      </c>
-      <c r="Z16" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>11000.00</v>
-      </c>
-      <c r="AA16" s="10" t="str">
-        <f t="shared" si="16"/>
+      <c r="Z16" s="13">
+        <f>ROUND(O16*P16,2)</f>
+        <v>27681.82</v>
+      </c>
+      <c r="AA16" s="13">
+        <f>O16+Z16</f>
+        <v>159499.99812999999</v>
+      </c>
+      <c r="AB16" s="10" t="str">
+        <f>IF(RIGHT(F16,1)="A",SUBSTITUTE(TEXT(O16,"0,00"),",","."),SUBSTITUTE(TEXT(AA16,"0,00"),",","."))</f>
+        <v>131818.18</v>
+      </c>
+      <c r="AC16" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA16,0)-AA16,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1">
-        <f t="shared" si="17"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1">
+        <f>ROW(K16)</f>
         <v>16</v>
       </c>
-      <c r="AD16" s="1" t="str">
+      <c r="AF16" s="15" t="str">
         <f>J16&amp;"-"&amp;COUNTIF($J$1:J16,J16)</f>
-        <v>37473042-2</v>
-      </c>
-      <c r="AF16" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG16" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH16" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+        <v>30684125792-2</v>
+      </c>
+      <c r="AG16" s="1">
+        <f>IF(K15=K16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH16" s="1">
+        <f>IF(K16=K17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="1" t="str">
+        <f>RIGHT(F16)</f>
+        <v>A</v>
+      </c>
+      <c r="AJ16" s="1">
+        <f>IF(LEFT(F16,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="13">
+        <f>CEILING(N16*M16*(1+P16),500)</f>
+        <v>159500</v>
+      </c>
+      <c r="AM16" s="13">
+        <f>ROUND((AL16/(1+P16)),2)</f>
+        <v>131818.18</v>
+      </c>
+      <c r="AN16" s="18">
+        <f>ROUND(AM16/N16,6)</f>
+        <v>7.0594479999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>44992</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f>TEXT(DATE(YEAR(C17),MONTH(C17),1),"dd/mm/aaaa")</f>
         <v>01/02/2023</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>TEXT(EOMONTH(A17,-1),"dd/mm/aaaa")</f>
         <v>28/02/2023</v>
       </c>
       <c r="D17" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f>TEXT(A17+14,"dd/mm/aaaa")</f>
         <v>21/03/2023</v>
       </c>
       <c r="E17" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>39</v>
@@ -2958,86 +3406,121 @@
       <c r="I17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="2"/>
+      <c r="J17" s="2">
+        <v>37473042</v>
+      </c>
       <c r="K17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B17,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <v>56</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="M17" s="4">
-        <v>1.03</v>
-      </c>
-      <c r="N17" s="2">
-        <v>8851.52</v>
+        <v>1.0843659999999999</v>
+      </c>
+      <c r="N17" s="5">
+        <v>18672.59</v>
       </c>
       <c r="O17" s="5">
-        <v>0</v>
+        <f>ROUND(M17*N17,6)</f>
+        <v>20247.921728000001</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="1" t="str">
-        <f t="shared" si="11"/>
-        <v>00000</v>
-      </c>
-      <c r="V17" s="1" t="str">
-        <f t="shared" si="12"/>
-        <v>00000000</v>
+      <c r="Q17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="T17" s="12">
+        <v>44816</v>
+      </c>
+      <c r="U17" s="14">
+        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
+        <v>2</v>
+      </c>
+      <c r="V17" s="14" t="str">
+        <f>SUBSTITUTE(M17,",",".")</f>
+        <v>1.084366</v>
       </c>
       <c r="W17" s="1" t="str">
+        <f>TEXT(R17,"00000")</f>
+        <v>00002</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <f>TEXT(S17,"00000000")</f>
+        <v>00000153</v>
+      </c>
+      <c r="Y17" s="1" t="str">
         <f>TEXT(T17,"DD/MM/aaaa")</f>
-        <v>00/01/1900</v>
-      </c>
-      <c r="X17" s="14">
-        <f t="shared" si="13"/>
+        <v>12/09/2022</v>
+      </c>
+      <c r="Z17" s="13">
+        <f>ROUND(O17*P17,2)</f>
+        <v>4252.0600000000004</v>
+      </c>
+      <c r="AA17" s="13">
+        <f>O17+Z17</f>
+        <v>24499.981728000002</v>
+      </c>
+      <c r="AB17" s="10" t="str">
+        <f>IF(RIGHT(F17,1)="A",SUBSTITUTE(TEXT(O17,"0,00"),",","."),SUBSTITUTE(TEXT(AA17,"0,00"),",","."))</f>
+        <v>24499.98</v>
+      </c>
+      <c r="AC17" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AA17,0)-AA17,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1">
+        <f>ROW(K17)</f>
+        <v>17</v>
+      </c>
+      <c r="AF17" s="15" t="str">
+        <f>J17&amp;"-"&amp;COUNTIF($J$1:J17,J17)</f>
+        <v>37473042-2</v>
+      </c>
+      <c r="AG17" s="1">
+        <f>IF(K16=K17,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Y17" s="14">
-        <f t="shared" si="14"/>
+      <c r="AH17" s="1">
+        <f>IF(K17=K18,1,0)</f>
         <v>0</v>
       </c>
-      <c r="Z17" s="10" t="str">
-        <f t="shared" si="15"/>
-        <v>0.00</v>
-      </c>
-      <c r="AA17" s="10" t="str">
-        <f t="shared" si="16"/>
-        <v>0.00</v>
-      </c>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1">
-        <f t="shared" si="17"/>
-        <v>17</v>
-      </c>
-      <c r="AD17" s="1" t="str">
-        <f>J17&amp;"-"&amp;COUNTIF($J$1:J17,J17)</f>
-        <v>-0</v>
-      </c>
-      <c r="AF17" s="15">
-        <f t="shared" si="18"/>
-        <v>11500</v>
-      </c>
-      <c r="AG17" s="15">
-        <f t="shared" si="19"/>
-        <v>9504.1299999999992</v>
-      </c>
-      <c r="AH17" s="16">
-        <f t="shared" si="20"/>
-        <v>1.0737000000000001</v>
+      <c r="AI17" s="1" t="str">
+        <f>RIGHT(F17)</f>
+        <v>B</v>
+      </c>
+      <c r="AJ17" s="1">
+        <f>IF(LEFT(F17,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="13">
+        <f>CEILING(N17*M17*(1+P17),500)</f>
+        <v>24500</v>
+      </c>
+      <c r="AM17" s="13">
+        <f>ROUND((AL17/(1+P17)),2)</f>
+        <v>20247.93</v>
+      </c>
+      <c r="AN17" s="18">
+        <f>ROUND(AM17/N17,6)</f>
+        <v>1.0843659999999999</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB13">
-    <sortCondition ref="F2:F13"/>
-    <sortCondition ref="H2:H13"/>
-    <sortCondition ref="J2:J13"/>
+  <autoFilter ref="A1:AF17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AN17">
+    <sortCondition ref="F2:F17"/>
+    <sortCondition ref="H2:H17"/>
+    <sortCondition ref="J2:J17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
V 4.0.4.3: Optimize Bot Guarda Facturas
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC968624-FBDD-40A1-BDC3-910F33AEC68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B1469D-2909-4808-AD50-4CDD04401DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="81">
   <si>
     <t>Fecha</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>Precio Facturador</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -770,6 +773,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -816,7 +830,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -839,6 +853,7 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1201,12 +1216,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO17"/>
+  <dimension ref="A1:AP17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="W17" sqref="W2:W17"/>
+      <selection pane="bottomLeft" activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,7 +1252,7 @@
     <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1361,8 +1376,11 @@
       <c r="AO1" s="17" t="s">
         <v>33</v>
       </c>
+      <c r="AP1" s="20" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44992</v>
       </c>
@@ -1497,8 +1515,9 @@
         <f t="shared" ref="AO2:AO17" si="17">ROUND(AN2/N2,6)</f>
         <v>9.1396619999999995</v>
       </c>
+      <c r="AP2" s="2"/>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44992</v>
       </c>
@@ -1634,8 +1653,9 @@
         <f t="shared" si="17"/>
         <v>8.0774249999999999</v>
       </c>
+      <c r="AP3" s="2"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44992</v>
       </c>
@@ -1771,8 +1791,9 @@
         <f t="shared" si="17"/>
         <v>10.113379</v>
       </c>
+      <c r="AP4" s="2"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44992</v>
       </c>
@@ -1908,8 +1929,9 @@
         <f t="shared" si="17"/>
         <v>9.1396619999999995</v>
       </c>
+      <c r="AP5" s="2"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44992</v>
       </c>
@@ -2053,8 +2075,9 @@
         <f t="shared" si="17"/>
         <v>5.0898839999999996</v>
       </c>
+      <c r="AP6" s="2"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44992</v>
       </c>
@@ -2189,8 +2212,9 @@
         <f t="shared" si="17"/>
         <v>5.0898839999999996</v>
       </c>
+      <c r="AP7" s="2"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44992</v>
       </c>
@@ -2326,8 +2350,9 @@
         <f t="shared" si="17"/>
         <v>10.113379</v>
       </c>
+      <c r="AP8" s="2"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44992</v>
       </c>
@@ -2463,8 +2488,9 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP9" s="2"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44992</v>
       </c>
@@ -2600,8 +2626,9 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP10" s="2"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44992</v>
       </c>
@@ -2737,8 +2764,9 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP11" s="2"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>44992</v>
       </c>
@@ -2874,8 +2902,9 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP12" s="2"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>44992</v>
       </c>
@@ -3009,8 +3038,9 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP13" s="2"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>44992</v>
       </c>
@@ -3153,8 +3183,9 @@
         <f t="shared" si="17"/>
         <v>7.0594479999999997</v>
       </c>
+      <c r="AP14" s="2"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>44992</v>
       </c>
@@ -3297,8 +3328,9 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP15" s="2"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>44992</v>
       </c>
@@ -3441,8 +3473,9 @@
         <f t="shared" si="17"/>
         <v>7.0594479999999997</v>
       </c>
+      <c r="AP16" s="2"/>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>44992</v>
       </c>
@@ -3585,6 +3618,7 @@
         <f t="shared" si="17"/>
         <v>1.0843659999999999</v>
       </c>
+      <c r="AP17" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:AG17" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update Excel to math example
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA17A7AD-B1CF-43D6-BDE7-301E4FF7C091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A4A983-B810-488F-AA74-E7D42F96C4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
   <si>
     <t>Fecha</t>
   </si>
@@ -293,7 +293,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.000000_ ;_ * \-#,##0.000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.000000_ ;_ * \-#,##0.000000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -825,7 +825,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -848,8 +848,7 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1214,10 +1213,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="AB5" sqref="AB5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,28 +1378,29 @@
       <c r="AP1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="AQ1" s="20" t="s">
+      <c r="AQ1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="AR1" s="20" t="s">
+      <c r="AR1" s="19" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <v>44992</v>
+        <f ca="1">TODAY()</f>
+        <v>45051</v>
       </c>
       <c r="B2" s="9" t="str">
-        <f t="shared" ref="B2:B17" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
-        <v>01/02/2023</v>
+        <f t="shared" ref="B2:B17" ca="1" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
+        <v>01/04/2023</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f t="shared" ref="C2:C17" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
-        <v>28/02/2023</v>
+        <f t="shared" ref="C2:C17" ca="1" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
+        <v>30/04/2023</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f t="shared" ref="D2:D17" si="2">TEXT(A2+14,"dd/mm/aaaa")</f>
-        <v>21/03/2023</v>
+        <f t="shared" ref="D2:D17" ca="1" si="2">TEXT(A2+14,"dd/mm/aaaa")</f>
+        <v>19/05/2023</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1448,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="V2" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+        <f t="shared" ref="V2:V17" si="3">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
       <c r="W2" s="18" t="str">
@@ -1456,19 +1456,19 @@
         <v>19000.00</v>
       </c>
       <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:X17" si="3">TEXT(R2,"00000")</f>
+        <f t="shared" ref="X2:X17" si="4">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="Y2" s="1" t="str">
-        <f t="shared" ref="Y2:Y17" si="4">TEXT(S2,"00000000")</f>
+        <f t="shared" ref="Y2:Y17" si="5">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="Z2" s="1" t="str">
-        <f t="shared" ref="Z2:Z17" si="5">TEXT(T2,"DD/MM/aaaa")</f>
+        <f t="shared" ref="Z2:Z17" si="6">TEXT(T2,"DD/MM/aaaa")</f>
         <v>00/01/1900</v>
       </c>
       <c r="AA2" s="13">
-        <f>IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+        <f t="shared" ref="AA2:AA17" si="7">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
         <v>27942.15</v>
       </c>
       <c r="AB2" s="13">
@@ -1476,7 +1476,7 @@
         <v>160999.99</v>
       </c>
       <c r="AC2" s="10" t="str">
-        <f t="shared" ref="AC2:AC17" si="6">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+        <f t="shared" ref="AC2:AC17" si="8">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
       <c r="AD2" s="10" t="str">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF17" si="7">ROW(K2)</f>
+        <f t="shared" ref="AF2:AF17" si="9">ROW(K2)</f>
         <v>2</v>
       </c>
       <c r="AG2" s="15" t="str">
@@ -1493,15 +1493,15 @@
         <v>30525390086-1</v>
       </c>
       <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH17" si="8">IF(K1=K2,1,0)</f>
+        <f t="shared" ref="AH2:AH17" si="10">IF(K1=K2,1,0)</f>
         <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <f t="shared" ref="AI2:AI17" si="9">IF(K2=K3,1,0)</f>
+        <f t="shared" ref="AI2:AI17" si="11">IF(K2=K3,1,0)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="10">RIGHT(F2)</f>
+        <f t="shared" ref="AJ2:AJ17" si="12">RIGHT(F2)</f>
         <v>A</v>
       </c>
       <c r="AK2" s="1">
@@ -1514,18 +1514,18 @@
         <v>160999.98000000001</v>
       </c>
       <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="11">ROUND((AM2/(1+P2)),2)</f>
+        <f t="shared" ref="AN2:AN17" si="13">ROUND((AM2/(1+P2)),2)</f>
         <v>133057.82999999999</v>
       </c>
-      <c r="AO2" s="21">
-        <f>IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+      <c r="AO2" s="20">
+        <f t="shared" ref="AO2:AO17" si="14">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
         <v>7.003044</v>
       </c>
       <c r="AP2" s="13">
-        <f>IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+        <f t="shared" ref="AP2:AP17" si="15">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
         <v>161000</v>
       </c>
-      <c r="AQ2" s="21">
+      <c r="AQ2" s="20">
         <f>IF(AJ2="A",ROUND(AN2/N2,6),AP2/N2)</f>
         <v>7.003044</v>
       </c>
@@ -1533,19 +1533,20 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <v>44992</v>
+        <f t="shared" ref="A3:A17" ca="1" si="16">TODAY()</f>
+        <v>45051</v>
       </c>
       <c r="B3" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1569,8 +1570,8 @@
         <v>50</v>
       </c>
       <c r="L3" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M3" s="4">
         <v>8.0252280000000003</v>
@@ -1579,7 +1580,7 @@
         <v>19000</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O17" si="12">M3*N3</f>
+        <f t="shared" ref="O3:O17" si="17">M3*N3</f>
         <v>152479.33199999999</v>
       </c>
       <c r="P3" s="11" t="s">
@@ -1594,35 +1595,35 @@
         <v>2</v>
       </c>
       <c r="V3" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ3="A",ROUND(O3/N3,6),ROUND(AB3/N3,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>8.025228</v>
       </c>
       <c r="W3" s="18" t="str">
-        <f t="shared" ref="W3:W17" si="13">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+        <f t="shared" ref="W3:W17" si="18">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
       <c r="X3" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y3" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z3" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA3" s="13">
-        <f>IF(AJ3="A",ROUND(O3*P3,2),ROUND(O3*P3/(1+P3),2))</f>
+        <f t="shared" si="7"/>
         <v>32020.66</v>
       </c>
       <c r="AB3" s="13">
-        <f t="shared" ref="AB3:AB17" si="14">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
+        <f t="shared" ref="AB3:AB17" si="19">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
         <v>184499.99</v>
       </c>
       <c r="AC3" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>152479.33</v>
       </c>
       <c r="AD3" s="10" t="str">
@@ -1631,7 +1632,7 @@
       </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AG3" s="15" t="str">
@@ -1639,59 +1640,60 @@
         <v>30525733870-1</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK3" s="1">
-        <f t="shared" ref="AK2:AK17" si="15">IF(LEFT(F3,4)="Nota",0,1)</f>
+        <f t="shared" ref="AK3:AK17" si="20">IF(LEFT(F3,4)="Nota",0,1)</f>
         <v>1</v>
       </c>
       <c r="AL3" s="2"/>
       <c r="AM3" s="13">
-        <f t="shared" ref="AM3:AM17" si="16">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
+        <f t="shared" ref="AM3:AM17" si="21">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
         <v>184499.99</v>
       </c>
       <c r="AN3" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>152479.32999999999</v>
       </c>
-      <c r="AO3" s="21">
-        <f>IF(AJ3="A",ROUND(AN3/N3,6),AM3/N3)</f>
+      <c r="AO3" s="20">
+        <f t="shared" si="14"/>
         <v>8.0252280000000003</v>
       </c>
       <c r="AP3" s="13">
-        <f>IF(AJ3="A",ROUND(CEILING(N3*M3*(1+P3),500),2),ROUND(CEILING(N3*M3,500),2))</f>
+        <f t="shared" si="15"/>
         <v>184500</v>
       </c>
-      <c r="AQ3" s="21">
-        <f t="shared" ref="AQ3:AQ17" si="17">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
+      <c r="AQ3" s="20">
+        <f t="shared" ref="AQ3:AQ17" si="22">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
         <v>8.0252280000000003</v>
       </c>
       <c r="AR3" s="2"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B4" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C4" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D4" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1715,8 +1717,8 @@
         <v>42</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M4" s="4">
         <v>10.004348999999999</v>
@@ -1725,7 +1727,7 @@
         <v>19000</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P4" s="11" t="s">
@@ -1740,35 +1742,35 @@
         <v>2</v>
       </c>
       <c r="V4" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ4="A",ROUND(O4/N4,6),ROUND(AB4/N4,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>10.004349</v>
       </c>
       <c r="W4" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X4" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y4" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z4" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA4" s="13">
-        <f>IF(AJ4="A",ROUND(O4*P4,2),ROUND(O4*P4/(1+P4),2))</f>
+        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB4" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>229999.98</v>
       </c>
       <c r="AC4" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>190082.63</v>
       </c>
       <c r="AD4" s="10" t="str">
@@ -1777,7 +1779,7 @@
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AG4" s="15" t="str">
@@ -1785,59 +1787,60 @@
         <v>30610252334-1</v>
       </c>
       <c r="AH4" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK4" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL4" s="2"/>
       <c r="AM4" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>229999.98</v>
       </c>
       <c r="AN4" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>190082.63</v>
       </c>
-      <c r="AO4" s="21">
-        <f>IF(AJ4="A",ROUND(AN4/N4,6),AM4/N4)</f>
+      <c r="AO4" s="20">
+        <f t="shared" si="14"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP4" s="13">
-        <f>IF(AJ4="A",ROUND(CEILING(N4*M4*(1+P4),500),2),ROUND(CEILING(N4*M4,500),2))</f>
+        <f t="shared" si="15"/>
         <v>230000</v>
       </c>
-      <c r="AQ4" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ4" s="20">
+        <f t="shared" si="22"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AR4" s="2"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B5" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C5" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D5" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1861,8 +1864,8 @@
         <v>51</v>
       </c>
       <c r="L5" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M5" s="4">
         <v>9.0256629999999998</v>
@@ -1871,7 +1874,7 @@
         <v>19000</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>171487.59700000001</v>
       </c>
       <c r="P5" s="11" t="s">
@@ -1886,35 +1889,35 @@
         <v>2</v>
       </c>
       <c r="V5" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ5="A",ROUND(O5/N5,6),ROUND(AB5/N5,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>9.025663</v>
       </c>
       <c r="W5" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X5" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA5" s="13">
-        <f>IF(AJ5="A",ROUND(O5*P5,2),ROUND(O5*P5/(1+P5),2))</f>
+        <f t="shared" si="7"/>
         <v>36012.400000000001</v>
       </c>
       <c r="AB5" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>207500</v>
       </c>
       <c r="AC5" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>171487.60</v>
       </c>
       <c r="AD5" s="10" t="str">
@@ -1923,7 +1926,7 @@
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AG5" s="15" t="str">
@@ -1931,59 +1934,60 @@
         <v>30710964277-1</v>
       </c>
       <c r="AH5" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK5" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL5" s="2"/>
       <c r="AM5" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>207499.99</v>
       </c>
       <c r="AN5" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>171487.6</v>
       </c>
-      <c r="AO5" s="21">
-        <f>IF(AJ5="A",ROUND(AN5/N5,6),AM5/N5)</f>
+      <c r="AO5" s="20">
+        <f t="shared" si="14"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AP5" s="13">
-        <f>IF(AJ5="A",ROUND(CEILING(N5*M5*(1+P5),500),2),ROUND(CEILING(N5*M5,500),2))</f>
+        <f t="shared" si="15"/>
         <v>207500</v>
       </c>
-      <c r="AQ5" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ5" s="20">
+        <f t="shared" si="22"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AR5" s="2"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B6" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C6" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D6" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2007,8 +2011,8 @@
         <v>37</v>
       </c>
       <c r="L6" s="1" t="str">
-        <f>"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M6" s="4">
         <v>5.0239229999999999</v>
@@ -2017,7 +2021,7 @@
         <v>19000</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>95454.536999999997</v>
       </c>
       <c r="P6" s="11" t="s">
@@ -2040,35 +2044,35 @@
         <v>2</v>
       </c>
       <c r="V6" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ6="A",ROUND(O6/N6,6),ROUND(AB6/N6,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>5.023923</v>
       </c>
       <c r="W6" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X6" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y6" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000003</v>
       </c>
       <c r="Z6" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12/09/2022</v>
       </c>
       <c r="AA6" s="13">
-        <f>IF(AJ6="A",ROUND(O6*P6,2),ROUND(O6*P6/(1+P6),2))</f>
+        <f t="shared" si="7"/>
         <v>20045.45</v>
       </c>
       <c r="AB6" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>115499.99</v>
       </c>
       <c r="AC6" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>95454.54</v>
       </c>
       <c r="AD6" s="10" t="str">
@@ -2077,7 +2081,7 @@
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AG6" s="15" t="str">
@@ -2085,59 +2089,60 @@
         <v>33610006189-1</v>
       </c>
       <c r="AH6" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK6" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL6" s="2"/>
       <c r="AM6" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>115499.99</v>
       </c>
       <c r="AN6" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>95454.54</v>
       </c>
-      <c r="AO6" s="21">
-        <f>IF(AJ6="A",ROUND(AN6/N6,6),AM6/N6)</f>
+      <c r="AO6" s="20">
+        <f t="shared" si="14"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AP6" s="13">
-        <f>IF(AJ6="A",ROUND(CEILING(N6*M6*(1+P6),500),2),ROUND(CEILING(N6*M6,500),2))</f>
+        <f t="shared" si="15"/>
         <v>115500</v>
       </c>
-      <c r="AQ6" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ6" s="20">
+        <f t="shared" si="22"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AR6" s="2"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B7" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C7" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D7" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2170,7 +2175,7 @@
         <v>19000</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>95041.305999999997</v>
       </c>
       <c r="P7" s="11" t="s">
@@ -2185,44 +2190,44 @@
         <v>3</v>
       </c>
       <c r="V7" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ7="A",ROUND(O7/N7,6),ROUND(AB7/N7,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>5.002174</v>
       </c>
       <c r="W7" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y7" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z7" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA7" s="13">
-        <f>IF(AJ7="A",ROUND(O7*P7,2),ROUND(O7*P7/(1+P7),2))</f>
+        <f t="shared" si="7"/>
         <v>19958.669999999998</v>
       </c>
       <c r="AB7" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>114999.98</v>
       </c>
       <c r="AC7" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>95041.31</v>
       </c>
       <c r="AD7" s="10" t="str">
-        <f t="shared" ref="AD7:AD17" si="18">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
+        <f t="shared" ref="AD7:AD17" si="23">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="AG7" s="15" t="str">
@@ -2230,59 +2235,60 @@
         <v>33610006189-2</v>
       </c>
       <c r="AH7" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AI7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK7" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL7" s="2"/>
       <c r="AM7" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>114999.98</v>
       </c>
       <c r="AN7" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>95041.31</v>
       </c>
-      <c r="AO7" s="21">
-        <f>IF(AJ7="A",ROUND(AN7/N7,6),AM7/N7)</f>
+      <c r="AO7" s="20">
+        <f t="shared" si="14"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AP7" s="13">
-        <f>IF(AJ7="A",ROUND(CEILING(N7*M7*(1+P7),500),2),ROUND(CEILING(N7*M7,500),2))</f>
+        <f t="shared" si="15"/>
         <v>115000</v>
       </c>
-      <c r="AQ7" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ7" s="20">
+        <f t="shared" si="22"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AR7" s="2"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B8" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C8" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D8" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2306,8 +2312,8 @@
         <v>52</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f t="shared" ref="L8:L13" si="19">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Febrero</v>
+        <f t="shared" ref="L8:L13" ca="1" si="24">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M8" s="4">
         <v>10.004348999999999</v>
@@ -2316,7 +2322,7 @@
         <v>19000</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P8" s="11" t="s">
@@ -2331,44 +2337,44 @@
         <v>2</v>
       </c>
       <c r="V8" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ8="A",ROUND(O8/N8,6),ROUND(AB8/N8,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>10.004349</v>
       </c>
       <c r="W8" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X8" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y8" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z8" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA8" s="13">
-        <f>IF(AJ8="A",ROUND(O8*P8,2),ROUND(O8*P8/(1+P8),2))</f>
+        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB8" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>229999.98</v>
       </c>
       <c r="AC8" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>190082.63</v>
       </c>
       <c r="AD8" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.02</v>
       </c>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AG8" s="15" t="str">
@@ -2376,59 +2382,60 @@
         <v>33615420269-1</v>
       </c>
       <c r="AH8" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK8" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL8" s="2"/>
       <c r="AM8" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>229999.98</v>
       </c>
       <c r="AN8" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>190082.63</v>
       </c>
-      <c r="AO8" s="21">
-        <f>IF(AJ8="A",ROUND(AN8/N8,6),AM8/N8)</f>
+      <c r="AO8" s="20">
+        <f t="shared" si="14"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP8" s="13">
-        <f>IF(AJ8="A",ROUND(CEILING(N8*M8*(1+P8),500),2),ROUND(CEILING(N8*M8,500),2))</f>
+        <f t="shared" si="15"/>
         <v>230000</v>
       </c>
-      <c r="AQ8" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ8" s="20">
+        <f t="shared" si="22"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AR8" s="2"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B9" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C9" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D9" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2452,8 +2459,8 @@
         <v>57</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>Honorarios Febrero</v>
+        <f t="shared" ca="1" si="24"/>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M9" s="4">
         <v>1.0221830000000001</v>
@@ -2462,7 +2469,7 @@
         <v>19000</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>19421.477000000003</v>
       </c>
       <c r="P9" s="11" t="s">
@@ -2477,44 +2484,44 @@
         <v>2</v>
       </c>
       <c r="V9" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ9="A",ROUND(O9/N9,6),ROUND(AB9/N9,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.022183</v>
       </c>
       <c r="W9" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X9" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y9" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z9" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA9" s="13">
-        <f>IF(AJ9="A",ROUND(O9*P9,2),ROUND(O9*P9/(1+P9),2))</f>
+        <f t="shared" si="7"/>
         <v>4078.51</v>
       </c>
       <c r="AB9" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>23499.99</v>
       </c>
       <c r="AC9" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19421.48</v>
       </c>
       <c r="AD9" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="AG9" s="15" t="str">
@@ -2522,59 +2529,60 @@
         <v>20147130202-1</v>
       </c>
       <c r="AH9" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK9" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL9" s="2"/>
       <c r="AM9" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>23499.99</v>
       </c>
       <c r="AN9" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>19421.48</v>
       </c>
-      <c r="AO9" s="21">
-        <f>IF(AJ9="A",ROUND(AN9/N9,6),AM9/N9)</f>
+      <c r="AO9" s="20">
+        <f t="shared" si="14"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AP9" s="13">
-        <f>IF(AJ9="A",ROUND(CEILING(N9*M9*(1+P9),500),2),ROUND(CEILING(N9*M9,500),2))</f>
+        <f t="shared" si="15"/>
         <v>23500</v>
       </c>
-      <c r="AQ9" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ9" s="20">
+        <f t="shared" si="22"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AR9" s="2"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B10" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C10" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D10" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2598,8 +2606,8 @@
         <v>56</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>Honorarios Febrero</v>
+        <f t="shared" ca="1" si="24"/>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M10" s="4">
         <v>1.0439320000000001</v>
@@ -2608,7 +2616,7 @@
         <v>19000</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>19834.708000000002</v>
       </c>
       <c r="P10" s="11" t="s">
@@ -2623,44 +2631,44 @@
         <v>2</v>
       </c>
       <c r="V10" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ10="A",ROUND(O10/N10,6),ROUND(AB10/N10,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.043932</v>
       </c>
       <c r="W10" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X10" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y10" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z10" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA10" s="13">
-        <f>IF(AJ10="A",ROUND(O10*P10,2),ROUND(O10*P10/(1+P10),2))</f>
+        <f t="shared" si="7"/>
         <v>4165.29</v>
       </c>
       <c r="AB10" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>24000</v>
       </c>
       <c r="AC10" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19834.71</v>
       </c>
       <c r="AD10" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="AG10" s="15" t="str">
@@ -2668,59 +2676,60 @@
         <v>20374730429-1</v>
       </c>
       <c r="AH10" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="AJ10" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK10" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL10" s="2"/>
       <c r="AM10" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>24000</v>
       </c>
       <c r="AN10" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>19834.71</v>
       </c>
-      <c r="AO10" s="21">
-        <f>IF(AJ10="A",ROUND(AN10/N10,6),AM10/N10)</f>
+      <c r="AO10" s="20">
+        <f t="shared" si="14"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AP10" s="13">
-        <f>IF(AJ10="A",ROUND(CEILING(N10*M10*(1+P10),500),2),ROUND(CEILING(N10*M10,500),2))</f>
+        <f t="shared" si="15"/>
         <v>24000</v>
       </c>
-      <c r="AQ10" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ10" s="20">
+        <f t="shared" si="22"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AR10" s="2"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B11" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C11" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D11" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2744,8 +2753,8 @@
         <v>56</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>Honorarios Febrero</v>
+        <f t="shared" ca="1" si="24"/>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M11" s="4">
         <v>1.3</v>
@@ -2754,7 +2763,7 @@
         <v>10000</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>13000</v>
       </c>
       <c r="P11" s="11" t="s">
@@ -2769,44 +2778,44 @@
         <v>2</v>
       </c>
       <c r="V11" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ11="A",ROUND(O11/N11,6),ROUND(AB11/N11,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.3</v>
       </c>
       <c r="W11" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>10000.00</v>
       </c>
       <c r="X11" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y11" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z11" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA11" s="13">
-        <f>IF(AJ11="A",ROUND(O11*P11,2),ROUND(O11*P11/(1+P11),2))</f>
+        <f t="shared" si="7"/>
         <v>2256.1999999999998</v>
       </c>
       <c r="AB11" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>13000</v>
       </c>
       <c r="AC11" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>13000.00</v>
       </c>
       <c r="AD11" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="AG11" s="15" t="str">
@@ -2814,59 +2823,60 @@
         <v>37473042-1</v>
       </c>
       <c r="AH11" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK11" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL11" s="2"/>
       <c r="AM11" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>13000</v>
       </c>
       <c r="AN11" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>10743.8</v>
       </c>
-      <c r="AO11" s="21">
-        <f>IF(AJ11="A",ROUND(AN11/N11,6),AM11/N11)</f>
+      <c r="AO11" s="20">
+        <f t="shared" si="14"/>
         <v>1.3</v>
       </c>
       <c r="AP11" s="13">
-        <f>IF(AJ11="A",ROUND(CEILING(N11*M11*(1+P11),500),2),ROUND(CEILING(N11*M11,500),2))</f>
+        <f t="shared" si="15"/>
         <v>13000</v>
       </c>
-      <c r="AQ11" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ11" s="20">
+        <f t="shared" si="22"/>
         <v>1.3</v>
       </c>
       <c r="AR11" s="2"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B12" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C12" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D12" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -2890,8 +2900,8 @@
         <v>60</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>Honorarios Febrero</v>
+        <f t="shared" ca="1" si="24"/>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M12" s="4">
         <v>1.2105263157894737</v>
@@ -2900,7 +2910,7 @@
         <v>19000</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>23000</v>
       </c>
       <c r="P12" s="11" t="s">
@@ -2915,44 +2925,44 @@
         <v>2</v>
       </c>
       <c r="V12" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ12="A",ROUND(O12/N12,6),ROUND(AB12/N12,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.210526</v>
       </c>
       <c r="W12" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X12" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y12" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z12" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA12" s="13">
-        <f>IF(AJ12="A",ROUND(O12*P12,2),ROUND(O12*P12/(1+P12),2))</f>
+        <f t="shared" si="7"/>
         <v>3991.74</v>
       </c>
       <c r="AB12" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>23000</v>
       </c>
       <c r="AC12" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>23000.00</v>
       </c>
       <c r="AD12" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="AG12" s="15" t="str">
@@ -2960,59 +2970,60 @@
         <v>30707354719-1</v>
       </c>
       <c r="AH12" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK12" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL12" s="2"/>
       <c r="AM12" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>23000</v>
       </c>
       <c r="AN12" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>19008.259999999998</v>
       </c>
-      <c r="AO12" s="21">
-        <f>IF(AJ12="A",ROUND(AN12/N12,6),AM12/N12)</f>
+      <c r="AO12" s="20">
+        <f t="shared" si="14"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AP12" s="13">
-        <f>IF(AJ12="A",ROUND(CEILING(N12*M12*(1+P12),500),2),ROUND(CEILING(N12*M12,500),2))</f>
+        <f t="shared" si="15"/>
         <v>23000</v>
       </c>
-      <c r="AQ12" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ12" s="20">
+        <f t="shared" si="22"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AR12" s="2"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B13" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C13" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D13" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3034,8 +3045,8 @@
         <v>70</v>
       </c>
       <c r="L13" s="1" t="str">
-        <f t="shared" si="19"/>
-        <v>Honorarios Febrero</v>
+        <f t="shared" ca="1" si="24"/>
+        <v>Honorarios Abril</v>
       </c>
       <c r="M13" s="4">
         <v>1.5</v>
@@ -3044,12 +3055,10 @@
         <v>19000</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>28500</v>
       </c>
-      <c r="P13" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
@@ -3059,44 +3068,44 @@
         <v>2</v>
       </c>
       <c r="V13" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ13="A",ROUND(O13/N13,6),ROUND(AB13/N13,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W13" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X13" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="Y13" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="Z13" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>00/01/1900</v>
       </c>
       <c r="AA13" s="13">
-        <f>IF(AJ13="A",ROUND(O13*P13,2),ROUND(O13*P13/(1+P13),2))</f>
-        <v>4946.28</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="AB13" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>28500</v>
       </c>
       <c r="AC13" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>28500.00</v>
       </c>
       <c r="AD13" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="AG13" s="15" t="str">
@@ -3104,59 +3113,60 @@
         <v>-0</v>
       </c>
       <c r="AH13" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>C</v>
       </c>
       <c r="AK13" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="AL13" s="2"/>
       <c r="AM13" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
       <c r="AN13" s="13">
-        <f t="shared" si="11"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AO13" s="21">
-        <f>IF(AJ13="A",ROUND(AN13/N13,6),AM13/N13)</f>
+        <f t="shared" si="13"/>
+        <v>28500</v>
+      </c>
+      <c r="AO13" s="20">
+        <f t="shared" si="14"/>
         <v>1.5</v>
       </c>
       <c r="AP13" s="13">
-        <f>IF(AJ13="A",ROUND(CEILING(N13*M13*(1+P13),500),2),ROUND(CEILING(N13*M13,500),2))</f>
+        <f t="shared" si="15"/>
         <v>28500</v>
       </c>
-      <c r="AQ13" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ13" s="20">
+        <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
       <c r="AR13" s="2"/>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B14" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C14" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D14" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3189,7 +3199,7 @@
         <v>19000</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>133471.06700000001</v>
       </c>
       <c r="P14" s="11" t="s">
@@ -3212,44 +3222,44 @@
         <v>2</v>
       </c>
       <c r="V14" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ14="A",ROUND(O14/N14,6),ROUND(AB14/N14,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>7.024793</v>
       </c>
       <c r="W14" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X14" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y14" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000150</v>
       </c>
       <c r="Z14" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12/09/2022</v>
       </c>
       <c r="AA14" s="13">
-        <f>IF(AJ14="A",ROUND(O14*P14,2),ROUND(O14*P14/(1+P14),2))</f>
+        <f t="shared" si="7"/>
         <v>28028.92</v>
       </c>
       <c r="AB14" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>161499.99</v>
       </c>
       <c r="AC14" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>133471.07</v>
       </c>
       <c r="AD14" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="AG14" s="15" t="str">
@@ -3257,59 +3267,60 @@
         <v>30684125792-1</v>
       </c>
       <c r="AH14" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK14" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AL14" s="2"/>
       <c r="AM14" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>161499.99</v>
       </c>
       <c r="AN14" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>133471.07</v>
       </c>
-      <c r="AO14" s="21">
-        <f>IF(AJ14="A",ROUND(AN14/N14,6),AM14/N14)</f>
+      <c r="AO14" s="20">
+        <f t="shared" si="14"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AP14" s="13">
-        <f>IF(AJ14="A",ROUND(CEILING(N14*M14*(1+P14),500),2),ROUND(CEILING(N14*M14,500),2))</f>
+        <f t="shared" si="15"/>
         <v>161500</v>
       </c>
-      <c r="AQ14" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ14" s="20">
+        <f t="shared" si="22"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AR14" s="2"/>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B15" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C15" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D15" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3342,7 +3353,7 @@
         <v>19000</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>28500</v>
       </c>
       <c r="P15" s="11" t="s">
@@ -3365,44 +3376,44 @@
         <v>2</v>
       </c>
       <c r="V15" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ15="A",ROUND(O15/N15,6),ROUND(AB15/N15,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W15" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X15" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y15" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000152</v>
       </c>
       <c r="Z15" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12/09/2022</v>
       </c>
       <c r="AA15" s="13">
-        <f>IF(AJ15="A",ROUND(O15*P15,2),ROUND(O15*P15/(1+P15),2))</f>
+        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB15" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>28500</v>
       </c>
       <c r="AC15" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>28500.00</v>
       </c>
       <c r="AD15" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="AG15" s="15" t="str">
@@ -3410,59 +3421,60 @@
         <v>30707354719-2</v>
       </c>
       <c r="AH15" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK15" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AL15" s="2"/>
       <c r="AM15" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
       <c r="AN15" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>23553.72</v>
       </c>
-      <c r="AO15" s="21">
-        <f>IF(AJ15="A",ROUND(AN15/N15,6),AM15/N15)</f>
+      <c r="AO15" s="20">
+        <f t="shared" si="14"/>
         <v>1.5</v>
       </c>
       <c r="AP15" s="13">
-        <f>IF(AJ15="A",ROUND(CEILING(N15*M15*(1+P15),500),2),ROUND(CEILING(N15*M15,500),2))</f>
+        <f t="shared" si="15"/>
         <v>28500</v>
       </c>
-      <c r="AQ15" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ15" s="20">
+        <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
       <c r="AR15" s="2"/>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B16" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C16" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D16" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3495,7 +3507,7 @@
         <v>19000</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>133057.83600000001</v>
       </c>
       <c r="P16" s="11" t="s">
@@ -3518,44 +3530,44 @@
         <v>2</v>
       </c>
       <c r="V16" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ16="A",ROUND(O16/N16,6),ROUND(AB16/N16,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>7.003044</v>
       </c>
       <c r="W16" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X16" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y16" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000151</v>
       </c>
       <c r="Z16" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12/09/2022</v>
       </c>
       <c r="AA16" s="13">
-        <f>IF(AJ16="A",ROUND(O16*P16,2),ROUND(O16*P16/(1+P16),2))</f>
+        <f t="shared" si="7"/>
         <v>27942.15</v>
       </c>
       <c r="AB16" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>160999.99</v>
       </c>
       <c r="AC16" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>133057.84</v>
       </c>
       <c r="AD16" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="AG16" s="15" t="str">
@@ -3563,59 +3575,60 @@
         <v>30684125792-2</v>
       </c>
       <c r="AH16" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>A</v>
       </c>
       <c r="AK16" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AL16" s="2"/>
       <c r="AM16" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>160999.98000000001</v>
       </c>
       <c r="AN16" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>133057.82999999999</v>
       </c>
-      <c r="AO16" s="21">
-        <f>IF(AJ16="A",ROUND(AN16/N16,6),AM16/N16)</f>
+      <c r="AO16" s="20">
+        <f t="shared" si="14"/>
         <v>7.003044</v>
       </c>
       <c r="AP16" s="13">
-        <f>IF(AJ16="A",ROUND(CEILING(N16*M16*(1+P16),500),2),ROUND(CEILING(N16*M16,500),2))</f>
+        <f t="shared" si="15"/>
         <v>161000</v>
       </c>
-      <c r="AQ16" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ16" s="20">
+        <f t="shared" si="22"/>
         <v>7.003044</v>
       </c>
       <c r="AR16" s="2"/>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>44992</v>
+        <f t="shared" ca="1" si="16"/>
+        <v>45051</v>
       </c>
       <c r="B17" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>01/02/2023</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>01/04/2023</v>
       </c>
       <c r="C17" s="9" t="str">
-        <f t="shared" si="1"/>
-        <v>28/02/2023</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>30/04/2023</v>
       </c>
       <c r="D17" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>21/03/2023</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>19/05/2023</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3648,7 +3661,7 @@
         <v>19000</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>28500</v>
       </c>
       <c r="P17" s="11" t="s">
@@ -3671,44 +3684,44 @@
         <v>2</v>
       </c>
       <c r="V17" s="18" t="str">
-        <f>SUBSTITUTE(IF(AJ17="A",ROUND(O17/N17,6),ROUND(AB17/N17,6)),",",".")</f>
+        <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
       <c r="W17" s="18" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>19000.00</v>
       </c>
       <c r="X17" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="Y17" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00000153</v>
       </c>
       <c r="Z17" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12/09/2022</v>
       </c>
       <c r="AA17" s="13">
-        <f>IF(AJ17="A",ROUND(O17*P17,2),ROUND(O17*P17/(1+P17),2))</f>
+        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB17" s="13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>28500</v>
       </c>
       <c r="AC17" s="10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>28500.00</v>
       </c>
       <c r="AD17" s="10" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="AG17" s="15" t="str">
@@ -3716,40 +3729,40 @@
         <v>37473042-2</v>
       </c>
       <c r="AH17" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI17" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>B</v>
       </c>
       <c r="AK17" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="AL17" s="2"/>
       <c r="AM17" s="13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
       <c r="AN17" s="13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>23553.72</v>
       </c>
-      <c r="AO17" s="21">
-        <f>IF(AJ17="A",ROUND(AN17/N17,6),AM17/N17)</f>
+      <c r="AO17" s="20">
+        <f t="shared" si="14"/>
         <v>1.5</v>
       </c>
       <c r="AP17" s="13">
-        <f>IF(AJ17="A",ROUND(CEILING(N17*M17*(1+P17),500),2),ROUND(CEILING(N17*M17,500),2))</f>
+        <f t="shared" si="15"/>
         <v>28500</v>
       </c>
-      <c r="AQ17" s="21">
-        <f t="shared" si="17"/>
+      <c r="AQ17" s="20">
+        <f t="shared" si="22"/>
         <v>1.5</v>
       </c>
       <c r="AR17" s="2"/>

</xml_diff>

<commit_message>
Update Excels to match new version
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A4A983-B810-488F-AA74-E7D42F96C4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B821D4-C4DC-42AF-8412-DBE9F7B71DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1216,7 +1216,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A17"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1233,8 @@
     <col min="13" max="13" width="9.140625" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="9.140625" customWidth="1"/>
+    <col min="16" max="25" width="9.140625" customWidth="1"/>
+    <col min="26" max="26" width="11" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" customWidth="1"/>
@@ -1388,19 +1389,19 @@
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45051</v>
-      </c>
-      <c r="B2" s="9" t="str">
-        <f t="shared" ref="B2:B17" ca="1" si="0">TEXT(DATE(YEAR(C2),MONTH(C2),1),"dd/mm/aaaa")</f>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C2" s="9" t="str">
-        <f t="shared" ref="C2:C17" ca="1" si="1">TEXT(EOMONTH(A2,-1),"dd/mm/aaaa")</f>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D2" s="9" t="str">
-        <f t="shared" ref="D2:D17" ca="1" si="2">TEXT(A2+14,"dd/mm/aaaa")</f>
-        <v>19/05/2023</v>
+        <v>45107</v>
+      </c>
+      <c r="B2" s="9">
+        <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
+        <v>45047</v>
+      </c>
+      <c r="C2" s="9">
+        <f ca="1">EOMONTH(A2,-1)</f>
+        <v>45077</v>
+      </c>
+      <c r="D2" s="9">
+        <f ca="1">A2+14</f>
+        <v>45121</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1448,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="V2" s="18" t="str">
-        <f t="shared" ref="V2:V17" si="3">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+        <f t="shared" ref="V2:V17" si="0">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
       <c r="W2" s="18" t="str">
@@ -1456,19 +1457,19 @@
         <v>19000.00</v>
       </c>
       <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:X17" si="4">TEXT(R2,"00000")</f>
+        <f t="shared" ref="X2:X17" si="1">TEXT(R2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="Y2" s="1" t="str">
-        <f t="shared" ref="Y2:Y17" si="5">TEXT(S2,"00000000")</f>
+        <f t="shared" ref="Y2:Y17" si="2">TEXT(S2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="Z2" s="1" t="str">
-        <f t="shared" ref="Z2:Z17" si="6">TEXT(T2,"DD/MM/aaaa")</f>
-        <v>00/01/1900</v>
+      <c r="Z2" s="9">
+        <f>T2</f>
+        <v>0</v>
       </c>
       <c r="AA2" s="13">
-        <f t="shared" ref="AA2:AA17" si="7">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+        <f t="shared" ref="AA2:AA17" si="3">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
         <v>27942.15</v>
       </c>
       <c r="AB2" s="13">
@@ -1476,7 +1477,7 @@
         <v>160999.99</v>
       </c>
       <c r="AC2" s="10" t="str">
-        <f t="shared" ref="AC2:AC17" si="8">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+        <f t="shared" ref="AC2:AC17" si="4">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
       <c r="AD2" s="10" t="str">
@@ -1485,7 +1486,7 @@
       </c>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF17" si="9">ROW(K2)</f>
+        <f t="shared" ref="AF2:AF17" si="5">ROW(K2)</f>
         <v>2</v>
       </c>
       <c r="AG2" s="15" t="str">
@@ -1493,15 +1494,15 @@
         <v>30525390086-1</v>
       </c>
       <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH17" si="10">IF(K1=K2,1,0)</f>
+        <f t="shared" ref="AH2:AH17" si="6">IF(K1=K2,1,0)</f>
         <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <f t="shared" ref="AI2:AI17" si="11">IF(K2=K3,1,0)</f>
+        <f t="shared" ref="AI2:AI17" si="7">IF(K2=K3,1,0)</f>
         <v>0</v>
       </c>
       <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="12">RIGHT(F2)</f>
+        <f t="shared" ref="AJ2:AJ17" si="8">RIGHT(F2)</f>
         <v>A</v>
       </c>
       <c r="AK2" s="1">
@@ -1514,15 +1515,15 @@
         <v>160999.98000000001</v>
       </c>
       <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="13">ROUND((AM2/(1+P2)),2)</f>
+        <f t="shared" ref="AN2:AN17" si="9">ROUND((AM2/(1+P2)),2)</f>
         <v>133057.82999999999</v>
       </c>
       <c r="AO2" s="20">
-        <f t="shared" ref="AO2:AO17" si="14">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+        <f t="shared" ref="AO2:AO17" si="10">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
         <v>7.003044</v>
       </c>
       <c r="AP2" s="13">
-        <f t="shared" ref="AP2:AP17" si="15">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+        <f t="shared" ref="AP2:AP17" si="11">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
         <v>161000</v>
       </c>
       <c r="AQ2" s="20">
@@ -1533,20 +1534,20 @@
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A17" ca="1" si="16">TODAY()</f>
-        <v>45051</v>
-      </c>
-      <c r="B3" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C3" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D3" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ref="A3:A17" ca="1" si="12">TODAY()</f>
+        <v>45107</v>
+      </c>
+      <c r="B3" s="9">
+        <f t="shared" ref="B3:B17" ca="1" si="13">DATE(YEAR(C3),MONTH(C3),1)</f>
+        <v>45047</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C17" ca="1" si="14">EOMONTH(A3,-1)</f>
+        <v>45077</v>
+      </c>
+      <c r="D3" s="9">
+        <f t="shared" ref="D3:D17" ca="1" si="15">A3+14</f>
+        <v>45121</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1571,7 +1572,7 @@
       </c>
       <c r="L3" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M3" s="4">
         <v>8.0252280000000003</v>
@@ -1580,7 +1581,7 @@
         <v>19000</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O17" si="17">M3*N3</f>
+        <f t="shared" ref="O3:O17" si="16">M3*N3</f>
         <v>152479.33199999999</v>
       </c>
       <c r="P3" s="11" t="s">
@@ -1595,27 +1596,27 @@
         <v>2</v>
       </c>
       <c r="V3" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>8.025228</v>
+      </c>
+      <c r="W3" s="18" t="str">
+        <f t="shared" ref="W3:W17" si="17">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+        <v>19000.00</v>
+      </c>
+      <c r="X3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y3" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z3" s="9">
+        <f t="shared" ref="Z3:Z17" si="18">T3</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="13">
         <f t="shared" si="3"/>
-        <v>8.025228</v>
-      </c>
-      <c r="W3" s="18" t="str">
-        <f t="shared" ref="W3:W17" si="18">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
-        <v>19000.00</v>
-      </c>
-      <c r="X3" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y3" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z3" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA3" s="13">
-        <f t="shared" si="7"/>
         <v>32020.66</v>
       </c>
       <c r="AB3" s="13">
@@ -1623,7 +1624,7 @@
         <v>184499.99</v>
       </c>
       <c r="AC3" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>152479.33</v>
       </c>
       <c r="AD3" s="10" t="str">
@@ -1632,7 +1633,7 @@
       </c>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="AG3" s="15" t="str">
@@ -1640,15 +1641,15 @@
         <v>30525733870-1</v>
       </c>
       <c r="AH3" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ3" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK3" s="1">
@@ -1661,15 +1662,15 @@
         <v>184499.99</v>
       </c>
       <c r="AN3" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>152479.32999999999</v>
       </c>
       <c r="AO3" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>8.0252280000000003</v>
       </c>
       <c r="AP3" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>184500</v>
       </c>
       <c r="AQ3" s="20">
@@ -1680,20 +1681,20 @@
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B4" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C4" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D4" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B4" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D4" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1718,7 +1719,7 @@
       </c>
       <c r="L4" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M4" s="4">
         <v>10.004348999999999</v>
@@ -1727,7 +1728,7 @@
         <v>19000</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P4" s="11" t="s">
@@ -1742,27 +1743,27 @@
         <v>2</v>
       </c>
       <c r="V4" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10.004349</v>
+      </c>
+      <c r="W4" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z4" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="13">
         <f t="shared" si="3"/>
-        <v>10.004349</v>
-      </c>
-      <c r="W4" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X4" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y4" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z4" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA4" s="13">
-        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB4" s="13">
@@ -1770,7 +1771,7 @@
         <v>229999.98</v>
       </c>
       <c r="AC4" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>190082.63</v>
       </c>
       <c r="AD4" s="10" t="str">
@@ -1779,7 +1780,7 @@
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="AG4" s="15" t="str">
@@ -1787,15 +1788,15 @@
         <v>30610252334-1</v>
       </c>
       <c r="AH4" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ4" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK4" s="1">
@@ -1808,15 +1809,15 @@
         <v>229999.98</v>
       </c>
       <c r="AN4" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>190082.63</v>
       </c>
       <c r="AO4" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP4" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>230000</v>
       </c>
       <c r="AQ4" s="20">
@@ -1827,20 +1828,20 @@
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B5" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C5" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D5" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B5" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D5" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1865,7 +1866,7 @@
       </c>
       <c r="L5" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M5" s="4">
         <v>9.0256629999999998</v>
@@ -1874,7 +1875,7 @@
         <v>19000</v>
       </c>
       <c r="O5" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>171487.59700000001</v>
       </c>
       <c r="P5" s="11" t="s">
@@ -1889,27 +1890,27 @@
         <v>2</v>
       </c>
       <c r="V5" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>9.025663</v>
+      </c>
+      <c r="W5" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z5" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="13">
         <f t="shared" si="3"/>
-        <v>9.025663</v>
-      </c>
-      <c r="W5" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X5" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y5" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z5" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA5" s="13">
-        <f t="shared" si="7"/>
         <v>36012.400000000001</v>
       </c>
       <c r="AB5" s="13">
@@ -1917,7 +1918,7 @@
         <v>207500</v>
       </c>
       <c r="AC5" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>171487.60</v>
       </c>
       <c r="AD5" s="10" t="str">
@@ -1926,7 +1927,7 @@
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AG5" s="15" t="str">
@@ -1934,15 +1935,15 @@
         <v>30710964277-1</v>
       </c>
       <c r="AH5" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ5" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK5" s="1">
@@ -1955,15 +1956,15 @@
         <v>207499.99</v>
       </c>
       <c r="AN5" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>171487.6</v>
       </c>
       <c r="AO5" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AP5" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>207500</v>
       </c>
       <c r="AQ5" s="20">
@@ -1974,20 +1975,20 @@
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B6" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C6" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D6" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B6" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D6" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2012,7 +2013,7 @@
       </c>
       <c r="L6" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M6" s="4">
         <v>5.0239229999999999</v>
@@ -2021,7 +2022,7 @@
         <v>19000</v>
       </c>
       <c r="O6" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>95454.536999999997</v>
       </c>
       <c r="P6" s="11" t="s">
@@ -2044,27 +2045,27 @@
         <v>2</v>
       </c>
       <c r="V6" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5.023923</v>
+      </c>
+      <c r="W6" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000003</v>
+      </c>
+      <c r="Z6" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA6" s="13">
         <f t="shared" si="3"/>
-        <v>5.023923</v>
-      </c>
-      <c r="W6" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X6" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y6" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000003</v>
-      </c>
-      <c r="Z6" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA6" s="13">
-        <f t="shared" si="7"/>
         <v>20045.45</v>
       </c>
       <c r="AB6" s="13">
@@ -2072,7 +2073,7 @@
         <v>115499.99</v>
       </c>
       <c r="AC6" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>95454.54</v>
       </c>
       <c r="AD6" s="10" t="str">
@@ -2081,7 +2082,7 @@
       </c>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="AG6" s="15" t="str">
@@ -2089,15 +2090,15 @@
         <v>33610006189-1</v>
       </c>
       <c r="AH6" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK6" s="1">
@@ -2110,15 +2111,15 @@
         <v>115499.99</v>
       </c>
       <c r="AN6" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>95454.54</v>
       </c>
       <c r="AO6" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AP6" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>115500</v>
       </c>
       <c r="AQ6" s="20">
@@ -2129,20 +2130,20 @@
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B7" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C7" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D7" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B7" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2175,7 +2176,7 @@
         <v>19000</v>
       </c>
       <c r="O7" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>95041.305999999997</v>
       </c>
       <c r="P7" s="11" t="s">
@@ -2190,27 +2191,27 @@
         <v>3</v>
       </c>
       <c r="V7" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>5.002174</v>
+      </c>
+      <c r="W7" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z7" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA7" s="13">
         <f t="shared" si="3"/>
-        <v>5.002174</v>
-      </c>
-      <c r="W7" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X7" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y7" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z7" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA7" s="13">
-        <f t="shared" si="7"/>
         <v>19958.669999999998</v>
       </c>
       <c r="AB7" s="13">
@@ -2218,7 +2219,7 @@
         <v>114999.98</v>
       </c>
       <c r="AC7" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>95041.31</v>
       </c>
       <c r="AD7" s="10" t="str">
@@ -2227,7 +2228,7 @@
       </c>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="AG7" s="15" t="str">
@@ -2235,15 +2236,15 @@
         <v>33610006189-2</v>
       </c>
       <c r="AH7" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AI7" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ7" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK7" s="1">
@@ -2256,15 +2257,15 @@
         <v>114999.98</v>
       </c>
       <c r="AN7" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>95041.31</v>
       </c>
       <c r="AO7" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AP7" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>115000</v>
       </c>
       <c r="AQ7" s="20">
@@ -2275,20 +2276,20 @@
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B8" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C8" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D8" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B8" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2313,7 +2314,7 @@
       </c>
       <c r="L8" s="1" t="str">
         <f t="shared" ref="L8:L13" ca="1" si="24">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M8" s="4">
         <v>10.004348999999999</v>
@@ -2322,7 +2323,7 @@
         <v>19000</v>
       </c>
       <c r="O8" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>190082.63099999999</v>
       </c>
       <c r="P8" s="11" t="s">
@@ -2337,27 +2338,27 @@
         <v>2</v>
       </c>
       <c r="V8" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10.004349</v>
+      </c>
+      <c r="W8" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z8" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="13">
         <f t="shared" si="3"/>
-        <v>10.004349</v>
-      </c>
-      <c r="W8" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y8" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z8" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA8" s="13">
-        <f t="shared" si="7"/>
         <v>39917.35</v>
       </c>
       <c r="AB8" s="13">
@@ -2365,7 +2366,7 @@
         <v>229999.98</v>
       </c>
       <c r="AC8" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>190082.63</v>
       </c>
       <c r="AD8" s="10" t="str">
@@ -2374,7 +2375,7 @@
       </c>
       <c r="AE8" s="1"/>
       <c r="AF8" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="AG8" s="15" t="str">
@@ -2382,15 +2383,15 @@
         <v>33615420269-1</v>
       </c>
       <c r="AH8" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ8" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK8" s="1">
@@ -2403,15 +2404,15 @@
         <v>229999.98</v>
       </c>
       <c r="AN8" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>190082.63</v>
       </c>
       <c r="AO8" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AP8" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>230000</v>
       </c>
       <c r="AQ8" s="20">
@@ -2422,20 +2423,20 @@
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B9" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C9" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D9" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B9" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D9" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2460,7 +2461,7 @@
       </c>
       <c r="L9" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M9" s="4">
         <v>1.0221830000000001</v>
@@ -2469,7 +2470,7 @@
         <v>19000</v>
       </c>
       <c r="O9" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>19421.477000000003</v>
       </c>
       <c r="P9" s="11" t="s">
@@ -2484,27 +2485,27 @@
         <v>2</v>
       </c>
       <c r="V9" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.022183</v>
+      </c>
+      <c r="W9" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z9" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="13">
         <f t="shared" si="3"/>
-        <v>1.022183</v>
-      </c>
-      <c r="W9" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y9" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z9" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA9" s="13">
-        <f t="shared" si="7"/>
         <v>4078.51</v>
       </c>
       <c r="AB9" s="13">
@@ -2512,7 +2513,7 @@
         <v>23499.99</v>
       </c>
       <c r="AC9" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>19421.48</v>
       </c>
       <c r="AD9" s="10" t="str">
@@ -2521,7 +2522,7 @@
       </c>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="AG9" s="15" t="str">
@@ -2529,15 +2530,15 @@
         <v>20147130202-1</v>
       </c>
       <c r="AH9" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI9" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ9" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK9" s="1">
@@ -2550,15 +2551,15 @@
         <v>23499.99</v>
       </c>
       <c r="AN9" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>19421.48</v>
       </c>
       <c r="AO9" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AP9" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>23500</v>
       </c>
       <c r="AQ9" s="20">
@@ -2569,20 +2570,20 @@
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C10" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D10" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B10" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D10" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2607,7 +2608,7 @@
       </c>
       <c r="L10" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M10" s="4">
         <v>1.0439320000000001</v>
@@ -2616,7 +2617,7 @@
         <v>19000</v>
       </c>
       <c r="O10" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>19834.708000000002</v>
       </c>
       <c r="P10" s="11" t="s">
@@ -2631,27 +2632,27 @@
         <v>2</v>
       </c>
       <c r="V10" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.043932</v>
+      </c>
+      <c r="W10" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z10" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="13">
         <f t="shared" si="3"/>
-        <v>1.043932</v>
-      </c>
-      <c r="W10" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y10" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z10" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA10" s="13">
-        <f t="shared" si="7"/>
         <v>4165.29</v>
       </c>
       <c r="AB10" s="13">
@@ -2659,7 +2660,7 @@
         <v>24000</v>
       </c>
       <c r="AC10" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>19834.71</v>
       </c>
       <c r="AD10" s="10" t="str">
@@ -2668,7 +2669,7 @@
       </c>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="AG10" s="15" t="str">
@@ -2676,15 +2677,15 @@
         <v>20374730429-1</v>
       </c>
       <c r="AH10" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI10" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="AJ10" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK10" s="1">
@@ -2697,15 +2698,15 @@
         <v>24000</v>
       </c>
       <c r="AN10" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>19834.71</v>
       </c>
       <c r="AO10" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AP10" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>24000</v>
       </c>
       <c r="AQ10" s="20">
@@ -2716,20 +2717,20 @@
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B11" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C11" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D11" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B11" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2754,7 +2755,7 @@
       </c>
       <c r="L11" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M11" s="4">
         <v>1.3</v>
@@ -2763,7 +2764,7 @@
         <v>10000</v>
       </c>
       <c r="O11" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>13000</v>
       </c>
       <c r="P11" s="11" t="s">
@@ -2778,27 +2779,27 @@
         <v>2</v>
       </c>
       <c r="V11" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+      <c r="W11" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>10000.00</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z11" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA11" s="13">
         <f t="shared" si="3"/>
-        <v>1.3</v>
-      </c>
-      <c r="W11" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>10000.00</v>
-      </c>
-      <c r="X11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y11" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z11" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA11" s="13">
-        <f t="shared" si="7"/>
         <v>2256.1999999999998</v>
       </c>
       <c r="AB11" s="13">
@@ -2806,7 +2807,7 @@
         <v>13000</v>
       </c>
       <c r="AC11" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>13000.00</v>
       </c>
       <c r="AD11" s="10" t="str">
@@ -2815,7 +2816,7 @@
       </c>
       <c r="AE11" s="1"/>
       <c r="AF11" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="AG11" s="15" t="str">
@@ -2823,15 +2824,15 @@
         <v>37473042-1</v>
       </c>
       <c r="AH11" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AI11" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ11" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK11" s="1">
@@ -2844,15 +2845,15 @@
         <v>13000</v>
       </c>
       <c r="AN11" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>10743.8</v>
       </c>
       <c r="AO11" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.3</v>
       </c>
       <c r="AP11" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>13000</v>
       </c>
       <c r="AQ11" s="20">
@@ -2863,20 +2864,20 @@
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B12" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C12" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D12" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B12" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -2901,7 +2902,7 @@
       </c>
       <c r="L12" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M12" s="4">
         <v>1.2105263157894737</v>
@@ -2910,7 +2911,7 @@
         <v>19000</v>
       </c>
       <c r="O12" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>23000</v>
       </c>
       <c r="P12" s="11" t="s">
@@ -2925,27 +2926,27 @@
         <v>2</v>
       </c>
       <c r="V12" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.210526</v>
+      </c>
+      <c r="W12" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z12" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA12" s="13">
         <f t="shared" si="3"/>
-        <v>1.210526</v>
-      </c>
-      <c r="W12" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X12" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y12" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z12" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA12" s="13">
-        <f t="shared" si="7"/>
         <v>3991.74</v>
       </c>
       <c r="AB12" s="13">
@@ -2953,7 +2954,7 @@
         <v>23000</v>
       </c>
       <c r="AC12" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>23000.00</v>
       </c>
       <c r="AD12" s="10" t="str">
@@ -2962,7 +2963,7 @@
       </c>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="AG12" s="15" t="str">
@@ -2970,15 +2971,15 @@
         <v>30707354719-1</v>
       </c>
       <c r="AH12" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI12" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ12" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK12" s="1">
@@ -2991,15 +2992,15 @@
         <v>23000</v>
       </c>
       <c r="AN12" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>19008.259999999998</v>
       </c>
       <c r="AO12" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AP12" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>23000</v>
       </c>
       <c r="AQ12" s="20">
@@ -3010,20 +3011,20 @@
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B13" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C13" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D13" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B13" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D13" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3046,7 +3047,7 @@
       </c>
       <c r="L13" s="1" t="str">
         <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Abril</v>
+        <v>Honorarios Mayo</v>
       </c>
       <c r="M13" s="4">
         <v>1.5</v>
@@ -3055,7 +3056,7 @@
         <v>19000</v>
       </c>
       <c r="O13" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="P13" s="11"/>
@@ -3068,27 +3069,27 @@
         <v>2</v>
       </c>
       <c r="V13" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W13" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00000</v>
+      </c>
+      <c r="Y13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000000</v>
+      </c>
+      <c r="Z13" s="9">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="13">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="W13" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X13" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00000</v>
-      </c>
-      <c r="Y13" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z13" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>00/01/1900</v>
-      </c>
-      <c r="AA13" s="13">
-        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AB13" s="13">
@@ -3096,7 +3097,7 @@
         <v>28500</v>
       </c>
       <c r="AC13" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>28500.00</v>
       </c>
       <c r="AD13" s="10" t="str">
@@ -3105,7 +3106,7 @@
       </c>
       <c r="AE13" s="1"/>
       <c r="AF13" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="AG13" s="15" t="str">
@@ -3113,15 +3114,15 @@
         <v>-0</v>
       </c>
       <c r="AH13" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ13" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>C</v>
       </c>
       <c r="AK13" s="1">
@@ -3134,15 +3135,15 @@
         <v>28500</v>
       </c>
       <c r="AN13" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>28500</v>
       </c>
       <c r="AO13" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="AP13" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>28500</v>
       </c>
       <c r="AQ13" s="20">
@@ -3153,20 +3154,20 @@
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B14" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C14" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D14" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B14" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D14" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3199,7 +3200,7 @@
         <v>19000</v>
       </c>
       <c r="O14" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>133471.06700000001</v>
       </c>
       <c r="P14" s="11" t="s">
@@ -3222,27 +3223,27 @@
         <v>2</v>
       </c>
       <c r="V14" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7.024793</v>
+      </c>
+      <c r="W14" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X14" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000150</v>
+      </c>
+      <c r="Z14" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA14" s="13">
         <f t="shared" si="3"/>
-        <v>7.024793</v>
-      </c>
-      <c r="W14" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y14" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000150</v>
-      </c>
-      <c r="Z14" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA14" s="13">
-        <f t="shared" si="7"/>
         <v>28028.92</v>
       </c>
       <c r="AB14" s="13">
@@ -3250,7 +3251,7 @@
         <v>161499.99</v>
       </c>
       <c r="AC14" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>133471.07</v>
       </c>
       <c r="AD14" s="10" t="str">
@@ -3259,7 +3260,7 @@
       </c>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="AG14" s="15" t="str">
@@ -3267,15 +3268,15 @@
         <v>30684125792-1</v>
       </c>
       <c r="AH14" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ14" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK14" s="1">
@@ -3288,15 +3289,15 @@
         <v>161499.99</v>
       </c>
       <c r="AN14" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>133471.07</v>
       </c>
       <c r="AO14" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AP14" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>161500</v>
       </c>
       <c r="AQ14" s="20">
@@ -3307,20 +3308,20 @@
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B15" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C15" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D15" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B15" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D15" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3353,7 +3354,7 @@
         <v>19000</v>
       </c>
       <c r="O15" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="P15" s="11" t="s">
@@ -3376,27 +3377,27 @@
         <v>2</v>
       </c>
       <c r="V15" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W15" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X15" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000152</v>
+      </c>
+      <c r="Z15" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA15" s="13">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="W15" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y15" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000152</v>
-      </c>
-      <c r="Z15" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA15" s="13">
-        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB15" s="13">
@@ -3404,7 +3405,7 @@
         <v>28500</v>
       </c>
       <c r="AC15" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>28500.00</v>
       </c>
       <c r="AD15" s="10" t="str">
@@ -3413,7 +3414,7 @@
       </c>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="AG15" s="15" t="str">
@@ -3421,15 +3422,15 @@
         <v>30707354719-2</v>
       </c>
       <c r="AH15" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI15" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ15" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK15" s="1">
@@ -3442,15 +3443,15 @@
         <v>28500</v>
       </c>
       <c r="AN15" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>23553.72</v>
       </c>
       <c r="AO15" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="AP15" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>28500</v>
       </c>
       <c r="AQ15" s="20">
@@ -3461,20 +3462,20 @@
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B16" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C16" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D16" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B16" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D16" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3507,7 +3508,7 @@
         <v>19000</v>
       </c>
       <c r="O16" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>133057.83600000001</v>
       </c>
       <c r="P16" s="11" t="s">
@@ -3530,27 +3531,27 @@
         <v>2</v>
       </c>
       <c r="V16" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>7.003044</v>
+      </c>
+      <c r="W16" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X16" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000151</v>
+      </c>
+      <c r="Z16" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA16" s="13">
         <f t="shared" si="3"/>
-        <v>7.003044</v>
-      </c>
-      <c r="W16" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y16" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000151</v>
-      </c>
-      <c r="Z16" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA16" s="13">
-        <f t="shared" si="7"/>
         <v>27942.15</v>
       </c>
       <c r="AB16" s="13">
@@ -3558,7 +3559,7 @@
         <v>160999.99</v>
       </c>
       <c r="AC16" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>133057.84</v>
       </c>
       <c r="AD16" s="10" t="str">
@@ -3567,7 +3568,7 @@
       </c>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="AG16" s="15" t="str">
@@ -3575,15 +3576,15 @@
         <v>30684125792-2</v>
       </c>
       <c r="AH16" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ16" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>A</v>
       </c>
       <c r="AK16" s="1">
@@ -3596,15 +3597,15 @@
         <v>160999.98000000001</v>
       </c>
       <c r="AN16" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>133057.82999999999</v>
       </c>
       <c r="AO16" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>7.003044</v>
       </c>
       <c r="AP16" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>161000</v>
       </c>
       <c r="AQ16" s="20">
@@ -3615,20 +3616,20 @@
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f t="shared" ca="1" si="16"/>
-        <v>45051</v>
-      </c>
-      <c r="B17" s="9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>01/04/2023</v>
-      </c>
-      <c r="C17" s="9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>30/04/2023</v>
-      </c>
-      <c r="D17" s="9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>19/05/2023</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>45107</v>
+      </c>
+      <c r="B17" s="9">
+        <f t="shared" ca="1" si="13"/>
+        <v>45047</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" ca="1" si="14"/>
+        <v>45077</v>
+      </c>
+      <c r="D17" s="9">
+        <f t="shared" ca="1" si="15"/>
+        <v>45121</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3661,7 +3662,7 @@
         <v>19000</v>
       </c>
       <c r="O17" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>28500</v>
       </c>
       <c r="P17" s="11" t="s">
@@ -3684,27 +3685,27 @@
         <v>2</v>
       </c>
       <c r="V17" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="W17" s="18" t="str">
+        <f t="shared" si="17"/>
+        <v>19000.00</v>
+      </c>
+      <c r="X17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>00002</v>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000153</v>
+      </c>
+      <c r="Z17" s="9">
+        <f t="shared" si="18"/>
+        <v>44816</v>
+      </c>
+      <c r="AA17" s="13">
         <f t="shared" si="3"/>
-        <v>1.5</v>
-      </c>
-      <c r="W17" s="18" t="str">
-        <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>00002</v>
-      </c>
-      <c r="Y17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>00000153</v>
-      </c>
-      <c r="Z17" s="1" t="str">
-        <f t="shared" si="6"/>
-        <v>12/09/2022</v>
-      </c>
-      <c r="AA17" s="13">
-        <f t="shared" si="7"/>
         <v>4946.28</v>
       </c>
       <c r="AB17" s="13">
@@ -3712,7 +3713,7 @@
         <v>28500</v>
       </c>
       <c r="AC17" s="10" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="4"/>
         <v>28500.00</v>
       </c>
       <c r="AD17" s="10" t="str">
@@ -3721,7 +3722,7 @@
       </c>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="AG17" s="15" t="str">
@@ -3729,15 +3730,15 @@
         <v>37473042-2</v>
       </c>
       <c r="AH17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AI17" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AJ17" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>B</v>
       </c>
       <c r="AK17" s="1">
@@ -3750,15 +3751,15 @@
         <v>28500</v>
       </c>
       <c r="AN17" s="13">
-        <f t="shared" si="13"/>
+        <f t="shared" si="9"/>
         <v>23553.72</v>
       </c>
       <c r="AO17" s="20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="10"/>
         <v>1.5</v>
       </c>
       <c r="AP17" s="13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="11"/>
         <v>28500</v>
       </c>
       <c r="AQ17" s="20">

</xml_diff>

<commit_message>
Add Cod y bonif
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B821D4-C4DC-42AF-8412-DBE9F7B71DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F54E1BB-2FE6-400B-98BA-4EAA00B97F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Factura" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AP$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AU$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
   <si>
     <t>Fecha</t>
   </si>
@@ -285,6 +285,21 @@
   </si>
   <si>
     <t>AUX unidades mult</t>
+  </si>
+  <si>
+    <t>Cod</t>
+  </si>
+  <si>
+    <t>Bonif</t>
+  </si>
+  <si>
+    <t>% Bonif</t>
+  </si>
+  <si>
+    <t>% Bonif (Facturador)</t>
+  </si>
+  <si>
+    <t>Bonif Facturador</t>
   </si>
 </sst>
 </file>
@@ -825,7 +840,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -849,6 +864,7 @@
     <xf numFmtId="2" fontId="0" fillId="35" borderId="10" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1211,7 +1227,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR17"/>
+  <dimension ref="A1:AW17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
@@ -1230,29 +1246,32 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="29" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="25" width="9.140625" customWidth="1"/>
-    <col min="26" max="26" width="11" customWidth="1"/>
-    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" customWidth="1"/>
-    <col min="32" max="32" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6" customWidth="1"/>
-    <col min="35" max="35" width="5.85546875" customWidth="1"/>
-    <col min="36" max="36" width="4" customWidth="1"/>
-    <col min="37" max="37" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="25" width="8" customWidth="1"/>
+    <col min="26" max="30" width="9.140625" customWidth="1"/>
+    <col min="31" max="31" width="11" customWidth="1"/>
+    <col min="32" max="32" width="10" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" customWidth="1"/>
+    <col min="35" max="35" width="11.5703125" customWidth="1"/>
+    <col min="36" max="36" width="9.140625" customWidth="1"/>
+    <col min="37" max="37" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6" customWidth="1"/>
+    <col min="40" max="40" width="5.85546875" customWidth="1"/>
+    <col min="41" max="41" width="4" customWidth="1"/>
+    <col min="42" max="42" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1290,118 +1309,133 @@
         <v>11</v>
       </c>
       <c r="M1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AF1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AG1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AH1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AI1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AK1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AL1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="16" t="s">
+      <c r="AM1" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" s="16" t="s">
+      <c r="AN1" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" s="16" t="s">
+      <c r="AO1" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" s="16" t="s">
+      <c r="AP1" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="AL1" s="16" t="s">
+      <c r="AQ1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="17" t="s">
+      <c r="AR1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="17" t="s">
+      <c r="AS1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="17" t="s">
+      <c r="AT1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="19" t="s">
+      <c r="AU1" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="AQ1" s="19" t="s">
+      <c r="AV1" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="AR1" s="19" t="s">
+      <c r="AW1" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45107</v>
+        <v>45140</v>
       </c>
       <c r="B2" s="9">
         <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
-        <v>45047</v>
+        <v>45108</v>
       </c>
       <c r="C2" s="9">
         <f ca="1">EOMONTH(A2,-1)</f>
-        <v>45077</v>
+        <v>45138</v>
       </c>
       <c r="D2" s="9">
         <f ca="1">A2+14</f>
-        <v>45121</v>
+        <v>45154</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1427,127 +1461,138 @@
       <c r="L2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="2"/>
+      <c r="N2" s="4">
         <v>7.003044</v>
       </c>
-      <c r="N2" s="5">
+      <c r="O2" s="5">
         <v>19000</v>
       </c>
-      <c r="O2" s="5">
-        <f>M2*N2</f>
+      <c r="P2" s="5">
+        <f>N2*O2</f>
         <v>133057.83600000001</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="14">
+      <c r="T2" s="11"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="1" t="str">
+        <f>SUBSTITUTE(V2,",",".")</f>
+        <v/>
+      </c>
+      <c r="Y2" s="1" t="str">
+        <f t="shared" ref="Y2:Y17" si="0">SUBSTITUTE(W2,",",".")</f>
+        <v/>
+      </c>
+      <c r="Z2" s="14">
         <f>COUNTIFS($F$1:F2,F2,$K$1:K2,K2)+1</f>
         <v>2</v>
       </c>
-      <c r="V2" s="18" t="str">
-        <f t="shared" ref="V2:V17" si="0">SUBSTITUTE(IF(AJ2="A",ROUND(O2/N2,6),ROUND(AB2/N2,6)),",",".")</f>
+      <c r="AA2" s="18" t="str">
+        <f t="shared" ref="AA2:AA17" si="1">SUBSTITUTE(IF(AO2="A",ROUND(P2/O2,6),ROUND(AG2/O2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
-      <c r="W2" s="18" t="str">
-        <f>SUBSTITUTE(TEXT(N2,"0,00"),",",".")</f>
+      <c r="AB2" s="18" t="str">
+        <f>SUBSTITUTE(TEXT(O2,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
-      <c r="X2" s="1" t="str">
-        <f t="shared" ref="X2:X17" si="1">TEXT(R2,"00000")</f>
+      <c r="AC2" s="1" t="str">
+        <f t="shared" ref="AC2:AC17" si="2">TEXT(S2,"00000")</f>
         <v>00000</v>
       </c>
-      <c r="Y2" s="1" t="str">
-        <f t="shared" ref="Y2:Y17" si="2">TEXT(S2,"00000000")</f>
+      <c r="AD2" s="1" t="str">
+        <f t="shared" ref="AD2:AD17" si="3">TEXT(T2,"00000000")</f>
         <v>00000000</v>
       </c>
-      <c r="Z2" s="9">
-        <f>T2</f>
-        <v>0</v>
-      </c>
-      <c r="AA2" s="13">
-        <f t="shared" ref="AA2:AA17" si="3">IF(AJ2="A",ROUND(O2*P2,2),ROUND(O2*P2/(1+P2),2))</f>
+      <c r="AE2" s="9">
+        <f>U2</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="13">
+        <f t="shared" ref="AF2:AF17" si="4">IF(AO2="A",ROUND(P2*Q2,2),ROUND(P2*Q2/(1+Q2),2))</f>
         <v>27942.15</v>
       </c>
-      <c r="AB2" s="13">
-        <f>IF(AJ2="A",ROUND(O2+AA2,2),ROUND(O2,2))</f>
+      <c r="AG2" s="13">
+        <f>IF(AO2="A",ROUND(P2+AF2,2),ROUND(P2,2))</f>
         <v>160999.99</v>
       </c>
-      <c r="AC2" s="10" t="str">
-        <f t="shared" ref="AC2:AC17" si="4">IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(O2,"0,00"),",","."),SUBSTITUTE(TEXT(AB2,"0,00"),",","."))</f>
+      <c r="AH2" s="10" t="str">
+        <f>IF(RIGHT(F2,1)="A",SUBSTITUTE(TEXT(P2,"0,00"),",","."),SUBSTITUTE(TEXT(AG2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
-      <c r="AD2" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB2,0)-AB2,"0,00"),",",".")</f>
+      <c r="AI2" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG2,0)-AG2,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1">
-        <f t="shared" ref="AF2:AF17" si="5">ROW(K2)</f>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1">
+        <f>ROW(K2)</f>
         <v>2</v>
       </c>
-      <c r="AG2" s="15" t="str">
+      <c r="AL2" s="15" t="str">
         <f>J2&amp;"-"&amp;COUNTIF($J$1:J2,J2)</f>
         <v>30525390086-1</v>
       </c>
-      <c r="AH2" s="1">
-        <f t="shared" ref="AH2:AH17" si="6">IF(K1=K2,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AI2" s="1">
-        <f t="shared" ref="AI2:AI17" si="7">IF(K2=K3,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="8">RIGHT(F2)</f>
+      <c r="AM2" s="1">
+        <f>IF(K1=K2,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN2" s="1">
+        <f>IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" s="1" t="str">
+        <f>RIGHT(F2)</f>
         <v>A</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AP2" s="1">
         <f>IF(LEFT(F2,4)="Nota",0,1)</f>
         <v>1</v>
       </c>
-      <c r="AL2" s="2"/>
-      <c r="AM2" s="13">
-        <f>IF(RIGHT(F2,1)="A",ROUND(N2*M2*(1+P2),2),AB2)</f>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="13">
+        <f>IF(RIGHT(F2,1)="A",ROUND(O2*N2*(1+Q2),2),AG2)</f>
         <v>160999.98000000001</v>
       </c>
-      <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="9">ROUND((AM2/(1+P2)),2)</f>
+      <c r="AS2" s="13">
+        <f t="shared" ref="AS2:AS17" si="5">ROUND((AR2/(1+Q2)),2)</f>
         <v>133057.82999999999</v>
       </c>
-      <c r="AO2" s="20">
-        <f t="shared" ref="AO2:AO17" si="10">IF(AJ2="A",ROUND(AN2/N2,6),AM2/N2)</f>
+      <c r="AT2" s="20">
+        <f t="shared" ref="AT2:AT17" si="6">IF(AO2="A",ROUND(AS2/O2,6),AR2/O2)</f>
         <v>7.003044</v>
       </c>
-      <c r="AP2" s="13">
-        <f t="shared" ref="AP2:AP17" si="11">IF(AJ2="A",ROUND(CEILING(N2*M2*(1+P2),500),2),ROUND(CEILING(N2*M2,500),2))</f>
+      <c r="AU2" s="13">
+        <f t="shared" ref="AU2:AU17" si="7">IF(AO2="A",ROUND(CEILING(O2*N2*(1+Q2),500),2),ROUND(CEILING(O2*N2,500),2))</f>
         <v>161000</v>
       </c>
-      <c r="AQ2" s="20">
-        <f>IF(AJ2="A",ROUND(AN2/N2,6),AP2/N2)</f>
+      <c r="AV2" s="20">
+        <f>IF(AO2="A",ROUND(AS2/O2,6),AU2/O2)</f>
         <v>7.003044</v>
       </c>
-      <c r="AR2" s="2"/>
+      <c r="AW2" s="2"/>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
-        <f t="shared" ref="A3:A17" ca="1" si="12">TODAY()</f>
-        <v>45107</v>
+        <f t="shared" ref="A3:A17" ca="1" si="8">TODAY()</f>
+        <v>45140</v>
       </c>
       <c r="B3" s="9">
-        <f t="shared" ref="B3:B17" ca="1" si="13">DATE(YEAR(C3),MONTH(C3),1)</f>
-        <v>45047</v>
+        <f t="shared" ref="B3:B17" ca="1" si="9">DATE(YEAR(C3),MONTH(C3),1)</f>
+        <v>45108</v>
       </c>
       <c r="C3" s="9">
-        <f t="shared" ref="C3:C17" ca="1" si="14">EOMONTH(A3,-1)</f>
-        <v>45077</v>
+        <f t="shared" ref="C3:C17" ca="1" si="10">EOMONTH(A3,-1)</f>
+        <v>45138</v>
       </c>
       <c r="D3" s="9">
-        <f t="shared" ref="D3:D17" ca="1" si="15">A3+14</f>
-        <v>45121</v>
+        <f t="shared" ref="D3:D17" ca="1" si="11">A3+14</f>
+        <v>45154</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1572,129 +1617,140 @@
       </c>
       <c r="L3" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B3,"mmmm"))</f>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M3" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="4">
         <v>8.0252280000000003</v>
       </c>
-      <c r="N3" s="5">
+      <c r="O3" s="5">
         <v>19000</v>
       </c>
-      <c r="O3" s="5">
-        <f t="shared" ref="O3:O17" si="16">M3*N3</f>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:P17" si="12">N3*O3</f>
         <v>152479.33199999999</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="Q3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="14">
+      <c r="T3" s="11"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="1" t="str">
+        <f t="shared" ref="X3:X17" si="13">SUBSTITUTE(V3,",",".")</f>
+        <v/>
+      </c>
+      <c r="Y3" s="1" t="str">
+        <f>SUBSTITUTE(W3,",",".")</f>
+        <v/>
+      </c>
+      <c r="Z3" s="14">
         <f>COUNTIFS($F$1:F3,F3,$K$1:K3,K3)+1</f>
         <v>2</v>
       </c>
-      <c r="V3" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA3" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>8.025228</v>
       </c>
-      <c r="W3" s="18" t="str">
-        <f t="shared" ref="W3:W17" si="17">SUBSTITUTE(TEXT(N3,"0,00"),",",".")</f>
+      <c r="AB3" s="18" t="str">
+        <f t="shared" ref="AB3:AB17" si="14">SUBSTITUTE(TEXT(O3,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
-      <c r="X3" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC3" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y3" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD3" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z3" s="9">
-        <f t="shared" ref="Z3:Z17" si="18">T3</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE3" s="9">
+        <f t="shared" ref="AE3:AE17" si="15">U3</f>
+        <v>0</v>
+      </c>
+      <c r="AF3" s="13">
+        <f t="shared" si="4"/>
         <v>32020.66</v>
       </c>
-      <c r="AB3" s="13">
-        <f t="shared" ref="AB3:AB17" si="19">IF(AJ3="A",ROUND(O3+AA3,2),ROUND(O3,2))</f>
+      <c r="AG3" s="13">
+        <f t="shared" ref="AG3:AG17" si="16">IF(AO3="A",ROUND(P3+AF3,2),ROUND(P3,2))</f>
         <v>184499.99</v>
       </c>
-      <c r="AC3" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH3" s="10" t="str">
+        <f>IF(RIGHT(F3,1)="A",SUBSTITUTE(TEXT(P3,"0,00"),",","."),SUBSTITUTE(TEXT(AG3,"0,00"),",","."))</f>
         <v>152479.33</v>
       </c>
-      <c r="AD3" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB3,0)-AB3,"0,00"),",",".")</f>
+      <c r="AI3" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG3,0)-AG3,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1">
+        <f>ROW(K3)</f>
         <v>3</v>
       </c>
-      <c r="AG3" s="15" t="str">
+      <c r="AL3" s="15" t="str">
         <f>J3&amp;"-"&amp;COUNTIF($J$1:J3,J3)</f>
         <v>30525733870-1</v>
       </c>
-      <c r="AH3" s="1">
+      <c r="AM3" s="1">
+        <f>IF(K2=K3,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="1">
+        <f>IF(K3=K4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO3" s="1" t="str">
+        <f>RIGHT(F3)</f>
+        <v>A</v>
+      </c>
+      <c r="AP3" s="1">
+        <f>IF(LEFT(F3,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="13">
+        <f>IF(RIGHT(F3,1)="A",ROUND(O3*N3*(1+Q3),2),AG3)</f>
+        <v>184499.99</v>
+      </c>
+      <c r="AS3" s="13">
+        <f t="shared" si="5"/>
+        <v>152479.32999999999</v>
+      </c>
+      <c r="AT3" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI3" s="1">
+        <v>8.0252280000000003</v>
+      </c>
+      <c r="AU3" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK3" s="1">
-        <f t="shared" ref="AK3:AK17" si="20">IF(LEFT(F3,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AL3" s="2"/>
-      <c r="AM3" s="13">
-        <f t="shared" ref="AM3:AM17" si="21">IF(RIGHT(F3,1)="A",ROUND(N3*M3*(1+P3),2),AB3)</f>
-        <v>184499.99</v>
-      </c>
-      <c r="AN3" s="13">
-        <f t="shared" si="9"/>
-        <v>152479.32999999999</v>
-      </c>
-      <c r="AO3" s="20">
-        <f t="shared" si="10"/>
+        <v>184500</v>
+      </c>
+      <c r="AV3" s="20">
+        <f t="shared" ref="AV3:AV17" si="17">IF(AO3="A",ROUND(AS3/O3,6),AU3/O3)</f>
         <v>8.0252280000000003</v>
       </c>
-      <c r="AP3" s="13">
-        <f t="shared" si="11"/>
-        <v>184500</v>
-      </c>
-      <c r="AQ3" s="20">
-        <f t="shared" ref="AQ3:AQ17" si="22">IF(AJ3="A",ROUND(AN3/N3,6),AP3/N3)</f>
-        <v>8.0252280000000003</v>
-      </c>
-      <c r="AR3" s="2"/>
+      <c r="AW3" s="2"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B4" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C4" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1719,129 +1775,140 @@
       </c>
       <c r="L4" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B4,"mmmm"))</f>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M4" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="4">
         <v>10.004348999999999</v>
       </c>
-      <c r="N4" s="5">
+      <c r="O4" s="5">
         <v>19000</v>
       </c>
-      <c r="O4" s="5">
-        <f t="shared" si="16"/>
+      <c r="P4" s="5">
+        <f t="shared" si="12"/>
         <v>190082.63099999999</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="Q4" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="14">
+      <c r="T4" s="11"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y4" s="1" t="str">
+        <f t="shared" ref="Y4:Y17" si="18">SUBSTITUTE(W4,",",".")</f>
+        <v/>
+      </c>
+      <c r="Z4" s="14">
         <f>COUNTIFS($F$1:F4,F4,$K$1:K4,K4)+1</f>
         <v>2</v>
       </c>
-      <c r="V4" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA4" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>10.004349</v>
       </c>
-      <c r="W4" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB4" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X4" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC4" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y4" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD4" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z4" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA4" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE4" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="13">
+        <f t="shared" si="4"/>
         <v>39917.35</v>
       </c>
-      <c r="AB4" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG4" s="13">
+        <f t="shared" si="16"/>
         <v>229999.98</v>
       </c>
-      <c r="AC4" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH4" s="10" t="str">
+        <f>IF(RIGHT(F4,1)="A",SUBSTITUTE(TEXT(P4,"0,00"),",","."),SUBSTITUTE(TEXT(AG4,"0,00"),",","."))</f>
         <v>190082.63</v>
       </c>
-      <c r="AD4" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB4,0)-AB4,"0,00"),",",".")</f>
+      <c r="AI4" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG4,0)-AG4,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1">
+        <f>ROW(K4)</f>
         <v>4</v>
       </c>
-      <c r="AG4" s="15" t="str">
+      <c r="AL4" s="15" t="str">
         <f>J4&amp;"-"&amp;COUNTIF($J$1:J4,J4)</f>
         <v>30610252334-1</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AM4" s="1">
+        <f>IF(K3=K4,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN4" s="1">
+        <f>IF(K4=K5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO4" s="1" t="str">
+        <f>RIGHT(F4)</f>
+        <v>A</v>
+      </c>
+      <c r="AP4" s="1">
+        <f>IF(LEFT(F4,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="13">
+        <f>IF(RIGHT(F4,1)="A",ROUND(O4*N4*(1+Q4),2),AG4)</f>
+        <v>229999.98</v>
+      </c>
+      <c r="AS4" s="13">
+        <f t="shared" si="5"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AT4" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI4" s="1">
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AU4" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK4" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL4" s="2"/>
-      <c r="AM4" s="13">
-        <f t="shared" si="21"/>
-        <v>229999.98</v>
-      </c>
-      <c r="AN4" s="13">
-        <f t="shared" si="9"/>
-        <v>190082.63</v>
-      </c>
-      <c r="AO4" s="20">
-        <f t="shared" si="10"/>
+        <v>230000</v>
+      </c>
+      <c r="AV4" s="20">
+        <f t="shared" si="17"/>
         <v>10.004348999999999</v>
       </c>
-      <c r="AP4" s="13">
-        <f t="shared" si="11"/>
-        <v>230000</v>
-      </c>
-      <c r="AQ4" s="20">
-        <f t="shared" si="22"/>
-        <v>10.004348999999999</v>
-      </c>
-      <c r="AR4" s="2"/>
+      <c r="AW4" s="2"/>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B5" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C5" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D5" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -1866,129 +1933,140 @@
       </c>
       <c r="L5" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B5,"mmmm"))</f>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M5" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="4">
         <v>9.0256629999999998</v>
       </c>
-      <c r="N5" s="5">
+      <c r="O5" s="5">
         <v>19000</v>
       </c>
-      <c r="O5" s="5">
-        <f t="shared" si="16"/>
+      <c r="P5" s="5">
+        <f t="shared" si="12"/>
         <v>171487.59700000001</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="Q5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
       <c r="S5" s="11"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="14">
+      <c r="T5" s="11"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z5" s="14">
         <f>COUNTIFS($F$1:F5,F5,$K$1:K5,K5)+1</f>
         <v>2</v>
       </c>
-      <c r="V5" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA5" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>9.025663</v>
       </c>
-      <c r="W5" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB5" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X5" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC5" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y5" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD5" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z5" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE5" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="13">
+        <f t="shared" si="4"/>
         <v>36012.400000000001</v>
       </c>
-      <c r="AB5" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG5" s="13">
+        <f t="shared" si="16"/>
         <v>207500</v>
       </c>
-      <c r="AC5" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH5" s="10" t="str">
+        <f>IF(RIGHT(F5,1)="A",SUBSTITUTE(TEXT(P5,"0,00"),",","."),SUBSTITUTE(TEXT(AG5,"0,00"),",","."))</f>
         <v>171487.60</v>
       </c>
-      <c r="AD5" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB5,0)-AB5,"0,00"),",",".")</f>
+      <c r="AI5" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG5,0)-AG5,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1">
+        <f>ROW(K5)</f>
         <v>5</v>
       </c>
-      <c r="AG5" s="15" t="str">
+      <c r="AL5" s="15" t="str">
         <f>J5&amp;"-"&amp;COUNTIF($J$1:J5,J5)</f>
         <v>30710964277-1</v>
       </c>
-      <c r="AH5" s="1">
+      <c r="AM5" s="1">
+        <f>IF(K4=K5,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN5" s="1">
+        <f>IF(K5=K6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO5" s="1" t="str">
+        <f>RIGHT(F5)</f>
+        <v>A</v>
+      </c>
+      <c r="AP5" s="1">
+        <f>IF(LEFT(F5,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="13">
+        <f>IF(RIGHT(F5,1)="A",ROUND(O5*N5*(1+Q5),2),AG5)</f>
+        <v>207499.99</v>
+      </c>
+      <c r="AS5" s="13">
+        <f t="shared" si="5"/>
+        <v>171487.6</v>
+      </c>
+      <c r="AT5" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI5" s="1">
+        <v>9.0256629999999998</v>
+      </c>
+      <c r="AU5" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK5" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL5" s="2"/>
-      <c r="AM5" s="13">
-        <f t="shared" si="21"/>
-        <v>207499.99</v>
-      </c>
-      <c r="AN5" s="13">
-        <f t="shared" si="9"/>
-        <v>171487.6</v>
-      </c>
-      <c r="AO5" s="20">
-        <f t="shared" si="10"/>
+        <v>207500</v>
+      </c>
+      <c r="AV5" s="20">
+        <f t="shared" si="17"/>
         <v>9.0256629999999998</v>
       </c>
-      <c r="AP5" s="13">
-        <f t="shared" si="11"/>
-        <v>207500</v>
-      </c>
-      <c r="AQ5" s="20">
-        <f t="shared" si="22"/>
-        <v>9.0256629999999998</v>
-      </c>
-      <c r="AR5" s="2"/>
+      <c r="AW5" s="2"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B6" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C6" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D6" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2013,137 +2091,148 @@
       </c>
       <c r="L6" s="1" t="str">
         <f ca="1">"Honorarios "&amp;PROPER(TEXT(B6,"mmmm"))</f>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M6" s="4">
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="4">
         <v>5.0239229999999999</v>
       </c>
-      <c r="N6" s="5">
+      <c r="O6" s="5">
         <v>19000</v>
       </c>
-      <c r="O6" s="5">
-        <f t="shared" si="16"/>
+      <c r="P6" s="5">
+        <f t="shared" si="12"/>
         <v>95454.536999999997</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="Q6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R6" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="S6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="T6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="T6" s="12">
+      <c r="U6" s="12">
         <v>44816</v>
       </c>
-      <c r="U6" s="14">
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y6" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z6" s="14">
         <f>COUNTIFS($F$1:F6,F6,$K$1:K6,K6)+1</f>
         <v>2</v>
       </c>
-      <c r="V6" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA6" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>5.023923</v>
       </c>
-      <c r="W6" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB6" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X6" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC6" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00002</v>
       </c>
-      <c r="Y6" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD6" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000003</v>
       </c>
-      <c r="Z6" s="9">
-        <f t="shared" si="18"/>
+      <c r="AE6" s="9">
+        <f t="shared" si="15"/>
         <v>44816</v>
       </c>
-      <c r="AA6" s="13">
-        <f t="shared" si="3"/>
+      <c r="AF6" s="13">
+        <f t="shared" si="4"/>
         <v>20045.45</v>
       </c>
-      <c r="AB6" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG6" s="13">
+        <f t="shared" si="16"/>
         <v>115499.99</v>
       </c>
-      <c r="AC6" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH6" s="10" t="str">
+        <f>IF(RIGHT(F6,1)="A",SUBSTITUTE(TEXT(P6,"0,00"),",","."),SUBSTITUTE(TEXT(AG6,"0,00"),",","."))</f>
         <v>95454.54</v>
       </c>
-      <c r="AD6" s="10" t="str">
-        <f>SUBSTITUTE(TEXT(ROUNDUP(AB6,0)-AB6,"0,00"),",",".")</f>
+      <c r="AI6" s="10" t="str">
+        <f>SUBSTITUTE(TEXT(ROUNDUP(AG6,0)-AG6,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1">
+        <f>ROW(K6)</f>
         <v>6</v>
       </c>
-      <c r="AG6" s="15" t="str">
+      <c r="AL6" s="15" t="str">
         <f>J6&amp;"-"&amp;COUNTIF($J$1:J6,J6)</f>
         <v>33610006189-1</v>
       </c>
-      <c r="AH6" s="1">
+      <c r="AM6" s="1">
+        <f>IF(K5=K6,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="1">
+        <f>IF(K6=K7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO6" s="1" t="str">
+        <f>RIGHT(F6)</f>
+        <v>A</v>
+      </c>
+      <c r="AP6" s="1">
+        <f>IF(LEFT(F6,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="13">
+        <f>IF(RIGHT(F6,1)="A",ROUND(O6*N6*(1+Q6),2),AG6)</f>
+        <v>115499.99</v>
+      </c>
+      <c r="AS6" s="13">
+        <f t="shared" si="5"/>
+        <v>95454.54</v>
+      </c>
+      <c r="AT6" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI6" s="1">
+        <v>5.0239229999999999</v>
+      </c>
+      <c r="AU6" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK6" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL6" s="2"/>
-      <c r="AM6" s="13">
-        <f t="shared" si="21"/>
-        <v>115499.99</v>
-      </c>
-      <c r="AN6" s="13">
-        <f t="shared" si="9"/>
-        <v>95454.54</v>
-      </c>
-      <c r="AO6" s="20">
-        <f t="shared" si="10"/>
+        <v>115500</v>
+      </c>
+      <c r="AV6" s="20">
+        <f t="shared" si="17"/>
         <v>5.0239229999999999</v>
       </c>
-      <c r="AP6" s="13">
-        <f t="shared" si="11"/>
-        <v>115500</v>
-      </c>
-      <c r="AQ6" s="20">
-        <f t="shared" si="22"/>
-        <v>5.0239229999999999</v>
-      </c>
-      <c r="AR6" s="2"/>
+      <c r="AW6" s="2"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B7" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C7" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D7" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2169,127 +2258,138 @@
       <c r="L7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="2"/>
+      <c r="N7" s="4">
         <v>5.0021740000000001</v>
       </c>
-      <c r="N7" s="5">
+      <c r="O7" s="5">
         <v>19000</v>
       </c>
-      <c r="O7" s="5">
-        <f t="shared" si="16"/>
+      <c r="P7" s="5">
+        <f t="shared" si="12"/>
         <v>95041.305999999997</v>
       </c>
-      <c r="P7" s="11" t="s">
+      <c r="Q7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q7" s="11"/>
       <c r="R7" s="11"/>
       <c r="S7" s="11"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="14">
+      <c r="T7" s="11"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z7" s="14">
         <f>COUNTIFS($F$1:F7,F7,$K$1:K7,K7)+1</f>
         <v>3</v>
       </c>
-      <c r="V7" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA7" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>5.002174</v>
       </c>
-      <c r="W7" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB7" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X7" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC7" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y7" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD7" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z7" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE7" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="13">
+        <f t="shared" si="4"/>
         <v>19958.669999999998</v>
       </c>
-      <c r="AB7" s="13">
-        <f t="shared" si="19"/>
+      <c r="AG7" s="13">
+        <f t="shared" si="16"/>
         <v>114999.98</v>
       </c>
-      <c r="AC7" s="10" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH7" s="10" t="str">
+        <f>IF(RIGHT(F7,1)="A",SUBSTITUTE(TEXT(P7,"0,00"),",","."),SUBSTITUTE(TEXT(AG7,"0,00"),",","."))</f>
         <v>95041.31</v>
       </c>
-      <c r="AD7" s="10" t="str">
-        <f t="shared" ref="AD7:AD17" si="23">SUBSTITUTE(TEXT(ROUNDUP(AB7,0)-AB7,"0,00"),",",".")</f>
+      <c r="AI7" s="10" t="str">
+        <f t="shared" ref="AI7:AI17" si="19">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1">
+        <f>ROW(K7)</f>
         <v>7</v>
       </c>
-      <c r="AG7" s="15" t="str">
+      <c r="AL7" s="15" t="str">
         <f>J7&amp;"-"&amp;COUNTIF($J$1:J7,J7)</f>
         <v>33610006189-2</v>
       </c>
-      <c r="AH7" s="1">
+      <c r="AM7" s="1">
+        <f>IF(K6=K7,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN7" s="1">
+        <f>IF(K7=K8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO7" s="1" t="str">
+        <f>RIGHT(F7)</f>
+        <v>A</v>
+      </c>
+      <c r="AP7" s="1">
+        <f>IF(LEFT(F7,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="13">
+        <f>IF(RIGHT(F7,1)="A",ROUND(O7*N7*(1+Q7),2),AG7)</f>
+        <v>114999.98</v>
+      </c>
+      <c r="AS7" s="13">
+        <f t="shared" si="5"/>
+        <v>95041.31</v>
+      </c>
+      <c r="AT7" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AI7" s="1">
+        <v>5.0021740000000001</v>
+      </c>
+      <c r="AU7" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK7" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL7" s="2"/>
-      <c r="AM7" s="13">
-        <f t="shared" si="21"/>
-        <v>114999.98</v>
-      </c>
-      <c r="AN7" s="13">
-        <f t="shared" si="9"/>
-        <v>95041.31</v>
-      </c>
-      <c r="AO7" s="20">
-        <f t="shared" si="10"/>
+        <v>115000</v>
+      </c>
+      <c r="AV7" s="20">
+        <f t="shared" si="17"/>
         <v>5.0021740000000001</v>
       </c>
-      <c r="AP7" s="13">
-        <f t="shared" si="11"/>
-        <v>115000</v>
-      </c>
-      <c r="AQ7" s="20">
-        <f t="shared" si="22"/>
-        <v>5.0021740000000001</v>
-      </c>
-      <c r="AR7" s="2"/>
+      <c r="AW7" s="2"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B8" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C8" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D8" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2313,130 +2413,141 @@
         <v>52</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f t="shared" ref="L8:L13" ca="1" si="24">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M8" s="4">
+        <f t="shared" ref="L8:L13" ca="1" si="20">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="4">
         <v>10.004348999999999</v>
       </c>
-      <c r="N8" s="5">
+      <c r="O8" s="5">
         <v>19000</v>
       </c>
-      <c r="O8" s="5">
-        <f t="shared" si="16"/>
+      <c r="P8" s="5">
+        <f t="shared" si="12"/>
         <v>190082.63099999999</v>
       </c>
-      <c r="P8" s="11" t="s">
+      <c r="Q8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q8" s="11"/>
       <c r="R8" s="11"/>
       <c r="S8" s="11"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="14">
+      <c r="T8" s="11"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y8" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z8" s="14">
         <f>COUNTIFS($F$1:F8,F8,$K$1:K8,K8)+1</f>
         <v>2</v>
       </c>
-      <c r="V8" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA8" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>10.004349</v>
       </c>
-      <c r="W8" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB8" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X8" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC8" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y8" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD8" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z8" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE8" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="13">
+        <f t="shared" si="4"/>
         <v>39917.35</v>
       </c>
-      <c r="AB8" s="13">
+      <c r="AG8" s="13">
+        <f t="shared" si="16"/>
+        <v>229999.98</v>
+      </c>
+      <c r="AH8" s="10" t="str">
+        <f>IF(RIGHT(F8,1)="A",SUBSTITUTE(TEXT(P8,"0,00"),",","."),SUBSTITUTE(TEXT(AG8,"0,00"),",","."))</f>
+        <v>190082.63</v>
+      </c>
+      <c r="AI8" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>229999.98</v>
-      </c>
-      <c r="AC8" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>190082.63</v>
-      </c>
-      <c r="AD8" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.02</v>
       </c>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1">
+        <f>ROW(K8)</f>
         <v>8</v>
       </c>
-      <c r="AG8" s="15" t="str">
+      <c r="AL8" s="15" t="str">
         <f>J8&amp;"-"&amp;COUNTIF($J$1:J8,J8)</f>
         <v>33615420269-1</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AM8" s="1">
+        <f>IF(K7=K8,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN8" s="1">
+        <f>IF(K8=K9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO8" s="1" t="str">
+        <f>RIGHT(F8)</f>
+        <v>A</v>
+      </c>
+      <c r="AP8" s="1">
+        <f>IF(LEFT(F8,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="13">
+        <f>IF(RIGHT(F8,1)="A",ROUND(O8*N8*(1+Q8),2),AG8)</f>
+        <v>229999.98</v>
+      </c>
+      <c r="AS8" s="13">
+        <f t="shared" si="5"/>
+        <v>190082.63</v>
+      </c>
+      <c r="AT8" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI8" s="1">
+        <v>10.004348999999999</v>
+      </c>
+      <c r="AU8" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK8" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL8" s="2"/>
-      <c r="AM8" s="13">
-        <f t="shared" si="21"/>
-        <v>229999.98</v>
-      </c>
-      <c r="AN8" s="13">
-        <f t="shared" si="9"/>
-        <v>190082.63</v>
-      </c>
-      <c r="AO8" s="20">
-        <f t="shared" si="10"/>
+        <v>230000</v>
+      </c>
+      <c r="AV8" s="20">
+        <f t="shared" si="17"/>
         <v>10.004348999999999</v>
       </c>
-      <c r="AP8" s="13">
-        <f t="shared" si="11"/>
-        <v>230000</v>
-      </c>
-      <c r="AQ8" s="20">
-        <f t="shared" si="22"/>
-        <v>10.004348999999999</v>
-      </c>
-      <c r="AR8" s="2"/>
+      <c r="AW8" s="2"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B9" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C9" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D9" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2460,130 +2571,141 @@
         <v>57</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M9" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="4">
         <v>1.0221830000000001</v>
       </c>
-      <c r="N9" s="5">
+      <c r="O9" s="5">
         <v>19000</v>
       </c>
-      <c r="O9" s="5">
-        <f t="shared" si="16"/>
+      <c r="P9" s="5">
+        <f t="shared" si="12"/>
         <v>19421.477000000003</v>
       </c>
-      <c r="P9" s="11" t="s">
+      <c r="Q9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q9" s="11"/>
       <c r="R9" s="11"/>
       <c r="S9" s="11"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="14">
+      <c r="T9" s="11"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y9" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z9" s="14">
         <f>COUNTIFS($F$1:F9,F9,$K$1:K9,K9)+1</f>
         <v>2</v>
       </c>
-      <c r="V9" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA9" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>1.022183</v>
       </c>
-      <c r="W9" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB9" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X9" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC9" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y9" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD9" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z9" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA9" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE9" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="13">
+        <f t="shared" si="4"/>
         <v>4078.51</v>
       </c>
-      <c r="AB9" s="13">
+      <c r="AG9" s="13">
+        <f t="shared" si="16"/>
+        <v>23499.99</v>
+      </c>
+      <c r="AH9" s="10" t="str">
+        <f>IF(RIGHT(F9,1)="A",SUBSTITUTE(TEXT(P9,"0,00"),",","."),SUBSTITUTE(TEXT(AG9,"0,00"),",","."))</f>
+        <v>19421.48</v>
+      </c>
+      <c r="AI9" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>23499.99</v>
-      </c>
-      <c r="AC9" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>19421.48</v>
-      </c>
-      <c r="AD9" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1">
+        <f>ROW(K9)</f>
         <v>9</v>
       </c>
-      <c r="AG9" s="15" t="str">
+      <c r="AL9" s="15" t="str">
         <f>J9&amp;"-"&amp;COUNTIF($J$1:J9,J9)</f>
         <v>20147130202-1</v>
       </c>
-      <c r="AH9" s="1">
+      <c r="AM9" s="1">
+        <f>IF(K8=K9,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN9" s="1">
+        <f>IF(K9=K10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO9" s="1" t="str">
+        <f>RIGHT(F9)</f>
+        <v>A</v>
+      </c>
+      <c r="AP9" s="1">
+        <f>IF(LEFT(F9,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="13">
+        <f>IF(RIGHT(F9,1)="A",ROUND(O9*N9*(1+Q9),2),AG9)</f>
+        <v>23499.99</v>
+      </c>
+      <c r="AS9" s="13">
+        <f t="shared" si="5"/>
+        <v>19421.48</v>
+      </c>
+      <c r="AT9" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI9" s="1">
+        <v>1.0221830000000001</v>
+      </c>
+      <c r="AU9" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK9" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL9" s="2"/>
-      <c r="AM9" s="13">
-        <f t="shared" si="21"/>
-        <v>23499.99</v>
-      </c>
-      <c r="AN9" s="13">
-        <f t="shared" si="9"/>
-        <v>19421.48</v>
-      </c>
-      <c r="AO9" s="20">
-        <f t="shared" si="10"/>
+        <v>23500</v>
+      </c>
+      <c r="AV9" s="20">
+        <f t="shared" si="17"/>
         <v>1.0221830000000001</v>
       </c>
-      <c r="AP9" s="13">
-        <f t="shared" si="11"/>
-        <v>23500</v>
-      </c>
-      <c r="AQ9" s="20">
-        <f t="shared" si="22"/>
-        <v>1.0221830000000001</v>
-      </c>
-      <c r="AR9" s="2"/>
+      <c r="AW9" s="2"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B10" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C10" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D10" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2607,130 +2729,141 @@
         <v>56</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M10" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="4">
         <v>1.0439320000000001</v>
       </c>
-      <c r="N10" s="5">
+      <c r="O10" s="5">
         <v>19000</v>
       </c>
-      <c r="O10" s="5">
-        <f t="shared" si="16"/>
+      <c r="P10" s="5">
+        <f t="shared" si="12"/>
         <v>19834.708000000002</v>
       </c>
-      <c r="P10" s="11" t="s">
+      <c r="Q10" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q10" s="11"/>
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="14">
+      <c r="T10" s="11"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y10" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z10" s="14">
         <f>COUNTIFS($F$1:F10,F10,$K$1:K10,K10)+1</f>
         <v>2</v>
       </c>
-      <c r="V10" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA10" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>1.043932</v>
       </c>
-      <c r="W10" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB10" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X10" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC10" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y10" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD10" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z10" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA10" s="13">
-        <f t="shared" si="3"/>
+      <c r="AE10" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="13">
+        <f t="shared" si="4"/>
         <v>4165.29</v>
       </c>
-      <c r="AB10" s="13">
+      <c r="AG10" s="13">
+        <f t="shared" si="16"/>
+        <v>24000</v>
+      </c>
+      <c r="AH10" s="10" t="str">
+        <f>IF(RIGHT(F10,1)="A",SUBSTITUTE(TEXT(P10,"0,00"),",","."),SUBSTITUTE(TEXT(AG10,"0,00"),",","."))</f>
+        <v>19834.71</v>
+      </c>
+      <c r="AI10" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>24000</v>
-      </c>
-      <c r="AC10" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>19834.71</v>
-      </c>
-      <c r="AD10" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1">
+        <f>ROW(K10)</f>
         <v>10</v>
       </c>
-      <c r="AG10" s="15" t="str">
+      <c r="AL10" s="15" t="str">
         <f>J10&amp;"-"&amp;COUNTIF($J$1:J10,J10)</f>
         <v>20374730429-1</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AM10" s="1">
+        <f>IF(K9=K10,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN10" s="1">
+        <f>IF(K10=K11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AO10" s="1" t="str">
+        <f>RIGHT(F10)</f>
+        <v>A</v>
+      </c>
+      <c r="AP10" s="1">
+        <f>IF(LEFT(F10,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="13">
+        <f>IF(RIGHT(F10,1)="A",ROUND(O10*N10*(1+Q10),2),AG10)</f>
+        <v>24000</v>
+      </c>
+      <c r="AS10" s="13">
+        <f t="shared" si="5"/>
+        <v>19834.71</v>
+      </c>
+      <c r="AT10" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI10" s="1">
+        <v>1.0439320000000001</v>
+      </c>
+      <c r="AU10" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AJ10" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK10" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL10" s="2"/>
-      <c r="AM10" s="13">
-        <f t="shared" si="21"/>
         <v>24000</v>
       </c>
-      <c r="AN10" s="13">
-        <f t="shared" si="9"/>
-        <v>19834.71</v>
-      </c>
-      <c r="AO10" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV10" s="20">
+        <f t="shared" si="17"/>
         <v>1.0439320000000001</v>
       </c>
-      <c r="AP10" s="13">
-        <f t="shared" si="11"/>
-        <v>24000</v>
-      </c>
-      <c r="AQ10" s="20">
-        <f t="shared" si="22"/>
-        <v>1.0439320000000001</v>
-      </c>
-      <c r="AR10" s="2"/>
+      <c r="AW10" s="2"/>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B11" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C11" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D11" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2754,130 +2887,141 @@
         <v>56</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M11" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="4">
         <v>1.3</v>
       </c>
-      <c r="N11" s="5">
+      <c r="O11" s="5">
         <v>10000</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="5">
+        <f t="shared" si="12"/>
+        <v>13000</v>
+      </c>
+      <c r="Q11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y11" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z11" s="14">
+        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA11" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.3</v>
+      </c>
+      <c r="AB11" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>10000.00</v>
+      </c>
+      <c r="AC11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000</v>
+      </c>
+      <c r="AD11" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000</v>
+      </c>
+      <c r="AE11" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF11" s="13">
+        <f t="shared" si="4"/>
+        <v>2256.1999999999998</v>
+      </c>
+      <c r="AG11" s="13">
         <f t="shared" si="16"/>
         <v>13000</v>
       </c>
-      <c r="P11" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="14">
-        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V11" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3</v>
-      </c>
-      <c r="W11" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>10000.00</v>
-      </c>
-      <c r="X11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00000</v>
-      </c>
-      <c r="Y11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z11" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="13">
-        <f t="shared" si="3"/>
-        <v>2256.1999999999998</v>
-      </c>
-      <c r="AB11" s="13">
+      <c r="AH11" s="10" t="str">
+        <f>IF(RIGHT(F11,1)="A",SUBSTITUTE(TEXT(P11,"0,00"),",","."),SUBSTITUTE(TEXT(AG11,"0,00"),",","."))</f>
+        <v>13000.00</v>
+      </c>
+      <c r="AI11" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>13000</v>
-      </c>
-      <c r="AC11" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>13000.00</v>
-      </c>
-      <c r="AD11" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1">
+        <f>ROW(K11)</f>
         <v>11</v>
       </c>
-      <c r="AG11" s="15" t="str">
+      <c r="AL11" s="15" t="str">
         <f>J11&amp;"-"&amp;COUNTIF($J$1:J11,J11)</f>
         <v>37473042-1</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AM11" s="1">
+        <f>IF(K10=K11,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AN11" s="1">
+        <f>IF(K11=K12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="1" t="str">
+        <f>RIGHT(F11)</f>
+        <v>B</v>
+      </c>
+      <c r="AP11" s="1">
+        <f>IF(LEFT(F11,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="13">
+        <f>IF(RIGHT(F11,1)="A",ROUND(O11*N11*(1+Q11),2),AG11)</f>
+        <v>13000</v>
+      </c>
+      <c r="AS11" s="13">
+        <f t="shared" si="5"/>
+        <v>10743.8</v>
+      </c>
+      <c r="AT11" s="20">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AI11" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="AU11" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK11" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL11" s="2"/>
-      <c r="AM11" s="13">
-        <f t="shared" si="21"/>
         <v>13000</v>
       </c>
-      <c r="AN11" s="13">
-        <f t="shared" si="9"/>
-        <v>10743.8</v>
-      </c>
-      <c r="AO11" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV11" s="20">
+        <f t="shared" si="17"/>
         <v>1.3</v>
       </c>
-      <c r="AP11" s="13">
-        <f t="shared" si="11"/>
-        <v>13000</v>
-      </c>
-      <c r="AQ11" s="20">
-        <f t="shared" si="22"/>
-        <v>1.3</v>
-      </c>
-      <c r="AR11" s="2"/>
+      <c r="AW11" s="2"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B12" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C12" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D12" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -2901,130 +3045,141 @@
         <v>60</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M12" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="4">
         <v>1.2105263157894737</v>
       </c>
-      <c r="N12" s="5">
+      <c r="O12" s="5">
         <v>19000</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
+        <f t="shared" si="12"/>
+        <v>23000</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y12" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z12" s="14">
+        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA12" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.210526</v>
+      </c>
+      <c r="AB12" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AC12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00000</v>
+      </c>
+      <c r="AD12" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000000</v>
+      </c>
+      <c r="AE12" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF12" s="13">
+        <f t="shared" si="4"/>
+        <v>3991.74</v>
+      </c>
+      <c r="AG12" s="13">
         <f t="shared" si="16"/>
         <v>23000</v>
       </c>
-      <c r="P12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="12"/>
-      <c r="U12" s="14">
-        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V12" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.210526</v>
-      </c>
-      <c r="W12" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00000</v>
-      </c>
-      <c r="Y12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000000</v>
-      </c>
-      <c r="Z12" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA12" s="13">
-        <f t="shared" si="3"/>
-        <v>3991.74</v>
-      </c>
-      <c r="AB12" s="13">
+      <c r="AH12" s="10" t="str">
+        <f>IF(RIGHT(F12,1)="A",SUBSTITUTE(TEXT(P12,"0,00"),",","."),SUBSTITUTE(TEXT(AG12,"0,00"),",","."))</f>
+        <v>23000.00</v>
+      </c>
+      <c r="AI12" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>23000</v>
-      </c>
-      <c r="AC12" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>23000.00</v>
-      </c>
-      <c r="AD12" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1">
+        <f>ROW(K12)</f>
         <v>12</v>
       </c>
-      <c r="AG12" s="15" t="str">
+      <c r="AL12" s="15" t="str">
         <f>J12&amp;"-"&amp;COUNTIF($J$1:J12,J12)</f>
         <v>30707354719-1</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AM12" s="1">
+        <f>IF(K11=K12,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN12" s="1">
+        <f>IF(K12=K13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO12" s="1" t="str">
+        <f>RIGHT(F12)</f>
+        <v>B</v>
+      </c>
+      <c r="AP12" s="1">
+        <f>IF(LEFT(F12,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="13">
+        <f>IF(RIGHT(F12,1)="A",ROUND(O12*N12*(1+Q12),2),AG12)</f>
+        <v>23000</v>
+      </c>
+      <c r="AS12" s="13">
+        <f t="shared" si="5"/>
+        <v>19008.259999999998</v>
+      </c>
+      <c r="AT12" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI12" s="1">
+        <v>1.2105263157894737</v>
+      </c>
+      <c r="AU12" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK12" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL12" s="2"/>
-      <c r="AM12" s="13">
-        <f t="shared" si="21"/>
         <v>23000</v>
       </c>
-      <c r="AN12" s="13">
-        <f t="shared" si="9"/>
-        <v>19008.259999999998</v>
-      </c>
-      <c r="AO12" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV12" s="20">
+        <f t="shared" si="17"/>
         <v>1.2105263157894737</v>
       </c>
-      <c r="AP12" s="13">
-        <f t="shared" si="11"/>
-        <v>23000</v>
-      </c>
-      <c r="AQ12" s="20">
-        <f t="shared" si="22"/>
-        <v>1.2105263157894737</v>
-      </c>
-      <c r="AR12" s="2"/>
+      <c r="AW12" s="2"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B13" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C13" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D13" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3046,128 +3201,139 @@
         <v>70</v>
       </c>
       <c r="L13" s="1" t="str">
-        <f t="shared" ca="1" si="24"/>
-        <v>Honorarios Mayo</v>
-      </c>
-      <c r="M13" s="4">
+        <f t="shared" ca="1" si="20"/>
+        <v>Honorarios Julio</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="4">
         <v>1.5</v>
       </c>
-      <c r="N13" s="5">
+      <c r="O13" s="5">
         <v>19000</v>
       </c>
-      <c r="O13" s="5">
-        <f t="shared" si="16"/>
+      <c r="P13" s="5">
+        <f t="shared" si="12"/>
         <v>28500</v>
       </c>
-      <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
       <c r="S13" s="11"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="14">
+      <c r="T13" s="11"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y13" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z13" s="14">
         <f>COUNTIFS($F$1:F13,F13,$K$1:K13,K13)+1</f>
         <v>2</v>
       </c>
-      <c r="V13" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA13" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="W13" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB13" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X13" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC13" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00000</v>
       </c>
-      <c r="Y13" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD13" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000000</v>
       </c>
-      <c r="Z13" s="9">
-        <f t="shared" si="18"/>
-        <v>0</v>
-      </c>
-      <c r="AA13" s="13">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AB13" s="13">
+      <c r="AE13" s="9">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AF13" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="13">
+        <f t="shared" si="16"/>
+        <v>28500</v>
+      </c>
+      <c r="AH13" s="10" t="str">
+        <f>IF(RIGHT(F13,1)="A",SUBSTITUTE(TEXT(P13,"0,00"),",","."),SUBSTITUTE(TEXT(AG13,"0,00"),",","."))</f>
+        <v>28500.00</v>
+      </c>
+      <c r="AI13" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>28500</v>
-      </c>
-      <c r="AC13" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>28500.00</v>
-      </c>
-      <c r="AD13" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1">
+        <f>ROW(K13)</f>
         <v>13</v>
       </c>
-      <c r="AG13" s="15" t="str">
+      <c r="AL13" s="15" t="str">
         <f>J13&amp;"-"&amp;COUNTIF($J$1:J13,J13)</f>
         <v>-0</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AM13" s="1">
+        <f>IF(K12=K13,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN13" s="1">
+        <f>IF(K13=K14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO13" s="1" t="str">
+        <f>RIGHT(F13)</f>
+        <v>C</v>
+      </c>
+      <c r="AP13" s="1">
+        <f>IF(LEFT(F13,4)="Nota",0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="13">
+        <f>IF(RIGHT(F13,1)="A",ROUND(O13*N13*(1+Q13),2),AG13)</f>
+        <v>28500</v>
+      </c>
+      <c r="AS13" s="13">
+        <f t="shared" si="5"/>
+        <v>28500</v>
+      </c>
+      <c r="AT13" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI13" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AU13" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>C</v>
-      </c>
-      <c r="AK13" s="1">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="AL13" s="2"/>
-      <c r="AM13" s="13">
-        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
-      <c r="AN13" s="13">
-        <f t="shared" si="9"/>
-        <v>28500</v>
-      </c>
-      <c r="AO13" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV13" s="20">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
-      <c r="AP13" s="13">
-        <f t="shared" si="11"/>
-        <v>28500</v>
-      </c>
-      <c r="AQ13" s="20">
-        <f t="shared" si="22"/>
-        <v>1.5</v>
-      </c>
-      <c r="AR13" s="2"/>
+      <c r="AW13" s="2"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B14" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C14" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D14" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3193,135 +3359,146 @@
       <c r="L14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="2"/>
+      <c r="N14" s="4">
         <v>7.0247929999999998</v>
       </c>
-      <c r="N14" s="5">
+      <c r="O14" s="5">
         <v>19000</v>
       </c>
-      <c r="O14" s="5">
-        <f t="shared" si="16"/>
+      <c r="P14" s="5">
+        <f t="shared" si="12"/>
         <v>133471.06700000001</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="Q14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="11" t="s">
+      <c r="R14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="R14" s="11" t="s">
+      <c r="S14" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="11" t="s">
+      <c r="T14" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T14" s="12">
+      <c r="U14" s="12">
         <v>44816</v>
       </c>
-      <c r="U14" s="14">
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y14" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z14" s="14">
         <f>COUNTIFS($F$1:F14,F14,$K$1:K14,K14)+1</f>
         <v>2</v>
       </c>
-      <c r="V14" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA14" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>7.024793</v>
       </c>
-      <c r="W14" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB14" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X14" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC14" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00002</v>
       </c>
-      <c r="Y14" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD14" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000150</v>
       </c>
-      <c r="Z14" s="9">
-        <f t="shared" si="18"/>
+      <c r="AE14" s="9">
+        <f t="shared" si="15"/>
         <v>44816</v>
       </c>
-      <c r="AA14" s="13">
-        <f t="shared" si="3"/>
+      <c r="AF14" s="13">
+        <f t="shared" si="4"/>
         <v>28028.92</v>
       </c>
-      <c r="AB14" s="13">
+      <c r="AG14" s="13">
+        <f t="shared" si="16"/>
+        <v>161499.99</v>
+      </c>
+      <c r="AH14" s="10" t="str">
+        <f>IF(RIGHT(F14,1)="A",SUBSTITUTE(TEXT(P14,"0,00"),",","."),SUBSTITUTE(TEXT(AG14,"0,00"),",","."))</f>
+        <v>133471.07</v>
+      </c>
+      <c r="AI14" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>161499.99</v>
-      </c>
-      <c r="AC14" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>133471.07</v>
-      </c>
-      <c r="AD14" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1">
+        <f>ROW(K14)</f>
         <v>14</v>
       </c>
-      <c r="AG14" s="15" t="str">
+      <c r="AL14" s="15" t="str">
         <f>J14&amp;"-"&amp;COUNTIF($J$1:J14,J14)</f>
         <v>30684125792-1</v>
       </c>
-      <c r="AH14" s="1">
+      <c r="AM14" s="1">
+        <f>IF(K13=K14,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN14" s="1">
+        <f>IF(K14=K15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO14" s="1" t="str">
+        <f>RIGHT(F14)</f>
+        <v>A</v>
+      </c>
+      <c r="AP14" s="1">
+        <f>IF(LEFT(F14,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="13">
+        <f>IF(RIGHT(F14,1)="A",ROUND(O14*N14*(1+Q14),2),AG14)</f>
+        <v>161499.99</v>
+      </c>
+      <c r="AS14" s="13">
+        <f t="shared" si="5"/>
+        <v>133471.07</v>
+      </c>
+      <c r="AT14" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI14" s="1">
+        <v>7.0247929999999998</v>
+      </c>
+      <c r="AU14" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK14" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="13">
-        <f t="shared" si="21"/>
-        <v>161499.99</v>
-      </c>
-      <c r="AN14" s="13">
-        <f t="shared" si="9"/>
-        <v>133471.07</v>
-      </c>
-      <c r="AO14" s="20">
-        <f t="shared" si="10"/>
+        <v>161500</v>
+      </c>
+      <c r="AV14" s="20">
+        <f t="shared" si="17"/>
         <v>7.0247929999999998</v>
       </c>
-      <c r="AP14" s="13">
-        <f t="shared" si="11"/>
-        <v>161500</v>
-      </c>
-      <c r="AQ14" s="20">
-        <f t="shared" si="22"/>
-        <v>7.0247929999999998</v>
-      </c>
-      <c r="AR14" s="2"/>
+      <c r="AW14" s="2"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B15" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C15" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D15" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3347,135 +3524,146 @@
       <c r="L15" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="2"/>
+      <c r="N15" s="4">
         <v>1.5</v>
       </c>
-      <c r="N15" s="5">
+      <c r="O15" s="5">
         <v>19000</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="5">
+        <f t="shared" si="12"/>
+        <v>28500</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="U15" s="12">
+        <v>44816</v>
+      </c>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y15" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z15" s="14">
+        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA15" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB15" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AC15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00002</v>
+      </c>
+      <c r="AD15" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000152</v>
+      </c>
+      <c r="AE15" s="9">
+        <f t="shared" si="15"/>
+        <v>44816</v>
+      </c>
+      <c r="AF15" s="13">
+        <f t="shared" si="4"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AG15" s="13">
         <f t="shared" si="16"/>
         <v>28500</v>
       </c>
-      <c r="P15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q15" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="R15" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S15" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="T15" s="12">
-        <v>44816</v>
-      </c>
-      <c r="U15" s="14">
-        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V15" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="W15" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00002</v>
-      </c>
-      <c r="Y15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000152</v>
-      </c>
-      <c r="Z15" s="9">
-        <f t="shared" si="18"/>
-        <v>44816</v>
-      </c>
-      <c r="AA15" s="13">
-        <f t="shared" si="3"/>
-        <v>4946.28</v>
-      </c>
-      <c r="AB15" s="13">
+      <c r="AH15" s="10" t="str">
+        <f>IF(RIGHT(F15,1)="A",SUBSTITUTE(TEXT(P15,"0,00"),",","."),SUBSTITUTE(TEXT(AG15,"0,00"),",","."))</f>
+        <v>28500.00</v>
+      </c>
+      <c r="AI15" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>28500</v>
-      </c>
-      <c r="AC15" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>28500.00</v>
-      </c>
-      <c r="AD15" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1">
+        <f>ROW(K15)</f>
         <v>15</v>
       </c>
-      <c r="AG15" s="15" t="str">
+      <c r="AL15" s="15" t="str">
         <f>J15&amp;"-"&amp;COUNTIF($J$1:J15,J15)</f>
         <v>30707354719-2</v>
       </c>
-      <c r="AH15" s="1">
+      <c r="AM15" s="1">
+        <f>IF(K14=K15,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN15" s="1">
+        <f>IF(K15=K16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO15" s="1" t="str">
+        <f>RIGHT(F15)</f>
+        <v>B</v>
+      </c>
+      <c r="AP15" s="1">
+        <f>IF(LEFT(F15,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="13">
+        <f>IF(RIGHT(F15,1)="A",ROUND(O15*N15*(1+Q15),2),AG15)</f>
+        <v>28500</v>
+      </c>
+      <c r="AS15" s="13">
+        <f t="shared" si="5"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AT15" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI15" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AU15" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK15" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL15" s="2"/>
-      <c r="AM15" s="13">
-        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
-      <c r="AN15" s="13">
-        <f t="shared" si="9"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AO15" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV15" s="20">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
-      <c r="AP15" s="13">
-        <f t="shared" si="11"/>
-        <v>28500</v>
-      </c>
-      <c r="AQ15" s="20">
-        <f t="shared" si="22"/>
-        <v>1.5</v>
-      </c>
-      <c r="AR15" s="2"/>
+      <c r="AW15" s="2"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B16" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C16" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D16" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3501,135 +3689,146 @@
       <c r="L16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="2"/>
+      <c r="N16" s="4">
         <v>7.003044</v>
       </c>
-      <c r="N16" s="5">
+      <c r="O16" s="5">
         <v>19000</v>
       </c>
-      <c r="O16" s="5">
-        <f t="shared" si="16"/>
+      <c r="P16" s="5">
+        <f t="shared" si="12"/>
         <v>133057.83600000001</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="Q16" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="R16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="S16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="T16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="T16" s="12">
+      <c r="U16" s="12">
         <v>44816</v>
       </c>
-      <c r="U16" s="14">
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y16" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z16" s="14">
         <f>COUNTIFS($F$1:F16,F16,$K$1:K16,K16)+1</f>
         <v>2</v>
       </c>
-      <c r="V16" s="18" t="str">
-        <f t="shared" si="0"/>
+      <c r="AA16" s="18" t="str">
+        <f t="shared" si="1"/>
         <v>7.003044</v>
       </c>
-      <c r="W16" s="18" t="str">
-        <f t="shared" si="17"/>
+      <c r="AB16" s="18" t="str">
+        <f t="shared" si="14"/>
         <v>19000.00</v>
       </c>
-      <c r="X16" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="AC16" s="1" t="str">
+        <f t="shared" si="2"/>
         <v>00002</v>
       </c>
-      <c r="Y16" s="1" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD16" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>00000151</v>
       </c>
-      <c r="Z16" s="9">
-        <f t="shared" si="18"/>
+      <c r="AE16" s="9">
+        <f t="shared" si="15"/>
         <v>44816</v>
       </c>
-      <c r="AA16" s="13">
-        <f t="shared" si="3"/>
+      <c r="AF16" s="13">
+        <f t="shared" si="4"/>
         <v>27942.15</v>
       </c>
-      <c r="AB16" s="13">
+      <c r="AG16" s="13">
+        <f t="shared" si="16"/>
+        <v>160999.99</v>
+      </c>
+      <c r="AH16" s="10" t="str">
+        <f>IF(RIGHT(F16,1)="A",SUBSTITUTE(TEXT(P16,"0,00"),",","."),SUBSTITUTE(TEXT(AG16,"0,00"),",","."))</f>
+        <v>133057.84</v>
+      </c>
+      <c r="AI16" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>160999.99</v>
-      </c>
-      <c r="AC16" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>133057.84</v>
-      </c>
-      <c r="AD16" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.01</v>
       </c>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1">
+        <f>ROW(K16)</f>
         <v>16</v>
       </c>
-      <c r="AG16" s="15" t="str">
+      <c r="AL16" s="15" t="str">
         <f>J16&amp;"-"&amp;COUNTIF($J$1:J16,J16)</f>
         <v>30684125792-2</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AM16" s="1">
+        <f>IF(K15=K16,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN16" s="1">
+        <f>IF(K16=K17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO16" s="1" t="str">
+        <f>RIGHT(F16)</f>
+        <v>A</v>
+      </c>
+      <c r="AP16" s="1">
+        <f>IF(LEFT(F16,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="13">
+        <f>IF(RIGHT(F16,1)="A",ROUND(O16*N16*(1+Q16),2),AG16)</f>
+        <v>160999.98000000001</v>
+      </c>
+      <c r="AS16" s="13">
+        <f t="shared" si="5"/>
+        <v>133057.82999999999</v>
+      </c>
+      <c r="AT16" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI16" s="1">
+        <v>7.003044</v>
+      </c>
+      <c r="AU16" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>A</v>
-      </c>
-      <c r="AK16" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL16" s="2"/>
-      <c r="AM16" s="13">
-        <f t="shared" si="21"/>
-        <v>160999.98000000001</v>
-      </c>
-      <c r="AN16" s="13">
-        <f t="shared" si="9"/>
-        <v>133057.82999999999</v>
-      </c>
-      <c r="AO16" s="20">
-        <f t="shared" si="10"/>
+        <v>161000</v>
+      </c>
+      <c r="AV16" s="20">
+        <f t="shared" si="17"/>
         <v>7.003044</v>
       </c>
-      <c r="AP16" s="13">
-        <f t="shared" si="11"/>
-        <v>161000</v>
-      </c>
-      <c r="AQ16" s="20">
-        <f t="shared" si="22"/>
-        <v>7.003044</v>
-      </c>
-      <c r="AR16" s="2"/>
+      <c r="AW16" s="2"/>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f t="shared" ca="1" si="12"/>
-        <v>45107</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>45140</v>
       </c>
       <c r="B17" s="9">
-        <f t="shared" ca="1" si="13"/>
-        <v>45047</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>45108</v>
       </c>
       <c r="C17" s="9">
-        <f t="shared" ca="1" si="14"/>
-        <v>45077</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>45138</v>
       </c>
       <c r="D17" s="9">
-        <f t="shared" ca="1" si="15"/>
-        <v>45121</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>45154</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3655,122 +3854,133 @@
       <c r="L17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="2"/>
+      <c r="N17" s="4">
         <v>1.5</v>
       </c>
-      <c r="N17" s="5">
+      <c r="O17" s="5">
         <v>19000</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="5">
+        <f t="shared" si="12"/>
+        <v>28500</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="U17" s="12">
+        <v>44816</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="Y17" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="Z17" s="14">
+        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA17" s="18" t="str">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="AB17" s="18" t="str">
+        <f t="shared" si="14"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AC17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>00002</v>
+      </c>
+      <c r="AD17" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>00000153</v>
+      </c>
+      <c r="AE17" s="9">
+        <f t="shared" si="15"/>
+        <v>44816</v>
+      </c>
+      <c r="AF17" s="13">
+        <f t="shared" si="4"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AG17" s="13">
         <f t="shared" si="16"/>
         <v>28500</v>
       </c>
-      <c r="P17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q17" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R17" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="S17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="T17" s="12">
-        <v>44816</v>
-      </c>
-      <c r="U17" s="14">
-        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
-        <v>2</v>
-      </c>
-      <c r="V17" s="18" t="str">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="W17" s="18" t="str">
-        <f t="shared" si="17"/>
-        <v>19000.00</v>
-      </c>
-      <c r="X17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>00002</v>
-      </c>
-      <c r="Y17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000153</v>
-      </c>
-      <c r="Z17" s="9">
-        <f t="shared" si="18"/>
-        <v>44816</v>
-      </c>
-      <c r="AA17" s="13">
-        <f t="shared" si="3"/>
-        <v>4946.28</v>
-      </c>
-      <c r="AB17" s="13">
+      <c r="AH17" s="10" t="str">
+        <f>IF(RIGHT(F17,1)="A",SUBSTITUTE(TEXT(P17,"0,00"),",","."),SUBSTITUTE(TEXT(AG17,"0,00"),",","."))</f>
+        <v>28500.00</v>
+      </c>
+      <c r="AI17" s="10" t="str">
         <f t="shared" si="19"/>
-        <v>28500</v>
-      </c>
-      <c r="AC17" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>28500.00</v>
-      </c>
-      <c r="AD17" s="10" t="str">
-        <f t="shared" si="23"/>
         <v>0.00</v>
       </c>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1">
-        <f t="shared" si="5"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1">
+        <f>ROW(K17)</f>
         <v>17</v>
       </c>
-      <c r="AG17" s="15" t="str">
+      <c r="AL17" s="15" t="str">
         <f>J17&amp;"-"&amp;COUNTIF($J$1:J17,J17)</f>
         <v>37473042-2</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AM17" s="1">
+        <f>IF(K16=K17,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AN17" s="1">
+        <f>IF(K17=K18,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AO17" s="1" t="str">
+        <f>RIGHT(F17)</f>
+        <v>B</v>
+      </c>
+      <c r="AP17" s="1">
+        <f>IF(LEFT(F17,4)="Nota",0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="13">
+        <f>IF(RIGHT(F17,1)="A",ROUND(O17*N17*(1+Q17),2),AG17)</f>
+        <v>28500</v>
+      </c>
+      <c r="AS17" s="13">
+        <f t="shared" si="5"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AT17" s="20">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AI17" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="AU17" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>B</v>
-      </c>
-      <c r="AK17" s="1">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="13">
-        <f t="shared" si="21"/>
         <v>28500</v>
       </c>
-      <c r="AN17" s="13">
-        <f t="shared" si="9"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AO17" s="20">
-        <f t="shared" si="10"/>
+      <c r="AV17" s="20">
+        <f t="shared" si="17"/>
         <v>1.5</v>
       </c>
-      <c r="AP17" s="13">
-        <f t="shared" si="11"/>
-        <v>28500</v>
-      </c>
-      <c r="AQ17" s="20">
-        <f t="shared" si="22"/>
-        <v>1.5</v>
-      </c>
-      <c r="AR17" s="2"/>
+      <c r="AW17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AP17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AO17">
+  <autoFilter ref="A1:AU17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AT17">
     <sortCondition ref="F2:F17"/>
     <sortCondition ref="H2:H17"/>
     <sortCondition ref="J2:J17"/>

</xml_diff>

<commit_message>
Update Excel to save Files in specific path
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808C8CFD-07D8-45CA-8342-D05B09214139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D8F79-BB93-4A98-95BE-CE9A56432F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Factura" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AU$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Factura!$A$1:$AZ$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="94">
   <si>
     <t>Fecha</t>
   </si>
@@ -300,6 +300,24 @@
   </si>
   <si>
     <t>Bonif Facturador</t>
+  </si>
+  <si>
+    <t>Domicilio</t>
+  </si>
+  <si>
+    <t>Guardar</t>
+  </si>
+  <si>
+    <t>Ubicación a Guardar</t>
+  </si>
+  <si>
+    <t>C:\Users\ABP\Desktop\Test\</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -840,7 +858,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -865,7 +883,6 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1228,12 +1245,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AW17"/>
+  <dimension ref="A1:AZ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AK1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="AJ1" sqref="AJ1"/>
+      <selection pane="bottomLeft" activeCell="AY12" sqref="AY12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1289,7 @@
     <col min="46" max="46" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1420,11 +1437,20 @@
       <c r="AW1" s="19" t="s">
         <v>80</v>
       </c>
+      <c r="AX1" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B2" s="9">
         <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
@@ -1436,7 +1462,7 @@
       </c>
       <c r="D2" s="9">
         <f ca="1">A2+14</f>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1530,7 +1556,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG2,0)-AG2,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AJ2" s="22"/>
+      <c r="AJ2" s="2"/>
       <c r="AK2" s="1">
         <f t="shared" ref="AK2:AK17" si="6">ROW(K2)</f>
         <v>2</v>
@@ -1577,11 +1603,18 @@
         <v>7.003044</v>
       </c>
       <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A17" ca="1" si="15">TODAY()</f>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B3" s="9">
         <f t="shared" ref="B3:B17" ca="1" si="16">DATE(YEAR(C3),MONTH(C3),1)</f>
@@ -1593,7 +1626,7 @@
       </c>
       <c r="D3" s="9">
         <f t="shared" ref="D3:D17" ca="1" si="18">A3+14</f>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1688,7 +1721,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG3,0)-AG3,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AJ3" s="22"/>
+      <c r="AJ3" s="2"/>
       <c r="AK3" s="1">
         <f t="shared" si="6"/>
         <v>3</v>
@@ -1735,11 +1768,18 @@
         <v>8.0252280000000003</v>
       </c>
       <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -1751,7 +1791,7 @@
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1846,7 +1886,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG4,0)-AG4,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AJ4" s="22"/>
+      <c r="AJ4" s="2"/>
       <c r="AK4" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
@@ -1893,11 +1933,18 @@
         <v>10.004348999999999</v>
       </c>
       <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -1909,7 +1956,7 @@
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -2004,7 +2051,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG5,0)-AG5,"0,00"),",",".")</f>
         <v>0.00</v>
       </c>
-      <c r="AJ5" s="22"/>
+      <c r="AJ5" s="2"/>
       <c r="AK5" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
@@ -2051,11 +2098,18 @@
         <v>9.0256629999999998</v>
       </c>
       <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2067,7 +2121,7 @@
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2170,7 +2224,7 @@
         <f>SUBSTITUTE(TEXT(ROUNDUP(AG6,0)-AG6,"0,00"),",",".")</f>
         <v>0.01</v>
       </c>
-      <c r="AJ6" s="22"/>
+      <c r="AJ6" s="2"/>
       <c r="AK6" s="1">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -2217,11 +2271,18 @@
         <v>5.0239229999999999</v>
       </c>
       <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ6" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2233,7 +2294,7 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2327,7 +2388,7 @@
         <f t="shared" ref="AI7:AI17" si="26">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
-      <c r="AJ7" s="22"/>
+      <c r="AJ7" s="2"/>
       <c r="AK7" s="1">
         <f t="shared" si="6"/>
         <v>7</v>
@@ -2374,11 +2435,18 @@
         <v>5.0021740000000001</v>
       </c>
       <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B8" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2390,7 +2458,7 @@
       </c>
       <c r="D8" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2485,7 +2553,7 @@
         <f t="shared" si="26"/>
         <v>0.02</v>
       </c>
-      <c r="AJ8" s="22"/>
+      <c r="AJ8" s="2"/>
       <c r="AK8" s="1">
         <f t="shared" si="6"/>
         <v>8</v>
@@ -2532,11 +2600,18 @@
         <v>10.004348999999999</v>
       </c>
       <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B9" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2548,7 +2623,7 @@
       </c>
       <c r="D9" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2643,7 +2718,7 @@
         <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AJ9" s="22"/>
+      <c r="AJ9" s="2"/>
       <c r="AK9" s="1">
         <f t="shared" si="6"/>
         <v>9</v>
@@ -2690,11 +2765,18 @@
         <v>1.0221830000000001</v>
       </c>
       <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ9" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B10" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2706,7 +2788,7 @@
       </c>
       <c r="D10" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2801,7 +2883,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ10" s="22"/>
+      <c r="AJ10" s="2"/>
       <c r="AK10" s="1">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -2848,11 +2930,18 @@
         <v>1.0439320000000001</v>
       </c>
       <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ10" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B11" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2864,7 +2953,7 @@
       </c>
       <c r="D11" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2959,7 +3048,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ11" s="22"/>
+      <c r="AJ11" s="2"/>
       <c r="AK11" s="1">
         <f t="shared" si="6"/>
         <v>11</v>
@@ -3006,11 +3095,16 @@
         <v>1.3</v>
       </c>
       <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ11" s="2"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B12" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3022,7 +3116,7 @@
       </c>
       <c r="D12" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -3117,7 +3211,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ12" s="22"/>
+      <c r="AJ12" s="2"/>
       <c r="AK12" s="1">
         <f t="shared" si="6"/>
         <v>12</v>
@@ -3164,11 +3258,16 @@
         <v>1.2105263157894737</v>
       </c>
       <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ12" s="2"/>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B13" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3180,7 +3279,7 @@
       </c>
       <c r="D13" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3271,7 +3370,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ13" s="22"/>
+      <c r="AJ13" s="2"/>
       <c r="AK13" s="1">
         <f t="shared" si="6"/>
         <v>13</v>
@@ -3318,11 +3417,16 @@
         <v>1.5</v>
       </c>
       <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ13" s="2"/>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B14" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3334,7 +3438,7 @@
       </c>
       <c r="D14" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3436,7 +3540,7 @@
         <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AJ14" s="22"/>
+      <c r="AJ14" s="2"/>
       <c r="AK14" s="1">
         <f t="shared" si="6"/>
         <v>14</v>
@@ -3483,11 +3587,16 @@
         <v>7.0247929999999998</v>
       </c>
       <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ14" s="2"/>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B15" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3499,7 +3608,7 @@
       </c>
       <c r="D15" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3601,7 +3710,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ15" s="22"/>
+      <c r="AJ15" s="2"/>
       <c r="AK15" s="1">
         <f t="shared" si="6"/>
         <v>15</v>
@@ -3648,11 +3757,16 @@
         <v>1.5</v>
       </c>
       <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ15" s="2"/>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B16" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3664,7 +3778,7 @@
       </c>
       <c r="D16" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3766,7 +3880,7 @@
         <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AJ16" s="22"/>
+      <c r="AJ16" s="2"/>
       <c r="AK16" s="1">
         <f t="shared" si="6"/>
         <v>16</v>
@@ -3813,11 +3927,16 @@
         <v>7.003044</v>
       </c>
       <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ16" s="2"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45140</v>
+        <v>45141</v>
       </c>
       <c r="B17" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3829,7 +3948,7 @@
       </c>
       <c r="D17" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45154</v>
+        <v>45155</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -3931,7 +4050,7 @@
         <f t="shared" si="26"/>
         <v>0.00</v>
       </c>
-      <c r="AJ17" s="22"/>
+      <c r="AJ17" s="2"/>
       <c r="AK17" s="1">
         <f t="shared" si="6"/>
         <v>17</v>
@@ -3978,14 +4097,24 @@
         <v>1.5</v>
       </c>
       <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AU17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AZ17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AT17">
     <sortCondition ref="F2:F17"/>
     <sortCondition ref="H2:H17"/>
     <sortCondition ref="J2:J17"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY17" xr:uid="{BFC33D16-50A8-46DB-B879-EC5A925DAA79}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Item de Excel
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325D8F79-BB93-4A98-95BE-CE9A56432F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05420977-D2CA-43ED-A60E-0ACE3D0EC790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1247,10 +1247,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft" activeCell="AY12" sqref="AY12"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,7 +1450,7 @@
     <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B2" s="9">
         <f ca="1">DATE(YEAR(C2),MONTH(C2),1)</f>
@@ -1462,7 +1462,7 @@
       </c>
       <c r="D2" s="9">
         <f ca="1">A2+14</f>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E2" s="2">
         <v>2</v>
@@ -1517,7 +1517,7 @@
         <v/>
       </c>
       <c r="Z2" s="14">
-        <f>COUNTIFS($F$1:F2,F2,$K$1:K2,K2)+1</f>
+        <f>COUNTIFS(K1:K2,K2,F1:F2,F2,J1:J2,J2)+1</f>
         <v>2</v>
       </c>
       <c r="AA2" s="18" t="str">
@@ -1614,7 +1614,7 @@
     <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <f t="shared" ref="A3:A17" ca="1" si="15">TODAY()</f>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B3" s="9">
         <f t="shared" ref="B3:B17" ca="1" si="16">DATE(YEAR(C3),MONTH(C3),1)</f>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="D3" s="9">
         <f t="shared" ref="D3:D17" ca="1" si="18">A3+14</f>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -1682,7 +1682,7 @@
         <v/>
       </c>
       <c r="Z3" s="14">
-        <f>COUNTIFS($F$1:F3,F3,$K$1:K3,K3)+1</f>
+        <f t="shared" ref="Z3:Z17" si="21">COUNTIFS(K2:K3,K3,F2:F3,F3,J2:J3,J3)+1</f>
         <v>2</v>
       </c>
       <c r="AA3" s="18" t="str">
@@ -1690,7 +1690,7 @@
         <v>8.025228</v>
       </c>
       <c r="AB3" s="18" t="str">
-        <f t="shared" ref="AB3:AB17" si="21">SUBSTITUTE(TEXT(O3,"0,00"),",",".")</f>
+        <f t="shared" ref="AB3:AB17" si="22">SUBSTITUTE(TEXT(O3,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
       <c r="AC3" s="1" t="str">
@@ -1702,7 +1702,7 @@
         <v>00000000</v>
       </c>
       <c r="AE3" s="9">
-        <f t="shared" ref="AE3:AE17" si="22">U3</f>
+        <f t="shared" ref="AE3:AE17" si="23">U3</f>
         <v>0</v>
       </c>
       <c r="AF3" s="13">
@@ -1710,7 +1710,7 @@
         <v>32020.66</v>
       </c>
       <c r="AG3" s="13">
-        <f t="shared" ref="AG3:AG17" si="23">IF(AO3="A",ROUND(P3+AF3,2),ROUND(P3,2))</f>
+        <f t="shared" ref="AG3:AG17" si="24">IF(AO3="A",ROUND(P3+AF3,2),ROUND(P3,2))</f>
         <v>184499.99</v>
       </c>
       <c r="AH3" s="10" t="str">
@@ -1764,7 +1764,7 @@
         <v>184500</v>
       </c>
       <c r="AV3" s="20">
-        <f t="shared" ref="AV3:AV17" si="24">IF(AO3="A",ROUND(AS3/O3,6),AU3/O3)</f>
+        <f t="shared" ref="AV3:AV17" si="25">IF(AO3="A",ROUND(AS3/O3,6),AU3/O3)</f>
         <v>8.0252280000000003</v>
       </c>
       <c r="AW3" s="2"/>
@@ -1779,7 +1779,7 @@
     <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B4" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="D4" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
@@ -1843,11 +1843,11 @@
         <v/>
       </c>
       <c r="Y4" s="1" t="str">
-        <f t="shared" ref="Y4:Y17" si="25">SUBSTITUTE(W4,",",".")</f>
+        <f t="shared" ref="Y4:Y17" si="26">SUBSTITUTE(W4,",",".")</f>
         <v/>
       </c>
       <c r="Z4" s="14">
-        <f>COUNTIFS($F$1:F4,F4,$K$1:K4,K4)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA4" s="18" t="str">
@@ -1855,7 +1855,7 @@
         <v>10.004349</v>
       </c>
       <c r="AB4" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC4" s="1" t="str">
@@ -1867,7 +1867,7 @@
         <v>00000000</v>
       </c>
       <c r="AE4" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF4" s="13">
@@ -1875,7 +1875,7 @@
         <v>39917.35</v>
       </c>
       <c r="AG4" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>229999.98</v>
       </c>
       <c r="AH4" s="10" t="str">
@@ -1929,7 +1929,7 @@
         <v>230000</v>
       </c>
       <c r="AV4" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AW4" s="2"/>
@@ -1944,7 +1944,7 @@
     <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B5" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="D5" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E5" s="2">
         <v>2</v>
@@ -2008,11 +2008,11 @@
         <v/>
       </c>
       <c r="Y5" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z5" s="14">
-        <f>COUNTIFS($F$1:F5,F5,$K$1:K5,K5)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA5" s="18" t="str">
@@ -2020,7 +2020,7 @@
         <v>9.025663</v>
       </c>
       <c r="AB5" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC5" s="1" t="str">
@@ -2032,7 +2032,7 @@
         <v>00000000</v>
       </c>
       <c r="AE5" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF5" s="13">
@@ -2040,7 +2040,7 @@
         <v>36012.400000000001</v>
       </c>
       <c r="AG5" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>207500</v>
       </c>
       <c r="AH5" s="10" t="str">
@@ -2094,7 +2094,7 @@
         <v>207500</v>
       </c>
       <c r="AV5" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AW5" s="2"/>
@@ -2109,7 +2109,7 @@
     <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B6" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="D6" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E6" s="2">
         <v>2</v>
@@ -2181,11 +2181,11 @@
         <v/>
       </c>
       <c r="Y6" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z6" s="14">
-        <f>COUNTIFS($F$1:F6,F6,$K$1:K6,K6)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA6" s="18" t="str">
@@ -2193,7 +2193,7 @@
         <v>5.023923</v>
       </c>
       <c r="AB6" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC6" s="1" t="str">
@@ -2205,7 +2205,7 @@
         <v>00000003</v>
       </c>
       <c r="AE6" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>44816</v>
       </c>
       <c r="AF6" s="13">
@@ -2213,7 +2213,7 @@
         <v>20045.45</v>
       </c>
       <c r="AG6" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>115499.99</v>
       </c>
       <c r="AH6" s="10" t="str">
@@ -2267,7 +2267,7 @@
         <v>115500</v>
       </c>
       <c r="AV6" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AW6" s="2"/>
@@ -2282,7 +2282,7 @@
     <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B7" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="D7" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E7" s="2">
         <v>2</v>
@@ -2345,11 +2345,11 @@
         <v/>
       </c>
       <c r="Y7" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z7" s="14">
-        <f>COUNTIFS($F$1:F7,F7,$K$1:K7,K7)+1</f>
+        <f t="shared" si="21"/>
         <v>3</v>
       </c>
       <c r="AA7" s="18" t="str">
@@ -2357,7 +2357,7 @@
         <v>5.002174</v>
       </c>
       <c r="AB7" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC7" s="1" t="str">
@@ -2369,7 +2369,7 @@
         <v>00000000</v>
       </c>
       <c r="AE7" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF7" s="13">
@@ -2377,7 +2377,7 @@
         <v>19958.669999999998</v>
       </c>
       <c r="AG7" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>114999.98</v>
       </c>
       <c r="AH7" s="10" t="str">
@@ -2385,7 +2385,7 @@
         <v>95041.31</v>
       </c>
       <c r="AI7" s="10" t="str">
-        <f t="shared" ref="AI7:AI17" si="26">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
+        <f t="shared" ref="AI7:AI17" si="27">SUBSTITUTE(TEXT(ROUNDUP(AG7,0)-AG7,"0,00"),",",".")</f>
         <v>0.02</v>
       </c>
       <c r="AJ7" s="2"/>
@@ -2431,7 +2431,7 @@
         <v>115000</v>
       </c>
       <c r="AV7" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AW7" s="2"/>
@@ -2446,7 +2446,7 @@
     <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B8" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="D8" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
@@ -2482,7 +2482,7 @@
         <v>52</v>
       </c>
       <c r="L8" s="1" t="str">
-        <f t="shared" ref="L8:L13" ca="1" si="27">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
+        <f t="shared" ref="L8:L13" ca="1" si="28">"Honorarios "&amp;PROPER(TEXT(B8,"mmmm"))</f>
         <v>Honorarios Julio</v>
       </c>
       <c r="M8" s="2"/>
@@ -2510,11 +2510,11 @@
         <v/>
       </c>
       <c r="Y8" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z8" s="14">
-        <f>COUNTIFS($F$1:F8,F8,$K$1:K8,K8)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA8" s="18" t="str">
@@ -2522,7 +2522,7 @@
         <v>10.004349</v>
       </c>
       <c r="AB8" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC8" s="1" t="str">
@@ -2534,7 +2534,7 @@
         <v>00000000</v>
       </c>
       <c r="AE8" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF8" s="13">
@@ -2542,7 +2542,7 @@
         <v>39917.35</v>
       </c>
       <c r="AG8" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>229999.98</v>
       </c>
       <c r="AH8" s="10" t="str">
@@ -2550,7 +2550,7 @@
         <v>190082.63</v>
       </c>
       <c r="AI8" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.02</v>
       </c>
       <c r="AJ8" s="2"/>
@@ -2596,7 +2596,7 @@
         <v>230000</v>
       </c>
       <c r="AV8" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AW8" s="2"/>
@@ -2611,7 +2611,7 @@
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B9" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2623,7 +2623,7 @@
       </c>
       <c r="D9" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E9" s="2">
         <v>2</v>
@@ -2647,7 +2647,7 @@
         <v>57</v>
       </c>
       <c r="L9" s="1" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="M9" s="2"/>
@@ -2675,11 +2675,11 @@
         <v/>
       </c>
       <c r="Y9" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z9" s="14">
-        <f>COUNTIFS($F$1:F9,F9,$K$1:K9,K9)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA9" s="18" t="str">
@@ -2687,7 +2687,7 @@
         <v>1.022183</v>
       </c>
       <c r="AB9" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC9" s="1" t="str">
@@ -2699,7 +2699,7 @@
         <v>00000000</v>
       </c>
       <c r="AE9" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF9" s="13">
@@ -2707,7 +2707,7 @@
         <v>4078.51</v>
       </c>
       <c r="AG9" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>23499.99</v>
       </c>
       <c r="AH9" s="10" t="str">
@@ -2715,7 +2715,7 @@
         <v>19421.48</v>
       </c>
       <c r="AI9" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.01</v>
       </c>
       <c r="AJ9" s="2"/>
@@ -2761,7 +2761,7 @@
         <v>23500</v>
       </c>
       <c r="AV9" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AW9" s="2"/>
@@ -2776,7 +2776,7 @@
     <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B10" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="D10" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -2812,7 +2812,7 @@
         <v>56</v>
       </c>
       <c r="L10" s="1" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="M10" s="2"/>
@@ -2840,11 +2840,11 @@
         <v/>
       </c>
       <c r="Y10" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z10" s="14">
-        <f>COUNTIFS($F$1:F10,F10,$K$1:K10,K10)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA10" s="18" t="str">
@@ -2852,7 +2852,7 @@
         <v>1.043932</v>
       </c>
       <c r="AB10" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC10" s="1" t="str">
@@ -2864,7 +2864,7 @@
         <v>00000000</v>
       </c>
       <c r="AE10" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF10" s="13">
@@ -2872,7 +2872,7 @@
         <v>4165.29</v>
       </c>
       <c r="AG10" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>24000</v>
       </c>
       <c r="AH10" s="10" t="str">
@@ -2880,7 +2880,7 @@
         <v>19834.71</v>
       </c>
       <c r="AI10" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.00</v>
       </c>
       <c r="AJ10" s="2"/>
@@ -2926,7 +2926,7 @@
         <v>24000</v>
       </c>
       <c r="AV10" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AW10" s="2"/>
@@ -2941,7 +2941,7 @@
     <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B11" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="D11" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
@@ -2977,7 +2977,7 @@
         <v>56</v>
       </c>
       <c r="L11" s="1" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="M11" s="2"/>
@@ -3005,11 +3005,11 @@
         <v/>
       </c>
       <c r="Y11" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z11" s="14">
-        <f>COUNTIFS($F$1:F11,F11,$K$1:K11,K11)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA11" s="18" t="str">
@@ -3017,7 +3017,7 @@
         <v>1.3</v>
       </c>
       <c r="AB11" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10000.00</v>
       </c>
       <c r="AC11" s="1" t="str">
@@ -3029,7 +3029,7 @@
         <v>00000000</v>
       </c>
       <c r="AE11" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF11" s="13">
@@ -3037,7 +3037,7 @@
         <v>2256.1999999999998</v>
       </c>
       <c r="AG11" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>13000</v>
       </c>
       <c r="AH11" s="10" t="str">
@@ -3045,7 +3045,7 @@
         <v>13000.00</v>
       </c>
       <c r="AI11" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.00</v>
       </c>
       <c r="AJ11" s="2"/>
@@ -3091,7 +3091,7 @@
         <v>13000</v>
       </c>
       <c r="AV11" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.3</v>
       </c>
       <c r="AW11" s="2"/>
@@ -3104,7 +3104,7 @@
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B12" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="D12" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
@@ -3140,7 +3140,7 @@
         <v>60</v>
       </c>
       <c r="L12" s="1" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="M12" s="2"/>
@@ -3168,11 +3168,11 @@
         <v/>
       </c>
       <c r="Y12" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z12" s="14">
-        <f>COUNTIFS($F$1:F12,F12,$K$1:K12,K12)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA12" s="18" t="str">
@@ -3180,7 +3180,7 @@
         <v>1.210526</v>
       </c>
       <c r="AB12" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC12" s="1" t="str">
@@ -3192,7 +3192,7 @@
         <v>00000000</v>
       </c>
       <c r="AE12" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF12" s="13">
@@ -3200,7 +3200,7 @@
         <v>3991.74</v>
       </c>
       <c r="AG12" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>23000</v>
       </c>
       <c r="AH12" s="10" t="str">
@@ -3208,7 +3208,7 @@
         <v>23000.00</v>
       </c>
       <c r="AI12" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.00</v>
       </c>
       <c r="AJ12" s="2"/>
@@ -3254,7 +3254,7 @@
         <v>23000</v>
       </c>
       <c r="AV12" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.2105263157894737</v>
       </c>
       <c r="AW12" s="2"/>
@@ -3267,7 +3267,7 @@
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B13" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="D13" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -3301,7 +3301,7 @@
         <v>70</v>
       </c>
       <c r="L13" s="1" t="str">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="28"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="M13" s="2"/>
@@ -3327,19 +3327,19 @@
         <v/>
       </c>
       <c r="Y13" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z13" s="14">
-        <f>COUNTIFS($F$1:F13,F13,$K$1:K13,K13)+1</f>
-        <v>2</v>
+        <f t="shared" si="21"/>
+        <v>1</v>
       </c>
       <c r="AA13" s="18" t="str">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="AB13" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC13" s="1" t="str">
@@ -3351,7 +3351,7 @@
         <v>00000000</v>
       </c>
       <c r="AE13" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AF13" s="13">
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="AG13" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>28500</v>
       </c>
       <c r="AH13" s="10" t="str">
@@ -3367,7 +3367,7 @@
         <v>28500.00</v>
       </c>
       <c r="AI13" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.00</v>
       </c>
       <c r="AJ13" s="2"/>
@@ -3413,7 +3413,7 @@
         <v>28500</v>
       </c>
       <c r="AV13" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.5</v>
       </c>
       <c r="AW13" s="2"/>
@@ -3426,7 +3426,7 @@
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B14" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="D14" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E14" s="2">
         <v>2</v>
@@ -3497,11 +3497,11 @@
         <v/>
       </c>
       <c r="Y14" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z14" s="14">
-        <f>COUNTIFS($F$1:F14,F14,$K$1:K14,K14)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA14" s="18" t="str">
@@ -3509,7 +3509,7 @@
         <v>7.024793</v>
       </c>
       <c r="AB14" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC14" s="1" t="str">
@@ -3521,7 +3521,7 @@
         <v>00000150</v>
       </c>
       <c r="AE14" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>44816</v>
       </c>
       <c r="AF14" s="13">
@@ -3529,7 +3529,7 @@
         <v>28028.92</v>
       </c>
       <c r="AG14" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>161499.99</v>
       </c>
       <c r="AH14" s="10" t="str">
@@ -3537,7 +3537,7 @@
         <v>133471.07</v>
       </c>
       <c r="AI14" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.01</v>
       </c>
       <c r="AJ14" s="2"/>
@@ -3583,7 +3583,7 @@
         <v>161500</v>
       </c>
       <c r="AV14" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AW14" s="2"/>
@@ -3596,7 +3596,7 @@
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B15" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="D15" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -3667,11 +3667,11 @@
         <v/>
       </c>
       <c r="Y15" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z15" s="14">
-        <f>COUNTIFS($F$1:F15,F15,$K$1:K15,K15)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA15" s="18" t="str">
@@ -3679,7 +3679,7 @@
         <v>1.5</v>
       </c>
       <c r="AB15" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC15" s="1" t="str">
@@ -3691,7 +3691,7 @@
         <v>00000152</v>
       </c>
       <c r="AE15" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>44816</v>
       </c>
       <c r="AF15" s="13">
@@ -3699,7 +3699,7 @@
         <v>4946.28</v>
       </c>
       <c r="AG15" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>28500</v>
       </c>
       <c r="AH15" s="10" t="str">
@@ -3707,7 +3707,7 @@
         <v>28500.00</v>
       </c>
       <c r="AI15" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.00</v>
       </c>
       <c r="AJ15" s="2"/>
@@ -3753,7 +3753,7 @@
         <v>28500</v>
       </c>
       <c r="AV15" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.5</v>
       </c>
       <c r="AW15" s="2"/>
@@ -3766,7 +3766,7 @@
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B16" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3778,7 +3778,7 @@
       </c>
       <c r="D16" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E16" s="2">
         <v>2</v>
@@ -3837,11 +3837,11 @@
         <v/>
       </c>
       <c r="Y16" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z16" s="14">
-        <f>COUNTIFS($F$1:F16,F16,$K$1:K16,K16)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA16" s="18" t="str">
@@ -3849,7 +3849,7 @@
         <v>7.003044</v>
       </c>
       <c r="AB16" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC16" s="1" t="str">
@@ -3861,7 +3861,7 @@
         <v>00000151</v>
       </c>
       <c r="AE16" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>44816</v>
       </c>
       <c r="AF16" s="13">
@@ -3869,7 +3869,7 @@
         <v>27942.15</v>
       </c>
       <c r="AG16" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>160999.99</v>
       </c>
       <c r="AH16" s="10" t="str">
@@ -3877,7 +3877,7 @@
         <v>133057.84</v>
       </c>
       <c r="AI16" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.01</v>
       </c>
       <c r="AJ16" s="2"/>
@@ -3923,7 +3923,7 @@
         <v>161000</v>
       </c>
       <c r="AV16" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>7.003044</v>
       </c>
       <c r="AW16" s="2"/>
@@ -3936,7 +3936,7 @@
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <f t="shared" ca="1" si="15"/>
-        <v>45141</v>
+        <v>45145</v>
       </c>
       <c r="B17" s="9">
         <f t="shared" ca="1" si="16"/>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="D17" s="9">
         <f t="shared" ca="1" si="18"/>
-        <v>45155</v>
+        <v>45159</v>
       </c>
       <c r="E17" s="2">
         <v>2</v>
@@ -4007,11 +4007,11 @@
         <v/>
       </c>
       <c r="Y17" s="1" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="Z17" s="14">
-        <f>COUNTIFS($F$1:F17,F17,$K$1:K17,K17)+1</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="AA17" s="18" t="str">
@@ -4019,7 +4019,7 @@
         <v>1.5</v>
       </c>
       <c r="AB17" s="18" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19000.00</v>
       </c>
       <c r="AC17" s="1" t="str">
@@ -4031,7 +4031,7 @@
         <v>00000153</v>
       </c>
       <c r="AE17" s="9">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>44816</v>
       </c>
       <c r="AF17" s="13">
@@ -4039,7 +4039,7 @@
         <v>4946.28</v>
       </c>
       <c r="AG17" s="13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>28500</v>
       </c>
       <c r="AH17" s="10" t="str">
@@ -4047,7 +4047,7 @@
         <v>28500.00</v>
       </c>
       <c r="AI17" s="10" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.00</v>
       </c>
       <c r="AJ17" s="2"/>
@@ -4093,7 +4093,7 @@
         <v>28500</v>
       </c>
       <c r="AV17" s="20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1.5</v>
       </c>
       <c r="AW17" s="2"/>

</xml_diff>

<commit_message>
add more notes to Excel
</commit_message>
<xml_diff>
--- a/Archivo para hacer Facturas 3.0.xlsx
+++ b/Archivo para hacer Facturas 3.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\BOT-Facturador-AFIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9D067D-90FD-46FE-8564-6AD332574543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B55724-159F-4EBB-88C1-53FE973874F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,6 +66,78 @@
           </rPr>
           <t xml:space="preserve">
 Acá se pone el nombre a guardar de las facturas. Si se deja vacío se guarda con el nombre que define AFIP.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{145828BA-C2F6-4D99-9916-A141DEC4F2EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Agustín Bustos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sin ST: SI: ejecutar cuando el bot no guarda los archivos con el nombre/ubicación definida</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F0D38E68-6A29-4ACF-8101-B3185BB736E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Agustín Bustos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Si se desae guardar el Archivo poner SI</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{A6804AC2-672B-4DDA-AD87-CE9C0D7B96C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Agustín Bustos:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+la ubicación va desde el disco hasta la \final</t>
         </r>
       </text>
     </comment>
@@ -1053,7 +1125,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1078,7 +1150,6 @@
     <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1587,7 +1658,7 @@
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="K17" sqref="K17"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1864,7 @@
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
-        <f>CONCATENATE(J2," - ",O2," - ",P2," - ",S2)</f>
+        <f t="shared" ref="A2:A17" si="0">CONCATENATE(J2," - ",O2," - ",P2," - ",S2)</f>
         <v>2 - 30525390086 - COCA COLA FEMSA DE BUENOS AIRES S A - Ajustes Marzo/Abril 2022</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1878,15 +1949,15 @@
         <v/>
       </c>
       <c r="AF2" s="1" t="str">
-        <f t="shared" ref="AF2" si="0">SUBSTITUTE(AD2,",",".")</f>
+        <f t="shared" ref="AF2" si="1">SUBSTITUTE(AD2,",",".")</f>
         <v/>
       </c>
       <c r="AG2" s="14">
-        <f>COUNTIFS(J1:J2,J2,K1:K2,K2,P1:P2,P2)+1</f>
+        <f t="shared" ref="AG2:AG17" si="2">COUNTIFS(J1:J2,J2,K1:K2,K2,P1:P2,P2)+1</f>
         <v>2</v>
       </c>
       <c r="AH2" s="18" t="str">
-        <f t="shared" ref="AH2:AH17" si="1">SUBSTITUTE(IF(AU2="A",ROUND(W2/V2,6),ROUND(AN2/V2,6)),",",".")</f>
+        <f t="shared" ref="AH2:AH17" si="3">SUBSTITUTE(IF(AU2="A",ROUND(W2/V2,6),ROUND(AN2/V2,6)),",",".")</f>
         <v>7.003044</v>
       </c>
       <c r="AI2" s="18" t="str">
@@ -1894,11 +1965,11 @@
         <v>19000.00</v>
       </c>
       <c r="AJ2" s="1" t="str">
-        <f t="shared" ref="AJ2:AJ17" si="2">TEXT(Z2,"00000")</f>
+        <f t="shared" ref="AJ2:AJ17" si="4">TEXT(Z2,"00000")</f>
         <v>00000</v>
       </c>
       <c r="AK2" s="1" t="str">
-        <f t="shared" ref="AK2:AK17" si="3">TEXT(AA2,"00000000")</f>
+        <f t="shared" ref="AK2:AK17" si="5">TEXT(AA2,"00000000")</f>
         <v>00000000</v>
       </c>
       <c r="AL2" s="9">
@@ -1906,15 +1977,15 @@
         <v>0</v>
       </c>
       <c r="AM2" s="13">
-        <f t="shared" ref="AM2:AM17" si="4">IF(AU2="A",ROUND(W2*X2,2),ROUND(W2*X2/(1+X2),2))</f>
+        <f t="shared" ref="AM2:AM17" si="6">IF(AU2="A",ROUND(W2*X2,2),ROUND(W2*X2/(1+X2),2))</f>
         <v>27942.15</v>
       </c>
       <c r="AN2" s="13">
-        <f t="shared" ref="AN2:AN17" si="5">IF(AU2="A",ROUND(W2+AM2,2),ROUND(W2,2))</f>
+        <f t="shared" ref="AN2:AN17" si="7">IF(AU2="A",ROUND(W2+AM2,2),ROUND(W2,2))</f>
         <v>160999.99</v>
       </c>
       <c r="AO2" s="10" t="str">
-        <f>IF(RIGHT(K2,1)="A",SUBSTITUTE(TEXT(W2,"0,00"),",","."),SUBSTITUTE(TEXT(AN2,"0,00"),",","."))</f>
+        <f t="shared" ref="AO2:AO17" si="8">IF(RIGHT(K2,1)="A",SUBSTITUTE(TEXT(W2,"0,00"),",","."),SUBSTITUTE(TEXT(AN2,"0,00"),",","."))</f>
         <v>133057.84</v>
       </c>
       <c r="AP2" s="10" t="str">
@@ -1922,53 +1993,53 @@
         <v>0.01</v>
       </c>
       <c r="AQ2" s="1">
-        <f t="shared" ref="AQ2:AQ17" si="6">ROW(P2)</f>
+        <f t="shared" ref="AQ2:AQ17" si="9">ROW(P2)</f>
         <v>2</v>
       </c>
       <c r="AR2" s="15" t="str">
-        <f>O2&amp;"-"&amp;AQ2</f>
+        <f t="shared" ref="AR2:AR17" si="10">O2&amp;"-"&amp;AQ2</f>
         <v>30525390086-2</v>
       </c>
       <c r="AS2" s="1">
-        <f>COUNTIFS(J1:J2,J2,K1:K2,K2,P1:P2,P2)-1</f>
+        <f t="shared" ref="AS2:AS17" si="11">COUNTIFS(J1:J2,J2,K1:K2,K2,P1:P2,P2)-1</f>
         <v>0</v>
       </c>
       <c r="AT2" s="1">
-        <f ca="1">IF(F3="",0,COUNTIFS(J2:J3,J3,K2:K3,K3,P2:P3,P3)-1)</f>
+        <f t="shared" ref="AT2:AT17" ca="1" si="12">IF(F3="",0,COUNTIFS(J2:J3,J3,K2:K3,K3,P2:P3,P3)-1)</f>
         <v>0</v>
       </c>
       <c r="AU2" s="1" t="str">
-        <f t="shared" ref="AU2:AU17" si="7">RIGHT(K2)</f>
+        <f t="shared" ref="AU2:AU17" si="13">RIGHT(K2)</f>
         <v>A</v>
       </c>
       <c r="AV2" s="1">
-        <f>IF(LEFT(K2,4)="Nota",0,1)</f>
+        <f t="shared" ref="AV2:AV17" si="14">IF(LEFT(K2,4)="Nota",0,1)</f>
         <v>1</v>
       </c>
       <c r="AW2" s="13">
-        <f>IF(RIGHT(K2,1)="A",ROUND(V2*U2*(1+X2),2),AN2)</f>
+        <f t="shared" ref="AW2:AW17" si="15">IF(RIGHT(K2,1)="A",ROUND(V2*U2*(1+X2),2),AN2)</f>
         <v>160999.98000000001</v>
       </c>
       <c r="AX2" s="13">
-        <f t="shared" ref="AX2:AX17" si="8">ROUND((AW2/(1+X2)),2)</f>
+        <f t="shared" ref="AX2:AX17" si="16">ROUND((AW2/(1+X2)),2)</f>
         <v>133057.82999999999</v>
       </c>
       <c r="AY2" s="20">
-        <f t="shared" ref="AY2:AY17" si="9">IF(AU2="A",ROUND(AX2/V2,6),AW2/V2)</f>
+        <f t="shared" ref="AY2:AY17" si="17">IF(AU2="A",ROUND(AX2/V2,6),AW2/V2)</f>
         <v>7.003044</v>
       </c>
       <c r="AZ2" s="13">
-        <f t="shared" ref="AZ2:AZ17" si="10">IF(AU2="A",ROUND(CEILING(V2*U2*(1+X2),500),2),ROUND(CEILING(V2*U2,500),2))</f>
+        <f t="shared" ref="AZ2:AZ17" si="18">IF(AU2="A",ROUND(CEILING(V2*U2*(1+X2),500),2),ROUND(CEILING(V2*U2,500),2))</f>
         <v>161000</v>
       </c>
       <c r="BA2" s="20">
-        <f t="shared" ref="BA2:BA17" si="11">IF(AU2="A",ROUND(AX2/V2,6),AZ2/V2)</f>
+        <f t="shared" ref="BA2:BA17" si="19">IF(AU2="A",ROUND(AX2/V2,6),AZ2/V2)</f>
         <v>7.003044</v>
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
-        <f ca="1">CONCATENATE(J3," - ",O3," - ",P3," - ",S3)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 30525733870 - PRICE WATERHOUSE &amp; CO SOCIEDAD DE RESPONSABILIDAD LIMITADA - Honorarios Julio</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1985,19 +2056,19 @@
         <v>90</v>
       </c>
       <c r="F3" s="8">
-        <f t="shared" ref="F3:F17" ca="1" si="12">TODAY()</f>
+        <f t="shared" ref="F3:F17" ca="1" si="20">TODAY()</f>
         <v>45149</v>
       </c>
       <c r="G3" s="9">
-        <f t="shared" ref="G3:G17" ca="1" si="13">DATE(YEAR(H3),MONTH(H3),1)</f>
+        <f t="shared" ref="G3:G17" ca="1" si="21">DATE(YEAR(H3),MONTH(H3),1)</f>
         <v>45108</v>
       </c>
       <c r="H3" s="9">
-        <f t="shared" ref="H3:H17" ca="1" si="14">EOMONTH(F3,-1)</f>
+        <f t="shared" ref="H3:H17" ca="1" si="22">EOMONTH(F3,-1)</f>
         <v>45138</v>
       </c>
       <c r="I3" s="9">
-        <f t="shared" ref="I3:I17" ca="1" si="15">F3+14</f>
+        <f t="shared" ref="I3:I17" ca="1" si="23">F3+14</f>
         <v>45163</v>
       </c>
       <c r="J3" s="2">
@@ -2037,7 +2108,7 @@
         <v>19000</v>
       </c>
       <c r="W3" s="5">
-        <f t="shared" ref="W3:W17" si="16">U3*V3</f>
+        <f t="shared" ref="W3:W17" si="24">U3*V3</f>
         <v>152479.33199999999</v>
       </c>
       <c r="X3" s="11" t="s">
@@ -2050,7 +2121,7 @@
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1" t="str">
-        <f t="shared" ref="AE3:AE17" si="17">SUBSTITUTE(AC3,",",".")</f>
+        <f t="shared" ref="AE3:AE17" si="25">SUBSTITUTE(AC3,",",".")</f>
         <v/>
       </c>
       <c r="AF3" s="1" t="str">
@@ -2058,39 +2129,39 @@
         <v/>
       </c>
       <c r="AG3" s="14">
-        <f>COUNTIFS(J2:J3,J3,K2:K3,K3,P2:P3,P3)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH3" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.025228</v>
       </c>
       <c r="AI3" s="18" t="str">
-        <f t="shared" ref="AI3:AI17" si="18">SUBSTITUTE(TEXT(V3,"0,00"),",",".")</f>
+        <f t="shared" ref="AI3:AI17" si="26">SUBSTITUTE(TEXT(V3,"0,00"),",",".")</f>
         <v>19000.00</v>
       </c>
       <c r="AJ3" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK3" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL3" s="9">
-        <f t="shared" ref="AL3:AL17" si="19">AB3</f>
+        <f t="shared" ref="AL3:AL17" si="27">AB3</f>
         <v>0</v>
       </c>
       <c r="AM3" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32020.66</v>
       </c>
       <c r="AN3" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>184499.99</v>
       </c>
       <c r="AO3" s="10" t="str">
-        <f>IF(RIGHT(K3,1)="A",SUBSTITUTE(TEXT(W3,"0,00"),",","."),SUBSTITUTE(TEXT(AN3,"0,00"),",","."))</f>
+        <f t="shared" si="8"/>
         <v>152479.33</v>
       </c>
       <c r="AP3" s="10" t="str">
@@ -2098,53 +2169,53 @@
         <v>0.01</v>
       </c>
       <c r="AQ3" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AR3" s="15" t="str">
-        <f>O3&amp;"-"&amp;AQ3</f>
+        <f t="shared" si="10"/>
         <v>30525733870-3</v>
       </c>
       <c r="AS3" s="1">
-        <f>COUNTIFS(J2:J3,J3,K2:K3,K3,P2:P3,P3)-1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AT3" s="1">
-        <f ca="1">IF(F4="",0,COUNTIFS(J3:J4,J4,K3:K4,K4,P3:P4,P4)-1)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
       <c r="AU3" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>A</v>
       </c>
       <c r="AV3" s="1">
-        <f>IF(LEFT(K3,4)="Nota",0,1)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AW3" s="13">
-        <f>IF(RIGHT(K3,1)="A",ROUND(V3*U3*(1+X3),2),AN3)</f>
+        <f t="shared" si="15"/>
         <v>184499.99</v>
       </c>
       <c r="AX3" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>152479.32999999999</v>
       </c>
       <c r="AY3" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>8.0252280000000003</v>
       </c>
       <c r="AZ3" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>184500</v>
       </c>
       <c r="BA3" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>8.0252280000000003</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
-        <f ca="1">CONCATENATE(J4," - ",O4," - ",P4," - ",S4)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 30610252334 - ARCOS DORADOS ARGENTINA SOCIEDAD ANONIMA - Honorarios Julio</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2161,19 +2232,19 @@
         <v>90</v>
       </c>
       <c r="F4" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G4" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H4" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I4" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J4" s="2">
@@ -2213,7 +2284,7 @@
         <v>19000</v>
       </c>
       <c r="W4" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>190082.63099999999</v>
       </c>
       <c r="X4" s="11" t="s">
@@ -2226,47 +2297,47 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF4" s="1" t="str">
-        <f t="shared" ref="AF4:AF17" si="20">SUBSTITUTE(AD4,",",".")</f>
+        <f t="shared" ref="AF4:AF17" si="28">SUBSTITUTE(AD4,",",".")</f>
         <v/>
       </c>
       <c r="AG4" s="14">
-        <f>COUNTIFS(J3:J4,J4,K3:K4,K4,P3:P4,P4)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH4" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.004349</v>
       </c>
       <c r="AI4" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ4" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK4" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL4" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AM4" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>39917.35</v>
       </c>
       <c r="AN4" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>229999.98</v>
       </c>
       <c r="AO4" s="10" t="str">
-        <f>IF(RIGHT(K4,1)="A",SUBSTITUTE(TEXT(W4,"0,00"),",","."),SUBSTITUTE(TEXT(AN4,"0,00"),",","."))</f>
+        <f t="shared" si="8"/>
         <v>190082.63</v>
       </c>
       <c r="AP4" s="10" t="str">
@@ -2274,53 +2345,53 @@
         <v>0.02</v>
       </c>
       <c r="AQ4" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AR4" s="15" t="str">
-        <f>O4&amp;"-"&amp;AQ4</f>
+        <f t="shared" si="10"/>
         <v>30610252334-4</v>
       </c>
       <c r="AS4" s="1">
-        <f>COUNTIFS(J3:J4,J4,K3:K4,K4,P3:P4,P4)-1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AT4" s="1">
-        <f ca="1">IF(F5="",0,COUNTIFS(J4:J5,J5,K4:K5,K5,P4:P5,P5)-1)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
       <c r="AU4" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>A</v>
       </c>
       <c r="AV4" s="1">
-        <f>IF(LEFT(K4,4)="Nota",0,1)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AW4" s="13">
-        <f>IF(RIGHT(K4,1)="A",ROUND(V4*U4*(1+X4),2),AN4)</f>
+        <f t="shared" si="15"/>
         <v>229999.98</v>
       </c>
       <c r="AX4" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>190082.63</v>
       </c>
       <c r="AY4" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AZ4" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>230000</v>
       </c>
       <c r="BA4" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>10.004348999999999</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
-        <f ca="1">CONCATENATE(J5," - ",O5," - ",P5," - ",S5)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 30710964277 - LAKAUT S.A. - Honorarios Julio</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2337,19 +2408,19 @@
         <v>90</v>
       </c>
       <c r="F5" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G5" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H5" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I5" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J5" s="2">
@@ -2389,7 +2460,7 @@
         <v>19000</v>
       </c>
       <c r="W5" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>171487.59700000001</v>
       </c>
       <c r="X5" s="11" t="s">
@@ -2402,47 +2473,47 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF5" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG5" s="14">
-        <f>COUNTIFS(J4:J5,J5,K4:K5,K5,P4:P5,P5)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH5" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.025663</v>
       </c>
       <c r="AI5" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK5" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL5" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AM5" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>36012.400000000001</v>
       </c>
       <c r="AN5" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>207500</v>
       </c>
       <c r="AO5" s="10" t="str">
-        <f>IF(RIGHT(K5,1)="A",SUBSTITUTE(TEXT(W5,"0,00"),",","."),SUBSTITUTE(TEXT(AN5,"0,00"),",","."))</f>
+        <f t="shared" si="8"/>
         <v>171487.60</v>
       </c>
       <c r="AP5" s="10" t="str">
@@ -2450,53 +2521,53 @@
         <v>0.00</v>
       </c>
       <c r="AQ5" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AR5" s="15" t="str">
-        <f>O5&amp;"-"&amp;AQ5</f>
+        <f t="shared" si="10"/>
         <v>30710964277-5</v>
       </c>
       <c r="AS5" s="1">
-        <f>COUNTIFS(J4:J5,J5,K4:K5,K5,P4:P5,P5)-1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AT5" s="1">
-        <f ca="1">IF(F6="",0,COUNTIFS(J5:J6,J6,K5:K6,K6,P5:P6,P6)-1)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>0</v>
       </c>
       <c r="AU5" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>A</v>
       </c>
       <c r="AV5" s="1">
-        <f>IF(LEFT(K5,4)="Nota",0,1)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AW5" s="13">
-        <f>IF(RIGHT(K5,1)="A",ROUND(V5*U5*(1+X5),2),AN5)</f>
+        <f t="shared" si="15"/>
         <v>207499.99</v>
       </c>
       <c r="AX5" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>171487.6</v>
       </c>
       <c r="AY5" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>9.0256629999999998</v>
       </c>
       <c r="AZ5" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>207500</v>
       </c>
       <c r="BA5" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>9.0256629999999998</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
-        <f ca="1">CONCATENATE(J6," - ",O6," - ",P6," - ",S6)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 33610006189 - ACCENTURE SOCIEDAD DE RESPONSABILIDAD LIMITADA - Honorarios Julio</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2513,19 +2584,19 @@
         <v>90</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G6" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H6" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I6" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J6" s="2">
@@ -2565,7 +2636,7 @@
         <v>19000</v>
       </c>
       <c r="W6" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>95454.536999999997</v>
       </c>
       <c r="X6" s="11" t="s">
@@ -2586,47 +2657,47 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF6" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG6" s="14">
-        <f>COUNTIFS(J5:J6,J6,K5:K6,K6,P5:P6,P6)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH6" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.023923</v>
       </c>
       <c r="AI6" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="AK6" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000003</v>
       </c>
       <c r="AL6" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>44816</v>
       </c>
       <c r="AM6" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>20045.45</v>
       </c>
       <c r="AN6" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>115499.99</v>
       </c>
       <c r="AO6" s="10" t="str">
-        <f>IF(RIGHT(K6,1)="A",SUBSTITUTE(TEXT(W6,"0,00"),",","."),SUBSTITUTE(TEXT(AN6,"0,00"),",","."))</f>
+        <f t="shared" si="8"/>
         <v>95454.54</v>
       </c>
       <c r="AP6" s="10" t="str">
@@ -2634,53 +2705,53 @@
         <v>0.01</v>
       </c>
       <c r="AQ6" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AR6" s="15" t="str">
-        <f>O6&amp;"-"&amp;AQ6</f>
+        <f t="shared" si="10"/>
         <v>33610006189-6</v>
       </c>
       <c r="AS6" s="1">
-        <f>COUNTIFS(J5:J6,J6,K5:K6,K6,P5:P6,P6)-1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AT6" s="1">
-        <f ca="1">IF(F7="",0,COUNTIFS(J6:J7,J7,K6:K7,K7,P6:P7,P7)-1)</f>
+        <f t="shared" ca="1" si="12"/>
         <v>1</v>
       </c>
       <c r="AU6" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>A</v>
       </c>
       <c r="AV6" s="1">
-        <f>IF(LEFT(K6,4)="Nota",0,1)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="AW6" s="13">
-        <f>IF(RIGHT(K6,1)="A",ROUND(V6*U6*(1+X6),2),AN6)</f>
+        <f t="shared" si="15"/>
         <v>115499.99</v>
       </c>
       <c r="AX6" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>95454.54</v>
       </c>
       <c r="AY6" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>5.0239229999999999</v>
       </c>
       <c r="AZ6" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>115500</v>
       </c>
       <c r="BA6" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>5.0239229999999999</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
-        <f>CONCATENATE(J7," - ",O7," - ",P7," - ",S7)</f>
+        <f t="shared" si="0"/>
         <v>2 - 33610006189 - ACCENTURE SOCIEDAD DE RESPONSABILIDAD LIMITADA - Horas extra</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2697,19 +2768,19 @@
         <v>90</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G7" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H7" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I7" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J7" s="2">
@@ -2748,7 +2819,7 @@
         <v>19000</v>
       </c>
       <c r="W7" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>95041.305999999997</v>
       </c>
       <c r="X7" s="11" t="s">
@@ -2761,101 +2832,101 @@
       <c r="AC7" s="2"/>
       <c r="AD7" s="2"/>
       <c r="AE7" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF7" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG7" s="14">
-        <f>COUNTIFS(J6:J7,J7,K6:K7,K7,P6:P7,P7)+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AH7" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.002174</v>
       </c>
       <c r="AI7" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK7" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL7" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AM7" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>19958.669999999998</v>
       </c>
       <c r="AN7" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>114999.98</v>
       </c>
       <c r="AO7" s="10" t="str">
-        <f>IF(RIGHT(K7,1)="A",SUBSTITUTE(TEXT(W7,"0,00"),",","."),SUBSTITUTE(TEXT(AN7,"0,00"),",","."))</f>
-        <v>95041.31</v>
-      </c>
-      <c r="AP7" s="10" t="str">
-        <f t="shared" ref="AP7:AP17" si="21">SUBSTITUTE(TEXT(ROUNDUP(AN7,0)-AN7,"0,00"),",",".")</f>
-        <v>0.02</v>
-      </c>
-      <c r="AQ7" s="1">
-        <f t="shared" si="6"/>
-        <v>7</v>
-      </c>
-      <c r="AR7" s="15" t="str">
-        <f>O7&amp;"-"&amp;AQ7</f>
-        <v>33610006189-7</v>
-      </c>
-      <c r="AS7" s="1">
-        <f>COUNTIFS(J6:J7,J7,K6:K7,K7,P6:P7,P7)-1</f>
-        <v>1</v>
-      </c>
-      <c r="AT7" s="1">
-        <f ca="1">IF(F8="",0,COUNTIFS(J7:J8,J8,K7:K8,K8,P7:P8,P8)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU7" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>A</v>
-      </c>
-      <c r="AV7" s="1">
-        <f>IF(LEFT(K7,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW7" s="13">
-        <f>IF(RIGHT(K7,1)="A",ROUND(V7*U7*(1+X7),2),AN7)</f>
-        <v>114999.98</v>
-      </c>
-      <c r="AX7" s="13">
         <f t="shared" si="8"/>
         <v>95041.31</v>
       </c>
+      <c r="AP7" s="10" t="str">
+        <f t="shared" ref="AP7:AP17" si="29">SUBSTITUTE(TEXT(ROUNDUP(AN7,0)-AN7,"0,00"),",",".")</f>
+        <v>0.02</v>
+      </c>
+      <c r="AQ7" s="1">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="AR7" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>33610006189-7</v>
+      </c>
+      <c r="AS7" s="1">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AT7" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU7" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>A</v>
+      </c>
+      <c r="AV7" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW7" s="13">
+        <f t="shared" si="15"/>
+        <v>114999.98</v>
+      </c>
+      <c r="AX7" s="13">
+        <f t="shared" si="16"/>
+        <v>95041.31</v>
+      </c>
       <c r="AY7" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>5.0021740000000001</v>
       </c>
       <c r="AZ7" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>115000</v>
       </c>
       <c r="BA7" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>5.0021740000000001</v>
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
-        <f ca="1">CONCATENATE(J8," - ",O8," - ",P8," - ",S8)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 33615420269 - AUSTRAL LINEAS AEREAS CIELOS DEL SUR S A - Honorarios Julio</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2872,19 +2943,19 @@
         <v>90</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H8" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I8" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J8" s="2">
@@ -2913,7 +2984,7 @@
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(G8,"mmmm"))</f>
+        <f t="shared" ref="S8:S13" ca="1" si="30">"Honorarios "&amp;PROPER(TEXT(G8,"mmmm"))</f>
         <v>Honorarios Julio</v>
       </c>
       <c r="T8" s="2"/>
@@ -2924,7 +2995,7 @@
         <v>19000</v>
       </c>
       <c r="W8" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>190082.63099999999</v>
       </c>
       <c r="X8" s="11" t="s">
@@ -2937,101 +3008,101 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="2"/>
       <c r="AE8" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF8" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG8" s="14">
-        <f>COUNTIFS(J7:J8,J8,K7:K8,K8,P7:P8,P8)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH8" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10.004349</v>
       </c>
       <c r="AI8" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK8" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL8" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AM8" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>39917.35</v>
       </c>
       <c r="AN8" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>229999.98</v>
       </c>
       <c r="AO8" s="10" t="str">
-        <f>IF(RIGHT(K8,1)="A",SUBSTITUTE(TEXT(W8,"0,00"),",","."),SUBSTITUTE(TEXT(AN8,"0,00"),",","."))</f>
-        <v>190082.63</v>
-      </c>
-      <c r="AP8" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.02</v>
-      </c>
-      <c r="AQ8" s="1">
-        <f t="shared" si="6"/>
-        <v>8</v>
-      </c>
-      <c r="AR8" s="15" t="str">
-        <f>O8&amp;"-"&amp;AQ8</f>
-        <v>33615420269-8</v>
-      </c>
-      <c r="AS8" s="1">
-        <f>COUNTIFS(J7:J8,J8,K7:K8,K8,P7:P8,P8)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT8" s="1">
-        <f ca="1">IF(F9="",0,COUNTIFS(J8:J9,J9,K8:K9,K9,P8:P9,P9)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU8" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>A</v>
-      </c>
-      <c r="AV8" s="1">
-        <f>IF(LEFT(K8,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW8" s="13">
-        <f>IF(RIGHT(K8,1)="A",ROUND(V8*U8*(1+X8),2),AN8)</f>
-        <v>229999.98</v>
-      </c>
-      <c r="AX8" s="13">
         <f t="shared" si="8"/>
         <v>190082.63</v>
       </c>
+      <c r="AP8" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.02</v>
+      </c>
+      <c r="AQ8" s="1">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="AR8" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>33615420269-8</v>
+      </c>
+      <c r="AS8" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT8" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>A</v>
+      </c>
+      <c r="AV8" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW8" s="13">
+        <f t="shared" si="15"/>
+        <v>229999.98</v>
+      </c>
+      <c r="AX8" s="13">
+        <f t="shared" si="16"/>
+        <v>190082.63</v>
+      </c>
       <c r="AY8" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>10.004348999999999</v>
       </c>
       <c r="AZ8" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>230000</v>
       </c>
       <c r="BA8" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>10.004348999999999</v>
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
-        <f ca="1">CONCATENATE(J9," - ",O9," - ",P9," - ",S9)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 20147130202 - BUSTOS JOSE MARTIN - Honorarios Julio</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -3048,19 +3119,19 @@
         <v>90</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H9" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I9" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J9" s="2">
@@ -3089,7 +3160,7 @@
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(G9,"mmmm"))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="T9" s="2"/>
@@ -3100,7 +3171,7 @@
         <v>19000</v>
       </c>
       <c r="W9" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>19421.477000000003</v>
       </c>
       <c r="X9" s="11" t="s">
@@ -3113,101 +3184,101 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
       <c r="AE9" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF9" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG9" s="14">
-        <f>COUNTIFS(J8:J9,J9,K8:K9,K9,P8:P9,P9)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH9" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.022183</v>
       </c>
       <c r="AI9" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK9" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL9" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AM9" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4078.51</v>
       </c>
       <c r="AN9" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>23499.99</v>
       </c>
       <c r="AO9" s="10" t="str">
-        <f>IF(RIGHT(K9,1)="A",SUBSTITUTE(TEXT(W9,"0,00"),",","."),SUBSTITUTE(TEXT(AN9,"0,00"),",","."))</f>
-        <v>19421.48</v>
-      </c>
-      <c r="AP9" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.01</v>
-      </c>
-      <c r="AQ9" s="1">
-        <f t="shared" si="6"/>
-        <v>9</v>
-      </c>
-      <c r="AR9" s="15" t="str">
-        <f>O9&amp;"-"&amp;AQ9</f>
-        <v>20147130202-9</v>
-      </c>
-      <c r="AS9" s="1">
-        <f>COUNTIFS(J8:J9,J9,K8:K9,K9,P8:P9,P9)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT9" s="1">
-        <f ca="1">IF(F10="",0,COUNTIFS(J9:J10,J10,K9:K10,K10,P9:P10,P10)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU9" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>A</v>
-      </c>
-      <c r="AV9" s="1">
-        <f>IF(LEFT(K9,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW9" s="13">
-        <f>IF(RIGHT(K9,1)="A",ROUND(V9*U9*(1+X9),2),AN9)</f>
-        <v>23499.99</v>
-      </c>
-      <c r="AX9" s="13">
         <f t="shared" si="8"/>
         <v>19421.48</v>
       </c>
+      <c r="AP9" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.01</v>
+      </c>
+      <c r="AQ9" s="1">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="AR9" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>20147130202-9</v>
+      </c>
+      <c r="AS9" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT9" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>A</v>
+      </c>
+      <c r="AV9" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW9" s="13">
+        <f t="shared" si="15"/>
+        <v>23499.99</v>
+      </c>
+      <c r="AX9" s="13">
+        <f t="shared" si="16"/>
+        <v>19421.48</v>
+      </c>
       <c r="AY9" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>1.0221830000000001</v>
       </c>
       <c r="AZ9" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>23500</v>
       </c>
       <c r="BA9" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1.0221830000000001</v>
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
-        <f ca="1">CONCATENATE(J10," - ",O10," - ",P10," - ",S10)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 20374730429 - BUSTOS PIASENTINI AGUSTIN - Honorarios Julio</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3224,19 +3295,19 @@
         <v>90</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H10" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I10" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J10" s="2">
@@ -3265,7 +3336,7 @@
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(G10,"mmmm"))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="T10" s="2"/>
@@ -3276,7 +3347,7 @@
         <v>19000</v>
       </c>
       <c r="W10" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>19834.708000000002</v>
       </c>
       <c r="X10" s="11" t="s">
@@ -3289,101 +3360,101 @@
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF10" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG10" s="14">
-        <f>COUNTIFS(J9:J10,J10,K9:K10,K10,P9:P10,P10)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH10" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.043932</v>
       </c>
       <c r="AI10" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ10" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00000</v>
       </c>
       <c r="AK10" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000000</v>
       </c>
       <c r="AL10" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AM10" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4165.29</v>
       </c>
       <c r="AN10" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>24000</v>
       </c>
       <c r="AO10" s="10" t="str">
-        <f>IF(RIGHT(K10,1)="A",SUBSTITUTE(TEXT(W10,"0,00"),",","."),SUBSTITUTE(TEXT(AN10,"0,00"),",","."))</f>
-        <v>19834.71</v>
-      </c>
-      <c r="AP10" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.00</v>
-      </c>
-      <c r="AQ10" s="1">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="AR10" s="15" t="str">
-        <f>O10&amp;"-"&amp;AQ10</f>
-        <v>20374730429-10</v>
-      </c>
-      <c r="AS10" s="1">
-        <f>COUNTIFS(J9:J10,J10,K9:K10,K10,P9:P10,P10)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT10" s="1">
-        <f ca="1">IF(F11="",0,COUNTIFS(J10:J11,J11,K10:K11,K11,P10:P11,P11)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU10" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>A</v>
-      </c>
-      <c r="AV10" s="1">
-        <f>IF(LEFT(K10,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW10" s="13">
-        <f>IF(RIGHT(K10,1)="A",ROUND(V10*U10*(1+X10),2),AN10)</f>
-        <v>24000</v>
-      </c>
-      <c r="AX10" s="13">
         <f t="shared" si="8"/>
         <v>19834.71</v>
       </c>
+      <c r="AP10" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.00</v>
+      </c>
+      <c r="AQ10" s="1">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="AR10" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>20374730429-10</v>
+      </c>
+      <c r="AS10" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT10" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>A</v>
+      </c>
+      <c r="AV10" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW10" s="13">
+        <f t="shared" si="15"/>
+        <v>24000</v>
+      </c>
+      <c r="AX10" s="13">
+        <f t="shared" si="16"/>
+        <v>19834.71</v>
+      </c>
       <c r="AY10" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>1.0439320000000001</v>
       </c>
       <c r="AZ10" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>24000</v>
       </c>
       <c r="BA10" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1.0439320000000001</v>
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
-        <f ca="1">CONCATENATE(J11," - ",O11," - ",P11," - ",S11)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 37473042 - BUSTOS PIASENTINI AGUSTIN - Honorarios Julio</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -3398,19 +3469,19 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G11" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H11" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I11" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J11" s="2">
@@ -3439,7 +3510,7 @@
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(G11,"mmmm"))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="T11" s="2"/>
@@ -3450,7 +3521,7 @@
         <v>10000</v>
       </c>
       <c r="W11" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>13000</v>
       </c>
       <c r="X11" s="11" t="s">
@@ -3463,101 +3534,101 @@
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="AF11" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AG11" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AH11" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>1.3</v>
+      </c>
+      <c r="AI11" s="18" t="str">
+        <f t="shared" si="26"/>
+        <v>10000.00</v>
+      </c>
+      <c r="AJ11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="AK11" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="AL11" s="9">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AM11" s="13">
+        <f t="shared" si="6"/>
+        <v>2256.1999999999998</v>
+      </c>
+      <c r="AN11" s="13">
+        <f t="shared" si="7"/>
+        <v>13000</v>
+      </c>
+      <c r="AO11" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>13000.00</v>
+      </c>
+      <c r="AP11" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.00</v>
+      </c>
+      <c r="AQ11" s="1">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="AR11" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>37473042-11</v>
+      </c>
+      <c r="AS11" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT11" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU11" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>B</v>
+      </c>
+      <c r="AV11" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW11" s="13">
+        <f t="shared" si="15"/>
+        <v>13000</v>
+      </c>
+      <c r="AX11" s="13">
+        <f t="shared" si="16"/>
+        <v>10743.8</v>
+      </c>
+      <c r="AY11" s="20">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AF11" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AG11" s="14">
-        <f>COUNTIFS(J10:J11,J11,K10:K11,K11,P10:P11,P11)+1</f>
-        <v>2</v>
-      </c>
-      <c r="AH11" s="18" t="str">
-        <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
-      <c r="AI11" s="18" t="str">
+      <c r="AZ11" s="13">
         <f t="shared" si="18"/>
-        <v>10000.00</v>
-      </c>
-      <c r="AJ11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000</v>
-      </c>
-      <c r="AK11" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>00000000</v>
-      </c>
-      <c r="AL11" s="9">
+        <v>13000</v>
+      </c>
+      <c r="BA11" s="20">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AM11" s="13">
-        <f t="shared" si="4"/>
-        <v>2256.1999999999998</v>
-      </c>
-      <c r="AN11" s="13">
-        <f t="shared" si="5"/>
-        <v>13000</v>
-      </c>
-      <c r="AO11" s="10" t="str">
-        <f>IF(RIGHT(K11,1)="A",SUBSTITUTE(TEXT(W11,"0,00"),",","."),SUBSTITUTE(TEXT(AN11,"0,00"),",","."))</f>
-        <v>13000.00</v>
-      </c>
-      <c r="AP11" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.00</v>
-      </c>
-      <c r="AQ11" s="1">
-        <f t="shared" si="6"/>
-        <v>11</v>
-      </c>
-      <c r="AR11" s="15" t="str">
-        <f>O11&amp;"-"&amp;AQ11</f>
-        <v>37473042-11</v>
-      </c>
-      <c r="AS11" s="1">
-        <f>COUNTIFS(J10:J11,J11,K10:K11,K11,P10:P11,P11)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT11" s="1">
-        <f ca="1">IF(F12="",0,COUNTIFS(J11:J12,J12,K11:K12,K12,P11:P12,P12)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU11" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>B</v>
-      </c>
-      <c r="AV11" s="1">
-        <f>IF(LEFT(K11,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW11" s="13">
-        <f>IF(RIGHT(K11,1)="A",ROUND(V11*U11*(1+X11),2),AN11)</f>
-        <v>13000</v>
-      </c>
-      <c r="AX11" s="13">
-        <f t="shared" si="8"/>
-        <v>10743.8</v>
-      </c>
-      <c r="AY11" s="20">
-        <f t="shared" si="9"/>
-        <v>1.3</v>
-      </c>
-      <c r="AZ11" s="13">
-        <f t="shared" si="10"/>
-        <v>13000</v>
-      </c>
-      <c r="BA11" s="20">
-        <f t="shared" si="11"/>
         <v>1.3</v>
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
-        <f ca="1">CONCATENATE(J12," - ",O12," - ",P12," - ",S12)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>2 - 30707354719 - CAMARA DE ELABORADORES DE TE ARGENTINO C. E. T.A. - Honorarios Julio</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3572,19 +3643,19 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G12" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H12" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I12" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J12" s="2">
@@ -3613,7 +3684,7 @@
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(G12,"mmmm"))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="T12" s="2"/>
@@ -3624,7 +3695,7 @@
         <v>19000</v>
       </c>
       <c r="W12" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>23000</v>
       </c>
       <c r="X12" s="11" t="s">
@@ -3637,101 +3708,101 @@
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="AF12" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AG12" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AH12" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>1.210526</v>
+      </c>
+      <c r="AI12" s="18" t="str">
+        <f t="shared" si="26"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AJ12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="AK12" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="AL12" s="9">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AM12" s="13">
+        <f t="shared" si="6"/>
+        <v>3991.74</v>
+      </c>
+      <c r="AN12" s="13">
+        <f t="shared" si="7"/>
+        <v>23000</v>
+      </c>
+      <c r="AO12" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>23000.00</v>
+      </c>
+      <c r="AP12" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.00</v>
+      </c>
+      <c r="AQ12" s="1">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="AR12" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>30707354719-12</v>
+      </c>
+      <c r="AS12" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT12" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU12" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>B</v>
+      </c>
+      <c r="AV12" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW12" s="13">
+        <f t="shared" si="15"/>
+        <v>23000</v>
+      </c>
+      <c r="AX12" s="13">
+        <f t="shared" si="16"/>
+        <v>19008.259999999998</v>
+      </c>
+      <c r="AY12" s="20">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AF12" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AG12" s="14">
-        <f>COUNTIFS(J11:J12,J12,K11:K12,K12,P11:P12,P12)+1</f>
-        <v>2</v>
-      </c>
-      <c r="AH12" s="18" t="str">
-        <f t="shared" si="1"/>
-        <v>1.210526</v>
-      </c>
-      <c r="AI12" s="18" t="str">
+        <v>1.2105263157894737</v>
+      </c>
+      <c r="AZ12" s="13">
         <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="AJ12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000</v>
-      </c>
-      <c r="AK12" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>00000000</v>
-      </c>
-      <c r="AL12" s="9">
+        <v>23000</v>
+      </c>
+      <c r="BA12" s="20">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AM12" s="13">
-        <f t="shared" si="4"/>
-        <v>3991.74</v>
-      </c>
-      <c r="AN12" s="13">
-        <f t="shared" si="5"/>
-        <v>23000</v>
-      </c>
-      <c r="AO12" s="10" t="str">
-        <f>IF(RIGHT(K12,1)="A",SUBSTITUTE(TEXT(W12,"0,00"),",","."),SUBSTITUTE(TEXT(AN12,"0,00"),",","."))</f>
-        <v>23000.00</v>
-      </c>
-      <c r="AP12" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.00</v>
-      </c>
-      <c r="AQ12" s="1">
-        <f t="shared" si="6"/>
-        <v>12</v>
-      </c>
-      <c r="AR12" s="15" t="str">
-        <f>O12&amp;"-"&amp;AQ12</f>
-        <v>30707354719-12</v>
-      </c>
-      <c r="AS12" s="1">
-        <f>COUNTIFS(J11:J12,J12,K11:K12,K12,P11:P12,P12)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT12" s="1">
-        <f ca="1">IF(F13="",0,COUNTIFS(J12:J13,J13,K12:K13,K13,P12:P13,P13)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU12" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>B</v>
-      </c>
-      <c r="AV12" s="1">
-        <f>IF(LEFT(K12,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW12" s="13">
-        <f>IF(RIGHT(K12,1)="A",ROUND(V12*U12*(1+X12),2),AN12)</f>
-        <v>23000</v>
-      </c>
-      <c r="AX12" s="13">
-        <f t="shared" si="8"/>
-        <v>19008.259999999998</v>
-      </c>
-      <c r="AY12" s="20">
-        <f t="shared" si="9"/>
-        <v>1.2105263157894737</v>
-      </c>
-      <c r="AZ12" s="13">
-        <f t="shared" si="10"/>
-        <v>23000</v>
-      </c>
-      <c r="BA12" s="20">
-        <f t="shared" si="11"/>
         <v>1.2105263157894737</v>
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="str">
-        <f ca="1">CONCATENATE(J13," - ",O13," - ",P13," - ",S13)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>1 -  - MARTIN BUSTOS - Honorarios Julio</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3746,19 +3817,19 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G13" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H13" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I13" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J13" s="2">
@@ -3785,7 +3856,7 @@
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="1" t="str">
-        <f ca="1">"Honorarios "&amp;PROPER(TEXT(G13,"mmmm"))</f>
+        <f t="shared" ca="1" si="30"/>
         <v>Honorarios Julio</v>
       </c>
       <c r="T13" s="2"/>
@@ -3796,7 +3867,7 @@
         <v>19000</v>
       </c>
       <c r="W13" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>28500</v>
       </c>
       <c r="X13" s="11"/>
@@ -3807,101 +3878,101 @@
       <c r="AC13" s="2"/>
       <c r="AD13" s="2"/>
       <c r="AE13" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="AF13" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AG13" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AH13" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="AI13" s="18" t="str">
+        <f t="shared" si="26"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AJ13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>00000</v>
+      </c>
+      <c r="AK13" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>00000000</v>
+      </c>
+      <c r="AL13" s="9">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AM13" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AN13" s="13">
+        <f t="shared" si="7"/>
+        <v>28500</v>
+      </c>
+      <c r="AO13" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>28500.00</v>
+      </c>
+      <c r="AP13" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.00</v>
+      </c>
+      <c r="AQ13" s="1">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="AR13" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>-13</v>
+      </c>
+      <c r="AS13" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT13" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>C</v>
+      </c>
+      <c r="AV13" s="1">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AW13" s="13">
+        <f t="shared" si="15"/>
+        <v>28500</v>
+      </c>
+      <c r="AX13" s="13">
+        <f t="shared" si="16"/>
+        <v>28500</v>
+      </c>
+      <c r="AY13" s="20">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AF13" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AG13" s="14">
-        <f>COUNTIFS(J12:J13,J13,K12:K13,K13,P12:P13,P13)+1</f>
-        <v>2</v>
-      </c>
-      <c r="AH13" s="18" t="str">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="AI13" s="18" t="str">
+      <c r="AZ13" s="13">
         <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="AJ13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00000</v>
-      </c>
-      <c r="AK13" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>00000000</v>
-      </c>
-      <c r="AL13" s="9">
+        <v>28500</v>
+      </c>
+      <c r="BA13" s="20">
         <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="AM13" s="13">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AN13" s="13">
-        <f t="shared" si="5"/>
-        <v>28500</v>
-      </c>
-      <c r="AO13" s="10" t="str">
-        <f>IF(RIGHT(K13,1)="A",SUBSTITUTE(TEXT(W13,"0,00"),",","."),SUBSTITUTE(TEXT(AN13,"0,00"),",","."))</f>
-        <v>28500.00</v>
-      </c>
-      <c r="AP13" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.00</v>
-      </c>
-      <c r="AQ13" s="1">
-        <f t="shared" si="6"/>
-        <v>13</v>
-      </c>
-      <c r="AR13" s="15" t="str">
-        <f>O13&amp;"-"&amp;AQ13</f>
-        <v>-13</v>
-      </c>
-      <c r="AS13" s="1">
-        <f>COUNTIFS(J12:J13,J13,K12:K13,K13,P12:P13,P13)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT13" s="1">
-        <f ca="1">IF(F14="",0,COUNTIFS(J13:J14,J14,K13:K14,K14,P13:P14,P14)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU13" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>C</v>
-      </c>
-      <c r="AV13" s="1">
-        <f>IF(LEFT(K13,4)="Nota",0,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AW13" s="13">
-        <f>IF(RIGHT(K13,1)="A",ROUND(V13*U13*(1+X13),2),AN13)</f>
-        <v>28500</v>
-      </c>
-      <c r="AX13" s="13">
-        <f t="shared" si="8"/>
-        <v>28500</v>
-      </c>
-      <c r="AY13" s="20">
-        <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="AZ13" s="13">
-        <f t="shared" si="10"/>
-        <v>28500</v>
-      </c>
-      <c r="BA13" s="20">
-        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
-        <f>CONCATENATE(J14," - ",O14," - ",P14," - ",S14)</f>
+        <f t="shared" si="0"/>
         <v>2 - 30684125792 - SAMSUNG ELECTRONICS ARGENTINA S A - Ajuste Honorarios</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -3916,19 +3987,19 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G14" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H14" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I14" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J14" s="2">
@@ -3967,7 +4038,7 @@
         <v>19000</v>
       </c>
       <c r="W14" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>133471.06700000001</v>
       </c>
       <c r="X14" s="11" t="s">
@@ -3988,101 +4059,101 @@
       <c r="AC14" s="2"/>
       <c r="AD14" s="2"/>
       <c r="AE14" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AF14" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="AG14" s="14">
-        <f>COUNTIFS(J13:J14,J14,K13:K14,K14,P13:P14,P14)+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AH14" s="18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.024793</v>
       </c>
       <c r="AI14" s="18" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>19000.00</v>
       </c>
       <c r="AJ14" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>00002</v>
       </c>
       <c r="AK14" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>00000150</v>
       </c>
       <c r="AL14" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="27"/>
         <v>44816</v>
       </c>
       <c r="AM14" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>28028.92</v>
       </c>
       <c r="AN14" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>161499.99</v>
       </c>
       <c r="AO14" s="10" t="str">
-        <f>IF(RIGHT(K14,1)="A",SUBSTITUTE(TEXT(W14,"0,00"),",","."),SUBSTITUTE(TEXT(AN14,"0,00"),",","."))</f>
-        <v>133471.07</v>
-      </c>
-      <c r="AP14" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.01</v>
-      </c>
-      <c r="AQ14" s="1">
-        <f t="shared" si="6"/>
-        <v>14</v>
-      </c>
-      <c r="AR14" s="15" t="str">
-        <f>O14&amp;"-"&amp;AQ14</f>
-        <v>30684125792-14</v>
-      </c>
-      <c r="AS14" s="1">
-        <f>COUNTIFS(J13:J14,J14,K13:K14,K14,P13:P14,P14)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT14" s="1">
-        <f ca="1">IF(F15="",0,COUNTIFS(J14:J15,J15,K14:K15,K15,P14:P15,P15)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU14" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>A</v>
-      </c>
-      <c r="AV14" s="1">
-        <f>IF(LEFT(K14,4)="Nota",0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AW14" s="13">
-        <f>IF(RIGHT(K14,1)="A",ROUND(V14*U14*(1+X14),2),AN14)</f>
-        <v>161499.99</v>
-      </c>
-      <c r="AX14" s="13">
         <f t="shared" si="8"/>
         <v>133471.07</v>
       </c>
+      <c r="AP14" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.01</v>
+      </c>
+      <c r="AQ14" s="1">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="AR14" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>30684125792-14</v>
+      </c>
+      <c r="AS14" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT14" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>A</v>
+      </c>
+      <c r="AV14" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AW14" s="13">
+        <f t="shared" si="15"/>
+        <v>161499.99</v>
+      </c>
+      <c r="AX14" s="13">
+        <f t="shared" si="16"/>
+        <v>133471.07</v>
+      </c>
       <c r="AY14" s="20">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>7.0247929999999998</v>
       </c>
       <c r="AZ14" s="13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>161500</v>
       </c>
       <c r="BA14" s="20">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>7.0247929999999998</v>
       </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
-        <f>CONCATENATE(J15," - ",O15," - ",P15," - ",S15)</f>
+        <f t="shared" si="0"/>
         <v>2 - 30707354719 - CAMARA DE ELABORADORES DE TE ARGENTINO C. E. T.A. - Ajuste</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -4097,19 +4168,19 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G15" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H15" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I15" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J15" s="2">
@@ -4148,7 +4219,7 @@
         <v>19000</v>
       </c>
       <c r="W15" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>28500</v>
       </c>
       <c r="X15" s="11" t="s">
@@ -4169,101 +4240,101 @@
       <c r="AC15" s="2"/>
       <c r="AD15" s="2"/>
       <c r="AE15" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="AF15" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AG15" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AH15" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="AI15" s="18" t="str">
+        <f t="shared" si="26"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AJ15" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>00002</v>
+      </c>
+      <c r="AK15" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>00000152</v>
+      </c>
+      <c r="AL15" s="9">
+        <f t="shared" si="27"/>
+        <v>44816</v>
+      </c>
+      <c r="AM15" s="13">
+        <f t="shared" si="6"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AN15" s="13">
+        <f t="shared" si="7"/>
+        <v>28500</v>
+      </c>
+      <c r="AO15" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>28500.00</v>
+      </c>
+      <c r="AP15" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.00</v>
+      </c>
+      <c r="AQ15" s="1">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="AR15" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>30707354719-15</v>
+      </c>
+      <c r="AS15" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT15" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU15" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>B</v>
+      </c>
+      <c r="AV15" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AW15" s="13">
+        <f t="shared" si="15"/>
+        <v>28500</v>
+      </c>
+      <c r="AX15" s="13">
+        <f t="shared" si="16"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AY15" s="20">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AF15" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AG15" s="14">
-        <f>COUNTIFS(J14:J15,J15,K14:K15,K15,P14:P15,P15)+1</f>
-        <v>2</v>
-      </c>
-      <c r="AH15" s="18" t="str">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="AI15" s="18" t="str">
+      <c r="AZ15" s="13">
         <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="AJ15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00002</v>
-      </c>
-      <c r="AK15" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>00000152</v>
-      </c>
-      <c r="AL15" s="9">
+        <v>28500</v>
+      </c>
+      <c r="BA15" s="20">
         <f t="shared" si="19"/>
-        <v>44816</v>
-      </c>
-      <c r="AM15" s="13">
-        <f t="shared" si="4"/>
-        <v>4946.28</v>
-      </c>
-      <c r="AN15" s="13">
-        <f t="shared" si="5"/>
-        <v>28500</v>
-      </c>
-      <c r="AO15" s="10" t="str">
-        <f>IF(RIGHT(K15,1)="A",SUBSTITUTE(TEXT(W15,"0,00"),",","."),SUBSTITUTE(TEXT(AN15,"0,00"),",","."))</f>
-        <v>28500.00</v>
-      </c>
-      <c r="AP15" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.00</v>
-      </c>
-      <c r="AQ15" s="1">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="AR15" s="15" t="str">
-        <f>O15&amp;"-"&amp;AQ15</f>
-        <v>30707354719-15</v>
-      </c>
-      <c r="AS15" s="1">
-        <f>COUNTIFS(J14:J15,J15,K14:K15,K15,P14:P15,P15)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT15" s="1">
-        <f ca="1">IF(F16="",0,COUNTIFS(J15:J16,J16,K15:K16,K16,P15:P16,P16)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU15" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>B</v>
-      </c>
-      <c r="AV15" s="1">
-        <f>IF(LEFT(K15,4)="Nota",0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AW15" s="13">
-        <f>IF(RIGHT(K15,1)="A",ROUND(V15*U15*(1+X15),2),AN15)</f>
-        <v>28500</v>
-      </c>
-      <c r="AX15" s="13">
-        <f t="shared" si="8"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AY15" s="20">
-        <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="AZ15" s="13">
-        <f t="shared" si="10"/>
-        <v>28500</v>
-      </c>
-      <c r="BA15" s="20">
-        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
-        <f>CONCATENATE(J16," - ",O16," - ",P16," - ",S16)</f>
+        <f t="shared" si="0"/>
         <v>2 - 30684125792 - SAMSUNG ELECTRONICS ARGENTINA S A - Ajuste Honorarios</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -4278,19 +4349,19 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G16" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H16" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I16" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J16" s="2">
@@ -4329,7 +4400,7 @@
         <v>19000</v>
       </c>
       <c r="W16" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>133057.83600000001</v>
       </c>
       <c r="X16" s="11" t="s">
@@ -4350,101 +4421,101 @@
       <c r="AC16" s="2"/>
       <c r="AD16" s="2"/>
       <c r="AE16" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="AF16" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AG16" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AH16" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>7.003044</v>
+      </c>
+      <c r="AI16" s="18" t="str">
+        <f t="shared" si="26"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AJ16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>00002</v>
+      </c>
+      <c r="AK16" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>00000151</v>
+      </c>
+      <c r="AL16" s="9">
+        <f t="shared" si="27"/>
+        <v>44816</v>
+      </c>
+      <c r="AM16" s="13">
+        <f t="shared" si="6"/>
+        <v>27942.15</v>
+      </c>
+      <c r="AN16" s="13">
+        <f t="shared" si="7"/>
+        <v>160999.99</v>
+      </c>
+      <c r="AO16" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>133057.84</v>
+      </c>
+      <c r="AP16" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.01</v>
+      </c>
+      <c r="AQ16" s="1">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="AR16" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>30684125792-16</v>
+      </c>
+      <c r="AS16" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT16" s="1">
+        <f t="shared" ca="1" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU16" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>A</v>
+      </c>
+      <c r="AV16" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AW16" s="13">
+        <f t="shared" si="15"/>
+        <v>160999.98000000001</v>
+      </c>
+      <c r="AX16" s="13">
+        <f t="shared" si="16"/>
+        <v>133057.82999999999</v>
+      </c>
+      <c r="AY16" s="20">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AF16" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AG16" s="14">
-        <f>COUNTIFS(J15:J16,J16,K15:K16,K16,P15:P16,P16)+1</f>
-        <v>2</v>
-      </c>
-      <c r="AH16" s="18" t="str">
-        <f t="shared" si="1"/>
         <v>7.003044</v>
       </c>
-      <c r="AI16" s="18" t="str">
+      <c r="AZ16" s="13">
         <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="AJ16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00002</v>
-      </c>
-      <c r="AK16" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>00000151</v>
-      </c>
-      <c r="AL16" s="9">
+        <v>161000</v>
+      </c>
+      <c r="BA16" s="20">
         <f t="shared" si="19"/>
-        <v>44816</v>
-      </c>
-      <c r="AM16" s="13">
-        <f t="shared" si="4"/>
-        <v>27942.15</v>
-      </c>
-      <c r="AN16" s="13">
-        <f t="shared" si="5"/>
-        <v>160999.99</v>
-      </c>
-      <c r="AO16" s="10" t="str">
-        <f>IF(RIGHT(K16,1)="A",SUBSTITUTE(TEXT(W16,"0,00"),",","."),SUBSTITUTE(TEXT(AN16,"0,00"),",","."))</f>
-        <v>133057.84</v>
-      </c>
-      <c r="AP16" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.01</v>
-      </c>
-      <c r="AQ16" s="1">
-        <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
-      <c r="AR16" s="15" t="str">
-        <f>O16&amp;"-"&amp;AQ16</f>
-        <v>30684125792-16</v>
-      </c>
-      <c r="AS16" s="1">
-        <f>COUNTIFS(J15:J16,J16,K15:K16,K16,P15:P16,P16)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT16" s="1">
-        <f ca="1">IF(F17="",0,COUNTIFS(J16:J17,J17,K16:K17,K17,P16:P17,P17)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU16" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>A</v>
-      </c>
-      <c r="AV16" s="1">
-        <f>IF(LEFT(K16,4)="Nota",0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AW16" s="13">
-        <f>IF(RIGHT(K16,1)="A",ROUND(V16*U16*(1+X16),2),AN16)</f>
-        <v>160999.98000000001</v>
-      </c>
-      <c r="AX16" s="13">
-        <f t="shared" si="8"/>
-        <v>133057.82999999999</v>
-      </c>
-      <c r="AY16" s="20">
-        <f t="shared" si="9"/>
-        <v>7.003044</v>
-      </c>
-      <c r="AZ16" s="13">
-        <f t="shared" si="10"/>
-        <v>161000</v>
-      </c>
-      <c r="BA16" s="20">
-        <f t="shared" si="11"/>
         <v>7.003044</v>
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
-        <f>CONCATENATE(J17," - ",O17," - ",P17," - ",S17)</f>
+        <f t="shared" si="0"/>
         <v>2 - 37473042 - BUSTOS PIASENTINI AGUSTIN - Ajuste</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -4459,19 +4530,19 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="8">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="20"/>
         <v>45149</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="21"/>
         <v>45108</v>
       </c>
       <c r="H17" s="9">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="22"/>
         <v>45138</v>
       </c>
       <c r="I17" s="9">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="23"/>
         <v>45163</v>
       </c>
       <c r="J17" s="2">
@@ -4510,7 +4581,7 @@
         <v>19000</v>
       </c>
       <c r="W17" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>28500</v>
       </c>
       <c r="X17" s="11" t="s">
@@ -4531,95 +4602,95 @@
       <c r="AC17" s="2"/>
       <c r="AD17" s="2"/>
       <c r="AE17" s="1" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+      <c r="AF17" s="1" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="AG17" s="14">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="AH17" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="AI17" s="18" t="str">
+        <f t="shared" si="26"/>
+        <v>19000.00</v>
+      </c>
+      <c r="AJ17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>00002</v>
+      </c>
+      <c r="AK17" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>00000153</v>
+      </c>
+      <c r="AL17" s="9">
+        <f t="shared" si="27"/>
+        <v>44816</v>
+      </c>
+      <c r="AM17" s="13">
+        <f t="shared" si="6"/>
+        <v>4946.28</v>
+      </c>
+      <c r="AN17" s="13">
+        <f t="shared" si="7"/>
+        <v>28500</v>
+      </c>
+      <c r="AO17" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>28500.00</v>
+      </c>
+      <c r="AP17" s="10" t="str">
+        <f t="shared" si="29"/>
+        <v>0.00</v>
+      </c>
+      <c r="AQ17" s="1">
+        <f t="shared" si="9"/>
+        <v>17</v>
+      </c>
+      <c r="AR17" s="15" t="str">
+        <f t="shared" si="10"/>
+        <v>37473042-17</v>
+      </c>
+      <c r="AS17" s="1">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT17" s="1">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AU17" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>B</v>
+      </c>
+      <c r="AV17" s="1">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AW17" s="13">
+        <f t="shared" si="15"/>
+        <v>28500</v>
+      </c>
+      <c r="AX17" s="13">
+        <f t="shared" si="16"/>
+        <v>23553.72</v>
+      </c>
+      <c r="AY17" s="20">
         <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="AF17" s="1" t="str">
-        <f t="shared" si="20"/>
-        <v/>
-      </c>
-      <c r="AG17" s="14">
-        <f>COUNTIFS(J16:J17,J17,K16:K17,K17,P16:P17,P17)+1</f>
-        <v>2</v>
-      </c>
-      <c r="AH17" s="18" t="str">
-        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="AI17" s="18" t="str">
+      <c r="AZ17" s="13">
         <f t="shared" si="18"/>
-        <v>19000.00</v>
-      </c>
-      <c r="AJ17" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>00002</v>
-      </c>
-      <c r="AK17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>00000153</v>
-      </c>
-      <c r="AL17" s="9">
+        <v>28500</v>
+      </c>
+      <c r="BA17" s="20">
         <f t="shared" si="19"/>
-        <v>44816</v>
-      </c>
-      <c r="AM17" s="13">
-        <f t="shared" si="4"/>
-        <v>4946.28</v>
-      </c>
-      <c r="AN17" s="13">
-        <f t="shared" si="5"/>
-        <v>28500</v>
-      </c>
-      <c r="AO17" s="10" t="str">
-        <f>IF(RIGHT(K17,1)="A",SUBSTITUTE(TEXT(W17,"0,00"),",","."),SUBSTITUTE(TEXT(AN17,"0,00"),",","."))</f>
-        <v>28500.00</v>
-      </c>
-      <c r="AP17" s="10" t="str">
-        <f t="shared" si="21"/>
-        <v>0.00</v>
-      </c>
-      <c r="AQ17" s="1">
-        <f t="shared" si="6"/>
-        <v>17</v>
-      </c>
-      <c r="AR17" s="15" t="str">
-        <f>O17&amp;"-"&amp;AQ17</f>
-        <v>37473042-17</v>
-      </c>
-      <c r="AS17" s="1">
-        <f>COUNTIFS(J16:J17,J17,K16:K17,K17,P16:P17,P17)-1</f>
-        <v>0</v>
-      </c>
-      <c r="AT17" s="1">
-        <f>IF(F18="",0,COUNTIFS(J17:J18,J18,K17:K18,K18,P17:P18,P18)-1)</f>
-        <v>0</v>
-      </c>
-      <c r="AU17" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>B</v>
-      </c>
-      <c r="AV17" s="1">
-        <f>IF(LEFT(K17,4)="Nota",0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AW17" s="13">
-        <f>IF(RIGHT(K17,1)="A",ROUND(V17*U17*(1+X17),2),AN17)</f>
-        <v>28500</v>
-      </c>
-      <c r="AX17" s="13">
-        <f t="shared" si="8"/>
-        <v>23553.72</v>
-      </c>
-      <c r="AY17" s="20">
-        <f t="shared" si="9"/>
-        <v>1.5</v>
-      </c>
-      <c r="AZ17" s="13">
-        <f t="shared" si="10"/>
-        <v>28500</v>
-      </c>
-      <c r="BA17" s="20">
-        <f t="shared" si="11"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4665,37 +4736,37 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>